<commit_message>
Cleaned up the XLSX file
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/pdf-registry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2CCE74-86D0-1844-ABB6-9280192BE0A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C407379F-05EA-E84F-AE03-870411D7AC72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17420" yWindow="460" windowWidth="20920" windowHeight="23880" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
+    <workbookView xWindow="13340" yWindow="460" windowWidth="25000" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -640,18 +640,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -664,22 +656,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -712,32 +690,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1053,14 +1015,14 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -1068,877 +1030,868 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="3" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2">
         <v>39932.427083333336</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="40" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3">
         <v>40060.538888888892</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4">
         <v>40079.444444444445</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5">
         <v>40081.550694444442</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6">
         <v>40094.793055555558</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7">
         <v>40105.464583333334</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8">
         <v>40164.4375</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9">
         <v>40305.557638888888</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10">
         <v>40522.519444444442</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>40560.762499999997</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>40664.775694444441</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>40714.365972222222</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>40854.607638888891</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+    </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>41039</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>72</v>
       </c>
+      <c r="F17"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <v>40997</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <v>40966</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20">
         <v>41736</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s">
         <v>92</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21">
         <v>41758</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>97</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22">
         <v>41780</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>102</v>
       </c>
+      <c r="F23"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24">
         <v>41854</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>109</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>111</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>112</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25">
         <v>41857</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>113</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>114</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>115</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>116</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26">
         <v>41890</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>120</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>122</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27">
         <v>41900</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>124</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>125</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" t="s">
         <v>126</v>
       </c>
-      <c r="F28" s="2">
+      <c r="E28"/>
+      <c r="F28">
         <v>41924</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>127</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>129</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>130</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>131</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29">
         <v>41931</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>132</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>134</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>135</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>136</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30">
         <v>41680</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" t="s">
         <v>140</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>141</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31">
         <v>42420</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>145</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>146</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32">
         <v>42439</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>147</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>149</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" t="s">
         <v>150</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>151</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33">
         <v>42467</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>152</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>153</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>154</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>155</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34">
         <v>42472</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>157</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>158</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>159</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35">
         <v>42492</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>160</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>161</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>162</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" t="s">
         <v>163</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>164</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36">
         <v>42505</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>167</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" t="s">
         <v>168</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>169</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37">
         <v>42530</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>170</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>171</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>172</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>173</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>174</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38">
         <v>42739</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>175</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>171</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>172</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>173</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>174</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39">
         <v>42739</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>176</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>177</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>178</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>179</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>180</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40">
         <v>42739</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>181</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>72</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41">
         <v>42852</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>182</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>183</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>184</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>185</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42">
         <v>43054</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>186</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>187</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>188</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>189</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>190</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43">
         <v>43212</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>191</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>192</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>193</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" t="s">
         <v>194</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>195</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44">
         <v>43231</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{569D482A-E106-2E44-93C8-132A931971A0}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{411F1819-9ECB-C54D-91CE-43A06A94AFDF}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{211FE2BB-DC7A-6148-84B1-54FCAB32A30D}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{291A8455-60A5-4143-8993-E42BA867AD3A}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{376718B5-B20D-DD48-AFAE-4DB44A86D2F6}"/>
-    <hyperlink ref="D12" r:id="rId6" xr:uid="{A9674ECF-4061-BF48-B611-DB28FF4A680B}"/>
-    <hyperlink ref="D14" r:id="rId7" xr:uid="{4AF35AFA-FB1C-6E44-BDD6-0FE605613C30}"/>
-    <hyperlink ref="D17" r:id="rId8" xr:uid="{FDC27BB4-3CB2-654F-B856-0F1CDF87E07E}"/>
-    <hyperlink ref="D18" r:id="rId9" xr:uid="{ACA187DF-B9A4-5E4A-9377-50FAF95A079D}"/>
-    <hyperlink ref="D19" r:id="rId10" xr:uid="{CCAFD539-E756-094F-9A86-9BFF09AF45DF}"/>
-    <hyperlink ref="D24" r:id="rId11" xr:uid="{18020BF1-BA7A-C648-B068-EA96312CDB55}"/>
-    <hyperlink ref="D28" r:id="rId12" xr:uid="{2AD9E267-1E0B-4A40-85FD-09AAD770BA43}"/>
-    <hyperlink ref="D31" r:id="rId13" xr:uid="{77958C2C-CA73-D749-A413-61805B158E11}"/>
-    <hyperlink ref="D33" r:id="rId14" xr:uid="{1FD40922-D561-024A-8F45-49C0AF1CC84E}"/>
-    <hyperlink ref="D36" r:id="rId15" xr:uid="{C62CC243-8B54-F943-979F-937A8BB307CD}"/>
-    <hyperlink ref="D37" r:id="rId16" xr:uid="{2BC3E656-05BC-8343-91DB-CE1075B02F04}"/>
-    <hyperlink ref="D41" r:id="rId17" xr:uid="{865BE0A6-62C0-7E42-9CE0-84DD4F6D9669}"/>
-    <hyperlink ref="D44" r:id="rId18" xr:uid="{58EF0196-CFA1-5D4B-B0C9-72ED8F3026CB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved Plib (for PDFLib) from private->public registry
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/pdf-registry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C407379F-05EA-E84F-AE03-870411D7AC72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F98C424-62F7-1445-A4F0-D72426E665F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13340" yWindow="460" windowWidth="25000" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
+    <workbookView xWindow="3140" yWindow="460" windowWidth="25000" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="207">
   <si>
     <t>ITXT</t>
   </si>
@@ -634,12 +634,30 @@
   </si>
   <si>
     <t>Create Date</t>
+  </si>
+  <si>
+    <t>Plib</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Merz</t>
+  </si>
+  <si>
+    <t>tm@pdflib.com</t>
+  </si>
+  <si>
+    <t>PDFlib GmbH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -657,7 +675,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -693,11 +711,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="H26" sqref="H26:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1030,865 +1050,874 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>39932.427083333336</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>40060.538888888892</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>40079.444444444445</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>40081.550694444442</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>40094.793055555558</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>40105.464583333334</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>40164.4375</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>40305.557638888888</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>40522.519444444442</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>40560.762499999997</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>40664.775694444441</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>40714.365972222222</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>40854.607638888891</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-    </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>41039</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F17"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>40997</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>40966</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>41736</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>41758</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>41780</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F23"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>41854</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>41857</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>41890</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>41900</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E28"/>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>41924</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>41931</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>41680</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>42420</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>42439</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>42467</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>42472</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>42492</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>42505</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>42530</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>42739</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>42739</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>42739</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>42852</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>43054</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2">
         <v>43212</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="2">
         <v>43231</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" s="3">
+        <v>37415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add WKTM prefix (#3)
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/pdf-registry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F98C424-62F7-1445-A4F0-D72426E665F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CCC1E5-68E4-2F41-9215-1368F63DC2AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3140" yWindow="460" windowWidth="25000" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="212">
   <si>
     <t>ITXT</t>
   </si>
@@ -649,6 +649,21 @@
   </si>
   <si>
     <t>PDFlib GmbH</t>
+  </si>
+  <si>
+    <t>WKTM</t>
+  </si>
+  <si>
+    <t>Colin</t>
+  </si>
+  <si>
+    <t>Borrowman</t>
+  </si>
+  <si>
+    <t>colin.borrowman@wolterskluwer.com</t>
+  </si>
+  <si>
+    <t>Walters Kluwer TeamMate</t>
   </si>
 </sst>
 </file>
@@ -656,7 +671,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -714,10 +729,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:H27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1920,6 +1935,26 @@
         <v>37415</v>
       </c>
     </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F46" s="3">
+        <v>43487</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Normex and PDF Association
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/pdf-registry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CCC1E5-68E4-2F41-9215-1368F63DC2AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3DC17C-3441-504E-8BFD-42F836760583}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="460" windowWidth="25000" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
+    <workbookView xWindow="12180" yWindow="460" windowWidth="25000" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="219">
   <si>
     <t>ITXT</t>
   </si>
@@ -664,6 +664,27 @@
   </si>
   <si>
     <t>Walters Kluwer TeamMate</t>
+  </si>
+  <si>
+    <t>NORM</t>
+  </si>
+  <si>
+    <t>Roman</t>
+  </si>
+  <si>
+    <t>Toda</t>
+  </si>
+  <si>
+    <t>toda@digitaldocuments.org</t>
+  </si>
+  <si>
+    <t>Normex s.r.o.</t>
+  </si>
+  <si>
+    <t>pdfa</t>
+  </si>
+  <si>
+    <t>PDF Association</t>
   </si>
 </sst>
 </file>
@@ -673,7 +694,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -692,6 +713,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -723,18 +752,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1047,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1955,7 +1987,51 @@
         <v>43487</v>
       </c>
     </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F47" s="2">
+        <v>43502</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F48" s="2">
+        <v>43502</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D47" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D48" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved the ISO_ prefix from the Adobe document to here while transferring ownership to ISO & 3DPDF Consortium
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/pdf-registry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A1F246-1CEB-8840-BDE1-AC8521229950}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13794D85-C5D9-9E44-A2E9-D136627A46EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="460" windowWidth="25000" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
+    <workbookView xWindow="13080" yWindow="460" windowWidth="25000" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="226">
   <si>
     <t>ITXT</t>
   </si>
@@ -697,6 +697,15 @@
   </si>
   <si>
     <t>klink@csi.com</t>
+  </si>
+  <si>
+    <t>ISO_</t>
+  </si>
+  <si>
+    <t>betsy.fanning@3dpdfconsortium.com</t>
+  </si>
+  <si>
+    <t>ISO (via the 3D PDF Consortium)</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1110,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2067,13 +2076,25 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E50"/>
+      <c r="A50" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E50" t="s">
+        <v>225</v>
+      </c>
+      <c r="F50" s="2">
+        <v>43614</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D47" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
     <hyperlink ref="D48" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
     <hyperlink ref="D49" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D50" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added `GTSm` for ISO 21812
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/pdf-registry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13794D85-C5D9-9E44-A2E9-D136627A46EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0058DD94-D2EA-9544-9A1F-FF6894DC13E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13080" yWindow="460" windowWidth="25000" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="231">
   <si>
     <t>ITXT</t>
   </si>
@@ -706,6 +706,21 @@
   </si>
   <si>
     <t>ISO (via the 3D PDF Consortium)</t>
+  </si>
+  <si>
+    <t>GTSm</t>
+  </si>
+  <si>
+    <t>Debbie</t>
+  </si>
+  <si>
+    <t>Orf</t>
+  </si>
+  <si>
+    <t>dorf@aptech.com</t>
+  </si>
+  <si>
+    <t>ISO TC130/WG2 as described in ISO 21812</t>
   </si>
 </sst>
 </file>
@@ -1107,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2089,12 +2104,33 @@
         <v>43614</v>
       </c>
     </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F51" s="2">
+        <v>43616</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D47" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
     <hyperlink ref="D48" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
     <hyperlink ref="D49" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
     <hyperlink ref="D50" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D51" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with 7 outstanding issues
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10607"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/pdf-registry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/PDF_Name_Registries/pdf-names-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E025F551-2D84-054B-9200-26AF98BCE6FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142C5A72-0B40-A046-8B43-985FE631B9B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="480" windowWidth="30920" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
+    <workbookView xWindow="5980" yWindow="460" windowWidth="34840" windowHeight="23540" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="277">
   <si>
     <t>ITXT</t>
   </si>
@@ -772,6 +772,93 @@
   </si>
   <si>
     <t>BFO</t>
+  </si>
+  <si>
+    <t>GeoD</t>
+  </si>
+  <si>
+    <t>Strebe</t>
+  </si>
+  <si>
+    <t>dstrebe@mapthematics.com</t>
+  </si>
+  <si>
+    <t>Mapthematics LLC</t>
+  </si>
+  <si>
+    <t>ICTI</t>
+  </si>
+  <si>
+    <t>Yongman</t>
+  </si>
+  <si>
+    <t>Jeong</t>
+  </si>
+  <si>
+    <t>ymjeong@icerti.com</t>
+  </si>
+  <si>
+    <t>iCerti</t>
+  </si>
+  <si>
+    <t>S4Cx</t>
+  </si>
+  <si>
+    <t>Ján</t>
+  </si>
+  <si>
+    <t>Hudec</t>
+  </si>
+  <si>
+    <t>info@sense4code.com</t>
+  </si>
+  <si>
+    <t>Sense4code s.r.o.</t>
+  </si>
+  <si>
+    <t>DMSK</t>
+  </si>
+  <si>
+    <t>István</t>
+  </si>
+  <si>
+    <t>Horváth</t>
+  </si>
+  <si>
+    <t>horvath.istvan@dmsone.hu</t>
+  </si>
+  <si>
+    <t>DMS One Zrt.</t>
+  </si>
+  <si>
+    <t>ABCp</t>
+  </si>
+  <si>
+    <t>Jos</t>
+  </si>
+  <si>
+    <t>Vernon</t>
+  </si>
+  <si>
+    <t>infohelp@websupergoo.com</t>
+  </si>
+  <si>
+    <t>Zandent Ltd</t>
+  </si>
+  <si>
+    <t>BECI</t>
+  </si>
+  <si>
+    <t>Jörg</t>
+  </si>
+  <si>
+    <t>Sonnenberger</t>
+  </si>
+  <si>
+    <t>joerg@bec.de</t>
+  </si>
+  <si>
+    <t>BEC GmbH &amp; Co KG</t>
   </si>
 </sst>
 </file>
@@ -781,7 +868,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -825,6 +912,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -856,7 +957,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -866,6 +967,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1181,13 +1285,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
@@ -1198,7 +1302,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>196</v>
       </c>
@@ -1218,7 +1322,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1342,7 @@
         <v>39932.427083333336</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1258,7 +1362,7 @@
         <v>40060.538888888892</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1278,7 +1382,7 @@
         <v>40079.444444444445</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1298,7 +1402,7 @@
         <v>40081.550694444442</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1318,7 +1422,7 @@
         <v>40094.793055555558</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1338,7 +1442,7 @@
         <v>40105.464583333334</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1358,7 +1462,7 @@
         <v>40164.4375</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1378,7 +1482,7 @@
         <v>40305.557638888888</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -1398,7 +1502,7 @@
         <v>40522.519444444442</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -1418,7 +1522,7 @@
         <v>40560.762499999997</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -1438,7 +1542,7 @@
         <v>40664.775694444441</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -1458,7 +1562,7 @@
         <v>40714.365972222222</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -1478,7 +1582,7 @@
         <v>40854.607638888891</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
@@ -1498,7 +1602,7 @@
         <v>41039</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -1515,7 +1619,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
@@ -1535,7 +1639,7 @@
         <v>40997</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>78</v>
       </c>
@@ -1555,7 +1659,7 @@
         <v>40966</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>83</v>
       </c>
@@ -1575,7 +1679,7 @@
         <v>41736</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>88</v>
       </c>
@@ -1595,7 +1699,7 @@
         <v>41758</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>93</v>
       </c>
@@ -1615,7 +1719,7 @@
         <v>41780</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>98</v>
       </c>
@@ -1632,7 +1736,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>103</v>
       </c>
@@ -1652,7 +1756,7 @@
         <v>41854</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>108</v>
       </c>
@@ -1672,7 +1776,7 @@
         <v>41857</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>113</v>
       </c>
@@ -1692,7 +1796,7 @@
         <v>41890</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>118</v>
       </c>
@@ -1712,7 +1816,7 @@
         <v>41900</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>123</v>
       </c>
@@ -1729,7 +1833,7 @@
         <v>41924</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>127</v>
       </c>
@@ -1749,7 +1853,7 @@
         <v>41931</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>132</v>
       </c>
@@ -1769,7 +1873,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>137</v>
       </c>
@@ -1789,7 +1893,7 @@
         <v>42420</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>142</v>
       </c>
@@ -1809,7 +1913,7 @@
         <v>42439</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>147</v>
       </c>
@@ -1829,7 +1933,7 @@
         <v>42467</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>152</v>
       </c>
@@ -1849,7 +1953,7 @@
         <v>42472</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>156</v>
       </c>
@@ -1869,7 +1973,7 @@
         <v>42492</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>160</v>
       </c>
@@ -1889,7 +1993,7 @@
         <v>42505</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>165</v>
       </c>
@@ -1909,7 +2013,7 @@
         <v>42530</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>170</v>
       </c>
@@ -1929,7 +2033,7 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>175</v>
       </c>
@@ -1949,7 +2053,7 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>176</v>
       </c>
@@ -1969,7 +2073,7 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>181</v>
       </c>
@@ -1989,7 +2093,7 @@
         <v>42852</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>182</v>
       </c>
@@ -2009,7 +2113,7 @@
         <v>43054</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>186</v>
       </c>
@@ -2029,7 +2133,7 @@
         <v>43212</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>191</v>
       </c>
@@ -2049,7 +2153,7 @@
         <v>43231</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>202</v>
       </c>
@@ -2069,7 +2173,7 @@
         <v>37415</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>207</v>
       </c>
@@ -2089,7 +2193,7 @@
         <v>43487</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>212</v>
       </c>
@@ -2109,7 +2213,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>217</v>
       </c>
@@ -2129,7 +2233,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>219</v>
       </c>
@@ -2149,7 +2253,7 @@
         <v>43503</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>223</v>
       </c>
@@ -2163,7 +2267,7 @@
         <v>43614</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>226</v>
       </c>
@@ -2183,7 +2287,7 @@
         <v>43616</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>231</v>
       </c>
@@ -2203,7 +2307,7 @@
         <v>43973</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>236</v>
       </c>
@@ -2217,7 +2321,7 @@
         <v>43973</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>237</v>
       </c>
@@ -2231,7 +2335,7 @@
         <v>43973</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>242</v>
       </c>
@@ -2252,7 +2356,7 @@
       </c>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>243</v>
       </c>
@@ -2270,6 +2374,146 @@
       </c>
       <c r="F56" s="2">
         <v>43997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F57" s="2">
+        <v>44037</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F58" s="2">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="F59" s="2">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="F60" s="2">
+        <v>44174</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="F61" s="2">
+        <v>44221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="F62" s="2">
+        <v>44280</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F63" s="11">
+        <v>42467</v>
       </c>
     </row>
   </sheetData>
@@ -2283,6 +2527,7 @@
     <hyperlink ref="D53" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
     <hyperlink ref="D54" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
     <hyperlink ref="D56" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
+    <hyperlink ref="D63" r:id="rId10" xr:uid="{CB1F48A1-505B-A741-ADDD-3777682713D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added FICL for Enfocus BV (Issue #23)
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9964B993-4831-40E8-9950-3A4295CA6815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C04FB15-1D47-4A01-AE31-B9E61F35338E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="312">
   <si>
     <t>ITXT</t>
   </si>
@@ -952,6 +952,21 @@
   </si>
   <si>
     <t>Duff Johnson Consulting</t>
+  </si>
+  <si>
+    <t>FICL</t>
+  </si>
+  <si>
+    <t>Bert</t>
+  </si>
+  <si>
+    <t>Van Kerckhove</t>
+  </si>
+  <si>
+    <t>bertvk@enfocus.com</t>
+  </si>
+  <si>
+    <t>Enfocus BV</t>
   </si>
 </sst>
 </file>
@@ -1367,11 +1382,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
+      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -1411,882 +1426,885 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>201</v>
+        <v>266</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>202</v>
+        <v>267</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" s="9">
-        <v>37415</v>
+        <v>268</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F2" s="7">
+        <v>44221</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="F3" s="7">
-        <v>39932.427083333336</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="31.75" x14ac:dyDescent="0.45">
+        <v>41931</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>301</v>
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="F4" s="7">
-        <v>40060.538888888892</v>
+        <v>40664.775694444441</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>157</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="F5" s="7">
-        <v>40079.444444444445</v>
+        <v>42492</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>271</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>272</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>273</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>275</v>
       </c>
       <c r="F6" s="7">
-        <v>40081.550694444442</v>
+        <v>44280</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>242</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>243</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>244</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>23</v>
+        <v>246</v>
       </c>
       <c r="F7" s="7">
-        <v>40094.793055555558</v>
+        <v>43997</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="F8" s="7">
-        <v>40105.464583333334</v>
+        <v>40997</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="F9" s="7">
-        <v>40164.4375</v>
+        <v>41758</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>169</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>170</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>36</v>
+        <v>171</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>172</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>38</v>
+        <v>173</v>
       </c>
       <c r="F10" s="7">
-        <v>40305.557638888888</v>
+        <v>42739</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>171</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="F11" s="7">
-        <v>40522.519444444442</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>42739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="31.75" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>301</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F12" s="7">
-        <v>40560.762499999997</v>
+        <v>40060.538888888892</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="F13" s="7">
-        <v>40664.775694444441</v>
+        <v>40105.464583333334</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>54</v>
+        <v>276</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>277</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>56</v>
+        <v>278</v>
+      </c>
+      <c r="E14" t="s">
+        <v>279</v>
       </c>
       <c r="F14" s="7">
-        <v>40714.365972222222</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
-        <v>57</v>
+        <v>261</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>58</v>
+        <v>262</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>61</v>
+        <v>263</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>265</v>
       </c>
       <c r="F15" s="7">
-        <v>40854.607638888891</v>
+        <v>44174</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="F16" s="7">
+        <v>41924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B17" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17" t="s">
+        <v>300</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E17" t="s">
+        <v>297</v>
+      </c>
+      <c r="F17" s="7">
+        <v>44580</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="F18" s="7">
+        <v>43231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C19" t="s">
+        <v>309</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F19" s="7">
+        <v>44581</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" s="7">
+        <v>41680</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="7">
+        <v>40079.444444444445</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="F22" s="7">
+        <v>44037</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="7">
+        <v>40714.365972222222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F24" s="7">
+        <v>43212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F25" s="7">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F26" s="7">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="7">
+        <v>40305.557638888888</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E28" t="s">
+        <v>284</v>
+      </c>
+      <c r="F28" s="7">
+        <v>44580</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F29" s="7">
         <v>40966</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="7">
-        <v>40997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="7">
-        <v>41039</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F19" s="7">
-        <v>41680</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="4" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F30" s="7">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F31" s="7">
         <v>41736</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="7">
-        <v>41758</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="7">
-        <v>41780</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" s="7">
-        <v>41854</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" s="7">
-        <v>41857</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="7">
-        <v>41890</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F26" s="7">
-        <v>41900</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="F27" s="7">
-        <v>41924</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="7">
-        <v>41931</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F29" s="7">
-        <v>42420</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F30" s="7">
-        <v>42439</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="F31" s="7">
-        <v>42467</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
-        <v>151</v>
+        <v>222</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>73</v>
+        <v>304</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>153</v>
+        <v>305</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>154</v>
+        <v>224</v>
       </c>
       <c r="F32" s="7">
-        <v>42472</v>
+        <v>43614</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>124</v>
+        <v>2</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>157</v>
+        <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
       <c r="F33" s="7">
-        <v>42492</v>
+        <v>39932.427083333336</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
-        <v>159</v>
+        <v>19</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>162</v>
+        <v>22</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>163</v>
+        <v>23</v>
       </c>
       <c r="F34" s="7">
-        <v>42505</v>
+        <v>40094.793055555558</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
-        <v>164</v>
+        <v>97</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>166</v>
+        <v>99</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F35" s="7">
-        <v>42530</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
-        <v>169</v>
+        <v>57</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>172</v>
+        <v>60</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>173</v>
+        <v>61</v>
       </c>
       <c r="F36" s="7">
-        <v>42739</v>
+        <v>40854.607638888891</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>170</v>
+        <v>218</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>173</v>
+        <v>220</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="F37" s="7">
-        <v>42739</v>
+        <v>43503</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
-        <v>175</v>
+        <v>62</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>176</v>
+        <v>63</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>178</v>
+        <v>65</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>179</v>
+        <v>66</v>
       </c>
       <c r="F38" s="7">
-        <v>42739</v>
+        <v>41039</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="F39" s="7">
-        <v>42852</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="F40" s="7">
-        <v>42852</v>
+        <v>40560.762499999997</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
-        <v>181</v>
+        <v>211</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>30</v>
+        <v>212</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>183</v>
+        <v>213</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
       <c r="F41" s="7">
-        <v>43054</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>187</v>
+        <v>285</v>
+      </c>
+      <c r="B42" t="s">
+        <v>288</v>
+      </c>
+      <c r="C42" t="s">
+        <v>289</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>189</v>
+        <v>290</v>
+      </c>
+      <c r="E42" t="s">
+        <v>287</v>
       </c>
       <c r="F42" s="7">
-        <v>43212</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>192</v>
+        <v>286</v>
+      </c>
+      <c r="B43" t="s">
+        <v>288</v>
+      </c>
+      <c r="C43" t="s">
+        <v>289</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>194</v>
+        <v>290</v>
+      </c>
+      <c r="E43" t="s">
+        <v>287</v>
       </c>
       <c r="F43" s="7">
-        <v>43231</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
-        <v>206</v>
+        <v>92</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>207</v>
+        <v>93</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>208</v>
+        <v>94</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="F44" s="9">
-        <v>43487</v>
+        <v>95</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="7">
+        <v>41780</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
-        <v>211</v>
+        <v>164</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>212</v>
+        <v>165</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>214</v>
+        <v>166</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>215</v>
+        <v>168</v>
       </c>
       <c r="F45" s="7">
-        <v>43502</v>
+        <v>42530</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
@@ -2311,498 +2329,519 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>78</v>
+        <v>29</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>219</v>
+        <v>31</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="F47" s="7">
-        <v>43503</v>
+        <v>40164.4375</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
-        <v>222</v>
+        <v>102</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="7">
+        <v>41854</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F49" s="9">
+        <v>37415</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F50" s="7">
+        <v>43997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="F51" s="7">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F52" s="7">
+        <v>41857</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F53" s="7">
+        <v>42467</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F54" s="7">
+        <v>42420</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F55" s="7">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="7">
+        <v>40081.550694444442</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F57" s="7">
+        <v>42472</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F58" s="7">
+        <v>43054</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="F48" s="7">
-        <v>43614</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A49" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F49" s="7">
-        <v>43616</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A50" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="F50" s="7">
+      <c r="F59" s="7">
         <v>43973</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A51" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="F51" s="7">
-        <v>43973</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A52" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="F52" s="7">
-        <v>43973</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A53" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="F53" s="7">
-        <v>43997</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A54" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="F54" s="7">
-        <v>43997</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A55" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="B55" s="4" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E60" t="s">
+        <v>292</v>
+      </c>
+      <c r="F60" s="7">
+        <v>44580</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="F55" s="7">
-        <v>44037</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A56" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="F56" s="7">
-        <v>44151</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A57" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="F57" s="7">
-        <v>44166</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A58" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="F58" s="7">
-        <v>44174</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A59" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="F59" s="7">
-        <v>44221</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A60" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="F60" s="7">
-        <v>44280</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A61" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="B61" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61" t="s">
-        <v>277</v>
+      <c r="C61" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E61" t="s">
-        <v>279</v>
+        <v>178</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="F61" s="7">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+        <v>42739</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="B62" t="s">
-        <v>299</v>
-      </c>
-      <c r="C62" t="s">
-        <v>300</v>
+        <v>39</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E62" t="s">
-        <v>297</v>
+        <v>42</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="F62" s="7">
-        <v>44580</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+        <v>40522.519444444442</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
-        <v>280</v>
+        <v>112</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>281</v>
+        <v>113</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>282</v>
+        <v>114</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E63" t="s">
-        <v>284</v>
+        <v>115</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="F63" s="7">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+        <v>41890</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="B64" t="s">
-        <v>288</v>
-      </c>
-      <c r="C64" t="s">
-        <v>289</v>
+        <v>67</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E64" t="s">
-        <v>287</v>
+        <v>70</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F64" s="7">
-        <v>44580</v>
+        <v>42852</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="B65" t="s">
-        <v>288</v>
-      </c>
-      <c r="C65" t="s">
-        <v>289</v>
+        <v>180</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E65" t="s">
-        <v>287</v>
+        <v>70</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F65" s="7">
-        <v>44580</v>
+        <v>42852</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="4" t="s">
-        <v>291</v>
+        <v>206</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>294</v>
+        <v>207</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>295</v>
+        <v>208</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E66" t="s">
-        <v>292</v>
-      </c>
-      <c r="F66" s="7">
-        <v>44580</v>
+        <v>209</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F66" s="9">
+        <v>43487</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="4" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>101</v>
+        <v>163</v>
+      </c>
+      <c r="F67" s="7">
+        <v>42505</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F68" s="7">
+        <v>42439</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G67">
-      <sortCondition ref="F1"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G68">
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D45" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D41" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
     <hyperlink ref="D46" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
-    <hyperlink ref="D47" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
-    <hyperlink ref="D48" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
-    <hyperlink ref="D49" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
-    <hyperlink ref="D51" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
-    <hyperlink ref="D50" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
-    <hyperlink ref="D52" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
-    <hyperlink ref="D53" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
-    <hyperlink ref="D60" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
-    <hyperlink ref="D59" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
-    <hyperlink ref="D58" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
-    <hyperlink ref="D57" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
-    <hyperlink ref="D56" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
-    <hyperlink ref="D55" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
-    <hyperlink ref="D54" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
-    <hyperlink ref="D44" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
-    <hyperlink ref="D2" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
-    <hyperlink ref="D43" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
-    <hyperlink ref="D42" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
-    <hyperlink ref="D41" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
-    <hyperlink ref="D40" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
-    <hyperlink ref="D38" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
-    <hyperlink ref="D37" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
-    <hyperlink ref="D36" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
-    <hyperlink ref="D35" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
-    <hyperlink ref="D34" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
-    <hyperlink ref="D3" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
-    <hyperlink ref="D5" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
-    <hyperlink ref="D6" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
-    <hyperlink ref="D7" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
-    <hyperlink ref="D8" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
-    <hyperlink ref="D9" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
-    <hyperlink ref="D10" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
-    <hyperlink ref="D11" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
-    <hyperlink ref="D12" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
-    <hyperlink ref="D13" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
-    <hyperlink ref="D14" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
-    <hyperlink ref="D15" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
-    <hyperlink ref="D18" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
-    <hyperlink ref="D39" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
-    <hyperlink ref="D17" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
-    <hyperlink ref="D16" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
-    <hyperlink ref="D20" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
-    <hyperlink ref="D21" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
-    <hyperlink ref="D22" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
-    <hyperlink ref="D67" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
-    <hyperlink ref="D23" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
-    <hyperlink ref="D24" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
-    <hyperlink ref="D25" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
-    <hyperlink ref="D26" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
-    <hyperlink ref="D27" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
-    <hyperlink ref="D28" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
-    <hyperlink ref="D19" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
-    <hyperlink ref="D29" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D30" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
-    <hyperlink ref="D31" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
-    <hyperlink ref="D32" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
-    <hyperlink ref="D33" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
-    <hyperlink ref="D61" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
-    <hyperlink ref="D63" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
-    <hyperlink ref="D64" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
-    <hyperlink ref="D65" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
-    <hyperlink ref="D66" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
-    <hyperlink ref="D62" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D37" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D32" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D26" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
+    <hyperlink ref="D55" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
+    <hyperlink ref="D25" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
+    <hyperlink ref="D59" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
+    <hyperlink ref="D2" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
+    <hyperlink ref="D51" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
+    <hyperlink ref="D30" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
+    <hyperlink ref="D22" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
+    <hyperlink ref="D50" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
+    <hyperlink ref="D66" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
+    <hyperlink ref="D49" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
+    <hyperlink ref="D18" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
+    <hyperlink ref="D24" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
+    <hyperlink ref="D58" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
+    <hyperlink ref="D65" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
+    <hyperlink ref="D61" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
+    <hyperlink ref="D11" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
+    <hyperlink ref="D10" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
+    <hyperlink ref="D45" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
+    <hyperlink ref="D67" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
+    <hyperlink ref="D33" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
+    <hyperlink ref="D21" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
+    <hyperlink ref="D56" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
+    <hyperlink ref="D34" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
+    <hyperlink ref="D13" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
+    <hyperlink ref="D47" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
+    <hyperlink ref="D27" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
+    <hyperlink ref="D62" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
+    <hyperlink ref="D40" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
+    <hyperlink ref="D4" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
+    <hyperlink ref="D23" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
+    <hyperlink ref="D36" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
+    <hyperlink ref="D38" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
+    <hyperlink ref="D64" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
+    <hyperlink ref="D8" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
+    <hyperlink ref="D29" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
+    <hyperlink ref="D31" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
+    <hyperlink ref="D9" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
+    <hyperlink ref="D44" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
+    <hyperlink ref="D35" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
+    <hyperlink ref="D48" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
+    <hyperlink ref="D52" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
+    <hyperlink ref="D63" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
+    <hyperlink ref="D39" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
+    <hyperlink ref="D16" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
+    <hyperlink ref="D3" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
+    <hyperlink ref="D20" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
+    <hyperlink ref="D54" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
+    <hyperlink ref="D68" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D53" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
+    <hyperlink ref="D57" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
+    <hyperlink ref="D5" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
+    <hyperlink ref="D14" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
+    <hyperlink ref="D28" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
+    <hyperlink ref="D42" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
+    <hyperlink ref="D43" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
+    <hyperlink ref="D60" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
+    <hyperlink ref="D17" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D19" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId66"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId67"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue #26 and Issue #28 requests done
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C04FB15-1D47-4A01-AE31-B9E61F35338E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E286D9-548E-4E7C-AB6E-FDE5942A788C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="322">
   <si>
     <t>ITXT</t>
   </si>
@@ -967,6 +967,36 @@
   </si>
   <si>
     <t>Enfocus BV</t>
+  </si>
+  <si>
+    <t>CLWN</t>
+  </si>
+  <si>
+    <t>Stefano</t>
+  </si>
+  <si>
+    <t>Chizzolini</t>
+  </si>
+  <si>
+    <t>info@stefanochizzolini.it</t>
+  </si>
+  <si>
+    <t>pdfclown.org</t>
+  </si>
+  <si>
+    <t>GLAU</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Misell</t>
+  </si>
+  <si>
+    <t>q@as207960.net</t>
+  </si>
+  <si>
+    <t>AS207960 Cyfyngedig</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1082,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1067,6 +1097,7 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1382,11 +1413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -1645,1201 +1676,1245 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="7">
-        <v>40105.464583333334</v>
-      </c>
+      <c r="A13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C13" t="s">
+        <v>314</v>
+      </c>
+      <c r="D13" t="s">
+        <v>315</v>
+      </c>
+      <c r="E13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F13" s="12">
+        <v>44676</v>
+      </c>
+      <c r="G13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="B14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" t="s">
-        <v>277</v>
+        <v>24</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E14" t="s">
-        <v>279</v>
+        <v>27</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="F14" s="7">
-        <v>44580</v>
+        <v>40105.464583333334</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>265</v>
+        <v>276</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>277</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E15" t="s">
+        <v>279</v>
       </c>
       <c r="F15" s="7">
-        <v>44174</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>122</v>
+        <v>261</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>123</v>
+        <v>262</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>306</v>
+        <v>263</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>265</v>
       </c>
       <c r="F16" s="7">
-        <v>41924</v>
+        <v>44174</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="B17" t="s">
-        <v>299</v>
-      </c>
-      <c r="C17" t="s">
-        <v>300</v>
+        <v>122</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E17" t="s">
-        <v>297</v>
+        <v>125</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="F17" s="7">
-        <v>44580</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>303</v>
+        <v>41924</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>192</v>
+        <v>296</v>
+      </c>
+      <c r="B18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C18" t="s">
+        <v>300</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>194</v>
+        <v>298</v>
+      </c>
+      <c r="E18" t="s">
+        <v>297</v>
       </c>
       <c r="F18" s="7">
-        <v>43231</v>
+        <v>44580</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
-        <v>307</v>
+        <v>190</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="C19" t="s">
-        <v>309</v>
+        <v>191</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>310</v>
+        <v>193</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>311</v>
+        <v>194</v>
       </c>
       <c r="F19" s="7">
-        <v>44581</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>303</v>
+        <v>43231</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
-        <v>131</v>
+        <v>307</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>133</v>
+        <v>308</v>
+      </c>
+      <c r="C20" t="s">
+        <v>309</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>135</v>
+        <v>311</v>
       </c>
       <c r="F20" s="7">
-        <v>41680</v>
+        <v>44581</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="F21" s="7">
-        <v>40079.444444444445</v>
+        <v>41680</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>247</v>
+        <v>9</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>176</v>
+        <v>10</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>248</v>
+        <v>11</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>249</v>
+        <v>12</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>250</v>
+        <v>13</v>
       </c>
       <c r="F22" s="7">
-        <v>44037</v>
+        <v>40079.444444444445</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
-        <v>53</v>
+        <v>247</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>54</v>
+        <v>248</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>249</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>56</v>
+        <v>250</v>
       </c>
       <c r="F23" s="7">
-        <v>40714.365972222222</v>
+        <v>44037</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>185</v>
+        <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>186</v>
+        <v>54</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>188</v>
+        <v>55</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>189</v>
+        <v>56</v>
       </c>
       <c r="F24" s="7">
-        <v>43212</v>
+        <v>40714.365972222222</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>304</v>
+        <v>186</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>223</v>
+        <v>187</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="F25" s="7">
-        <v>43973</v>
+        <v>43212</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F26" s="7">
-        <v>43616</v>
-      </c>
+      <c r="A26" t="s">
+        <v>317</v>
+      </c>
+      <c r="B26" t="s">
+        <v>318</v>
+      </c>
+      <c r="C26" t="s">
+        <v>319</v>
+      </c>
+      <c r="D26" t="s">
+        <v>320</v>
+      </c>
+      <c r="E26" t="s">
+        <v>321</v>
+      </c>
+      <c r="F26" s="12">
+        <v>44676</v>
+      </c>
+      <c r="G26"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
-        <v>34</v>
+        <v>235</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>35</v>
+        <v>304</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>37</v>
+        <v>305</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>38</v>
+        <v>224</v>
       </c>
       <c r="F27" s="7">
-        <v>40305.557638888888</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
-        <v>280</v>
+        <v>225</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>281</v>
+        <v>226</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E28" t="s">
-        <v>284</v>
+        <v>227</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>229</v>
       </c>
       <c r="F28" s="7">
-        <v>44580</v>
+        <v>43616</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="F29" s="7">
-        <v>40966</v>
+        <v>40305.557638888888</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>252</v>
+        <v>281</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>255</v>
+        <v>283</v>
+      </c>
+      <c r="E30" t="s">
+        <v>284</v>
       </c>
       <c r="F30" s="7">
-        <v>44151</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F31" s="7">
-        <v>41736</v>
+        <v>40966</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
-        <v>222</v>
+        <v>251</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>304</v>
+        <v>252</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>224</v>
+        <v>253</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>255</v>
       </c>
       <c r="F32" s="7">
-        <v>43614</v>
+        <v>44151</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="F33" s="7">
-        <v>39932.427083333336</v>
+        <v>41736</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
-        <v>19</v>
+        <v>222</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>20</v>
+        <v>304</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>22</v>
+        <v>305</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>23</v>
+        <v>224</v>
       </c>
       <c r="F34" s="7">
-        <v>40094.793055555558</v>
+        <v>43614</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>101</v>
+        <v>4</v>
+      </c>
+      <c r="F35" s="7">
+        <v>39932.427083333336</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="F36" s="7">
-        <v>40854.607638888891</v>
+        <v>40094.793055555558</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>78</v>
+        <v>97</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="F37" s="7">
-        <v>43503</v>
+        <v>99</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F38" s="7">
-        <v>41039</v>
+        <v>40854.607638888891</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>118</v>
+        <v>218</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>121</v>
+        <v>220</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="F39" s="7">
-        <v>41900</v>
+        <v>43503</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="F40" s="7">
-        <v>40560.762499999997</v>
+        <v>41039</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
-        <v>211</v>
+        <v>117</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>212</v>
+        <v>118</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>214</v>
+        <v>119</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>215</v>
+        <v>121</v>
       </c>
       <c r="F41" s="7">
-        <v>43502</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="B42" t="s">
-        <v>288</v>
-      </c>
-      <c r="C42" t="s">
-        <v>289</v>
+        <v>44</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E42" t="s">
-        <v>287</v>
+        <v>47</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="F42" s="7">
-        <v>44580</v>
+        <v>40560.762499999997</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="B43" t="s">
-        <v>288</v>
-      </c>
-      <c r="C43" t="s">
-        <v>289</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E43" t="s">
-        <v>287</v>
+        <v>211</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="F43" s="7">
-        <v>44580</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>94</v>
+        <v>285</v>
+      </c>
+      <c r="B44" t="s">
+        <v>288</v>
+      </c>
+      <c r="C44" t="s">
+        <v>289</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>96</v>
+        <v>290</v>
+      </c>
+      <c r="E44" t="s">
+        <v>287</v>
       </c>
       <c r="F44" s="7">
-        <v>41780</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>166</v>
+        <v>286</v>
+      </c>
+      <c r="B45" t="s">
+        <v>288</v>
+      </c>
+      <c r="C45" t="s">
+        <v>289</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>168</v>
+        <v>290</v>
+      </c>
+      <c r="E45" t="s">
+        <v>287</v>
       </c>
       <c r="F45" s="7">
-        <v>42530</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
-        <v>216</v>
+        <v>92</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>125</v>
+        <v>94</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>217</v>
+        <v>96</v>
       </c>
       <c r="F46" s="7">
-        <v>43502</v>
+        <v>41780</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>33</v>
+        <v>168</v>
       </c>
       <c r="F47" s="7">
-        <v>40164.4375</v>
+        <v>42530</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
-        <v>102</v>
+        <v>216</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>105</v>
+        <v>124</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>106</v>
+        <v>217</v>
       </c>
       <c r="F48" s="7">
-        <v>41854</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
-        <v>201</v>
+        <v>29</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>202</v>
+        <v>30</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>203</v>
+        <v>31</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F49" s="9">
-        <v>37415</v>
+        <v>32</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="7">
+        <v>40164.4375</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>238</v>
+      <c r="A50" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>240</v>
+        <v>105</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="F50" s="7">
-        <v>43997</v>
+        <v>41854</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="4" t="s">
-        <v>256</v>
+        <v>201</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>257</v>
+        <v>202</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>258</v>
+        <v>203</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="F51" s="7">
-        <v>44166</v>
+        <v>204</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F51" s="9">
+        <v>37415</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>109</v>
+      <c r="A52" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>238</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>111</v>
+        <v>239</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>240</v>
       </c>
       <c r="F52" s="7">
-        <v>41857</v>
+        <v>43997</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="4" t="s">
-        <v>146</v>
+        <v>256</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>147</v>
+        <v>257</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>148</v>
+        <v>258</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>150</v>
+        <v>259</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>260</v>
       </c>
       <c r="F53" s="7">
-        <v>42467</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="4" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="F54" s="7">
-        <v>42420</v>
+        <v>41857</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
-        <v>230</v>
+        <v>146</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>231</v>
+        <v>147</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>233</v>
+        <v>148</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>234</v>
+        <v>150</v>
       </c>
       <c r="F55" s="7">
-        <v>43973</v>
+        <v>42467</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="4" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>18</v>
+        <v>140</v>
       </c>
       <c r="F56" s="7">
-        <v>40081.550694444442</v>
+        <v>42420</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
-        <v>151</v>
+        <v>230</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>73</v>
+        <v>231</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>153</v>
+        <v>232</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>154</v>
+        <v>234</v>
       </c>
       <c r="F57" s="7">
-        <v>42472</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="4" t="s">
-        <v>181</v>
+        <v>14</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>182</v>
+        <v>16</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>183</v>
+        <v>17</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>184</v>
+        <v>18</v>
       </c>
       <c r="F58" s="7">
-        <v>43054</v>
+        <v>40081.550694444442</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="4" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>304</v>
+        <v>73</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>223</v>
+        <v>152</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>224</v>
+        <v>154</v>
       </c>
       <c r="F59" s="7">
-        <v>43973</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="4" t="s">
-        <v>291</v>
+        <v>181</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>294</v>
+        <v>30</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>295</v>
+        <v>182</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E60" t="s">
-        <v>292</v>
+        <v>183</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="F60" s="7">
-        <v>44580</v>
+        <v>43054</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="4" t="s">
-        <v>175</v>
+        <v>236</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>176</v>
+        <v>304</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>178</v>
+        <v>305</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="F61" s="7">
-        <v>42739</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
-        <v>39</v>
+        <v>291</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>40</v>
+        <v>294</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>41</v>
+        <v>295</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>43</v>
+        <v>293</v>
+      </c>
+      <c r="E62" t="s">
+        <v>292</v>
       </c>
       <c r="F62" s="7">
-        <v>40522.519444444442</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>115</v>
+        <v>178</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>116</v>
+        <v>179</v>
       </c>
       <c r="F63" s="7">
-        <v>41890</v>
+        <v>42739</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F64" s="7">
+        <v>40522.519444444442</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A65" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F65" s="7">
+        <v>41890</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A66" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E66" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F66" s="7">
         <v>42852</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A65" s="4" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A67" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E67" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F67" s="7">
         <v>42852</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A66" s="4" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A68" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="E68" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="F66" s="9">
+      <c r="F68" s="9">
         <v>43487</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A67" s="4" t="s">
+    <row r="69" spans="1:7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E69" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F69" s="7">
         <v>42505</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A68" s="4" t="s">
+      <c r="G69" s="4"/>
+    </row>
+    <row r="70" spans="1:7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E70" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F70" s="7">
         <v>42439</v>
       </c>
+      <c r="G70" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G68">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G70">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D41" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
-    <hyperlink ref="D46" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
-    <hyperlink ref="D37" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
-    <hyperlink ref="D32" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
-    <hyperlink ref="D26" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
-    <hyperlink ref="D55" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
-    <hyperlink ref="D25" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
-    <hyperlink ref="D59" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
+    <hyperlink ref="D43" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D48" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
+    <hyperlink ref="D39" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D34" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D28" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
+    <hyperlink ref="D57" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
+    <hyperlink ref="D27" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
+    <hyperlink ref="D61" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
     <hyperlink ref="D7" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
     <hyperlink ref="D6" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
     <hyperlink ref="D2" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
-    <hyperlink ref="D15" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
-    <hyperlink ref="D51" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
-    <hyperlink ref="D30" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
-    <hyperlink ref="D22" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
-    <hyperlink ref="D50" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
-    <hyperlink ref="D66" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
-    <hyperlink ref="D49" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
-    <hyperlink ref="D18" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
-    <hyperlink ref="D24" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
-    <hyperlink ref="D58" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
-    <hyperlink ref="D65" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
-    <hyperlink ref="D61" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
+    <hyperlink ref="D16" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
+    <hyperlink ref="D53" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
+    <hyperlink ref="D32" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
+    <hyperlink ref="D23" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
+    <hyperlink ref="D52" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
+    <hyperlink ref="D68" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
+    <hyperlink ref="D51" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
+    <hyperlink ref="D19" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
+    <hyperlink ref="D25" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
+    <hyperlink ref="D60" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
+    <hyperlink ref="D67" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
+    <hyperlink ref="D63" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
     <hyperlink ref="D11" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
     <hyperlink ref="D10" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
-    <hyperlink ref="D45" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
-    <hyperlink ref="D67" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
-    <hyperlink ref="D33" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
-    <hyperlink ref="D21" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
-    <hyperlink ref="D56" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
-    <hyperlink ref="D34" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
-    <hyperlink ref="D13" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
-    <hyperlink ref="D47" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
-    <hyperlink ref="D27" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
-    <hyperlink ref="D62" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
-    <hyperlink ref="D40" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
+    <hyperlink ref="D47" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
+    <hyperlink ref="D69" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
+    <hyperlink ref="D35" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
+    <hyperlink ref="D22" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
+    <hyperlink ref="D58" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
+    <hyperlink ref="D36" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
+    <hyperlink ref="D14" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
+    <hyperlink ref="D49" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
+    <hyperlink ref="D29" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
+    <hyperlink ref="D64" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
+    <hyperlink ref="D42" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
     <hyperlink ref="D4" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
-    <hyperlink ref="D23" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
-    <hyperlink ref="D36" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
-    <hyperlink ref="D38" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
-    <hyperlink ref="D64" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
+    <hyperlink ref="D24" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
+    <hyperlink ref="D38" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
+    <hyperlink ref="D40" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
+    <hyperlink ref="D66" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
     <hyperlink ref="D8" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
-    <hyperlink ref="D29" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
-    <hyperlink ref="D31" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
+    <hyperlink ref="D31" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
+    <hyperlink ref="D33" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
     <hyperlink ref="D9" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
-    <hyperlink ref="D44" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
-    <hyperlink ref="D35" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
-    <hyperlink ref="D48" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
-    <hyperlink ref="D52" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
-    <hyperlink ref="D63" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
-    <hyperlink ref="D39" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
-    <hyperlink ref="D16" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
+    <hyperlink ref="D46" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
+    <hyperlink ref="D37" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
+    <hyperlink ref="D50" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
+    <hyperlink ref="D54" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
+    <hyperlink ref="D65" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
+    <hyperlink ref="D41" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
+    <hyperlink ref="D17" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
     <hyperlink ref="D3" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
-    <hyperlink ref="D20" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
-    <hyperlink ref="D54" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D68" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
-    <hyperlink ref="D53" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
-    <hyperlink ref="D57" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
+    <hyperlink ref="D21" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
+    <hyperlink ref="D56" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
+    <hyperlink ref="D70" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D55" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
+    <hyperlink ref="D59" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
     <hyperlink ref="D5" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
-    <hyperlink ref="D14" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
-    <hyperlink ref="D28" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
-    <hyperlink ref="D42" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
-    <hyperlink ref="D43" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
-    <hyperlink ref="D60" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
-    <hyperlink ref="D17" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
-    <hyperlink ref="D19" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
+    <hyperlink ref="D15" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
+    <hyperlink ref="D30" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
+    <hyperlink ref="D44" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
+    <hyperlink ref="D45" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
+    <hyperlink ref="D62" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
+    <hyperlink ref="D18" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D20" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId67"/>

</xml_diff>

<commit_message>
Resolve Yin4Yang Issue #29
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8FD321-9FCB-49DC-96EF-D01FCC8E54FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DB7AB6-1D32-44D8-B86A-8EE905BBD953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="333">
   <si>
     <t>ITXT</t>
   </si>
@@ -935,10 +935,6 @@
     <t>Plettinck</t>
   </si>
   <si>
-    <t xml:space="preserve">Secretariat@cip4.org
-Tim.Donahue@Kodak.com </t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -978,9 +974,6 @@
     <t>Chizzolini</t>
   </si>
   <si>
-    <t>info@stefanochizzolini.it</t>
-  </si>
-  <si>
     <t>pdfclown.org</t>
   </si>
   <si>
@@ -993,9 +986,6 @@
     <t>Misell</t>
   </si>
   <si>
-    <t>q@as207960.net</t>
-  </si>
-  <si>
     <t>AS207960 Cyfyngedig</t>
   </si>
   <si>
@@ -1021,6 +1011,25 @@
   </si>
   <si>
     <t>FOXIT SOFTWARE INC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@stefanochizzolini.it </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secretariat@cip4.org 
+Tim.Donahue@Kodak.com  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q@as207960.net </t>
+  </si>
+  <si>
+    <t>_Y4Y</t>
+  </si>
+  <si>
+    <t>frank.vyncke@yin4yang.com</t>
+  </si>
+  <si>
+    <t>Yin4Yang BV</t>
   </si>
 </sst>
 </file>
@@ -1437,11 +1446,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -1476,192 +1485,195 @@
         <v>200</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>266</v>
+        <v>330</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>267</v>
+        <v>320</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>270</v>
+        <v>321</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E2" t="s">
+        <v>332</v>
       </c>
       <c r="F2" s="7">
-        <v>44221</v>
+        <v>44775</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>126</v>
+        <v>266</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>127</v>
+        <v>267</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>130</v>
+        <v>268</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>270</v>
       </c>
       <c r="F3" s="7">
-        <v>41931</v>
+        <v>44221</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>127</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="F4" s="7">
-        <v>40664.775694444441</v>
+        <v>41931</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>155</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>157</v>
+        <v>51</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>158</v>
+        <v>52</v>
       </c>
       <c r="F5" s="7">
-        <v>42492</v>
+        <v>40664.775694444441</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>271</v>
+        <v>155</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>272</v>
+        <v>156</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>275</v>
+        <v>124</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="F6" s="7">
-        <v>44280</v>
+        <v>42492</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>242</v>
+        <v>271</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>244</v>
+        <v>273</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>246</v>
+        <v>274</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>275</v>
       </c>
       <c r="F7" s="7">
-        <v>43997</v>
+        <v>44280</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>72</v>
+        <v>242</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>73</v>
+        <v>243</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>75</v>
+        <v>244</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>76</v>
+        <v>246</v>
       </c>
       <c r="F8" s="7">
-        <v>40997</v>
+        <v>43997</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F9" s="7">
-        <v>41758</v>
+        <v>40997</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>169</v>
+        <v>87</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>170</v>
+        <v>88</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>171</v>
+        <v>89</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>172</v>
+        <v>90</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="F10" s="7">
-        <v>42739</v>
+        <v>41758</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>170</v>
@@ -1679,714 +1691,714 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="31.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="7">
+        <v>42739</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.75" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D13" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F13" s="7">
         <v>40060.538888888892</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B14" t="s">
         <v>312</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
         <v>313</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D14" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E14" t="s">
         <v>314</v>
       </c>
-      <c r="D13" t="s">
-        <v>315</v>
-      </c>
-      <c r="E13" t="s">
-        <v>316</v>
-      </c>
-      <c r="F13" s="12">
+      <c r="F14" s="12">
         <v>44676</v>
       </c>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="7">
-        <v>40105.464583333334</v>
-      </c>
+      <c r="G14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="B15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" t="s">
-        <v>277</v>
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E15" t="s">
-        <v>279</v>
+        <v>27</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="F15" s="7">
-        <v>44580</v>
+        <v>40105.464583333334</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>265</v>
+        <v>276</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E16" t="s">
+        <v>279</v>
       </c>
       <c r="F16" s="7">
-        <v>44174</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
-        <v>122</v>
+        <v>261</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>123</v>
+        <v>262</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>306</v>
+        <v>263</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>265</v>
       </c>
       <c r="F17" s="7">
-        <v>41924</v>
+        <v>44174</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="B18" t="s">
-        <v>299</v>
-      </c>
-      <c r="C18" t="s">
-        <v>300</v>
+        <v>122</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E18" t="s">
-        <v>297</v>
+        <v>125</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>305</v>
       </c>
       <c r="F18" s="7">
-        <v>44580</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>303</v>
+        <v>41924</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>192</v>
+        <v>296</v>
+      </c>
+      <c r="B19" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19" t="s">
+        <v>300</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>194</v>
+        <v>298</v>
+      </c>
+      <c r="E19" t="s">
+        <v>297</v>
       </c>
       <c r="F19" s="7">
-        <v>43231</v>
+        <v>44580</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
-        <v>307</v>
+        <v>190</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="C20" t="s">
-        <v>309</v>
+        <v>191</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>310</v>
+        <v>193</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>311</v>
+        <v>194</v>
       </c>
       <c r="F20" s="7">
-        <v>44581</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>303</v>
+        <v>43231</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>131</v>
+        <v>306</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>133</v>
+        <v>307</v>
+      </c>
+      <c r="C21" t="s">
+        <v>308</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>134</v>
+        <v>309</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>135</v>
+        <v>310</v>
       </c>
       <c r="F21" s="7">
-        <v>41680</v>
+        <v>44581</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="F22" s="7">
-        <v>40079.444444444445</v>
+        <v>41680</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
-        <v>327</v>
+        <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>212</v>
+        <v>10</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>213</v>
+        <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="E23" t="s">
-        <v>329</v>
+        <v>12</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="F23" s="7">
-        <v>44774</v>
+        <v>40079.444444444445</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>247</v>
+        <v>324</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>176</v>
+        <v>212</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>250</v>
+        <v>325</v>
+      </c>
+      <c r="E24" t="s">
+        <v>326</v>
       </c>
       <c r="F24" s="7">
-        <v>44037</v>
+        <v>44774</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
-        <v>53</v>
+        <v>247</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>54</v>
+        <v>248</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>55</v>
+        <v>249</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>56</v>
+        <v>250</v>
       </c>
       <c r="F25" s="7">
-        <v>40714.365972222222</v>
+        <v>44037</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="7">
+        <v>40714.365972222222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F27" s="7">
         <v>43212</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>315</v>
+      </c>
+      <c r="B28" t="s">
+        <v>316</v>
+      </c>
+      <c r="C28" t="s">
         <v>317</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D28" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E28" t="s">
         <v>318</v>
       </c>
-      <c r="C27" t="s">
-        <v>319</v>
-      </c>
-      <c r="D27" t="s">
-        <v>320</v>
-      </c>
-      <c r="E27" t="s">
-        <v>321</v>
-      </c>
-      <c r="F27" s="12">
+      <c r="F28" s="12">
         <v>44676</v>
       </c>
-      <c r="G27"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="F28" s="7">
-        <v>43973</v>
-      </c>
+      <c r="G28"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>226</v>
+        <v>303</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>227</v>
+        <v>304</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F29" s="7">
-        <v>43616</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
-        <v>34</v>
+        <v>225</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>35</v>
+        <v>226</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>37</v>
+        <v>227</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>38</v>
+        <v>229</v>
       </c>
       <c r="F30" s="7">
-        <v>40305.557638888888</v>
+        <v>43616</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
-        <v>280</v>
+        <v>34</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>281</v>
+        <v>35</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E31" t="s">
-        <v>284</v>
+        <v>37</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="F31" s="7">
-        <v>44580</v>
+        <v>40305.557638888888</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
-        <v>77</v>
+        <v>280</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>78</v>
+        <v>281</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>79</v>
+        <v>282</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>81</v>
+        <v>283</v>
+      </c>
+      <c r="E32" t="s">
+        <v>284</v>
       </c>
       <c r="F32" s="7">
-        <v>40966</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
-        <v>322</v>
+        <v>77</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="C33" t="s">
-        <v>324</v>
+        <v>78</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E33" t="s">
-        <v>326</v>
+        <v>80</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="F33" s="7">
-        <v>44700</v>
+        <v>40966</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
-        <v>251</v>
+        <v>319</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>253</v>
+        <v>320</v>
+      </c>
+      <c r="C34" t="s">
+        <v>321</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>255</v>
+        <v>322</v>
+      </c>
+      <c r="E34" t="s">
+        <v>323</v>
       </c>
       <c r="F34" s="7">
-        <v>44151</v>
+        <v>44700</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
-        <v>82</v>
+        <v>251</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>84</v>
+        <v>253</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>86</v>
+        <v>254</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>255</v>
       </c>
       <c r="F35" s="7">
-        <v>41736</v>
+        <v>44151</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
-        <v>222</v>
+        <v>82</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>304</v>
+        <v>83</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>223</v>
+        <v>84</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>224</v>
+        <v>86</v>
       </c>
       <c r="F36" s="7">
-        <v>43614</v>
+        <v>41736</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
-        <v>0</v>
+        <v>222</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>1</v>
+        <v>303</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>3</v>
+        <v>304</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="F37" s="7">
-        <v>39932.427083333336</v>
+        <v>43614</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F38" s="7">
-        <v>40094.793055555558</v>
+        <v>39932.427083333336</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>101</v>
+        <v>23</v>
+      </c>
+      <c r="F39" s="7">
+        <v>40094.793055555558</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F40" s="7">
-        <v>40854.607638888891</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>78</v>
+        <v>57</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>219</v>
+        <v>59</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="F41" s="7">
-        <v>43503</v>
+        <v>40854.607638888891</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>63</v>
+        <v>218</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>66</v>
+        <v>220</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="F42" s="7">
-        <v>41039</v>
+        <v>43503</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="F43" s="7">
-        <v>41900</v>
+        <v>41039</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="F44" s="7">
-        <v>40560.762499999997</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>212</v>
+        <v>45</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>214</v>
+        <v>46</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>215</v>
+        <v>48</v>
       </c>
       <c r="F45" s="7">
-        <v>43502</v>
+        <v>40560.762499999997</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="B46" t="s">
-        <v>288</v>
-      </c>
-      <c r="C46" t="s">
-        <v>289</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E46" t="s">
-        <v>287</v>
+        <v>211</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="F46" s="7">
-        <v>44580</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B47" t="s">
         <v>288</v>
@@ -2406,427 +2418,427 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>94</v>
+        <v>286</v>
+      </c>
+      <c r="B48" t="s">
+        <v>288</v>
+      </c>
+      <c r="C48" t="s">
+        <v>289</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>96</v>
+        <v>290</v>
+      </c>
+      <c r="E48" t="s">
+        <v>287</v>
       </c>
       <c r="F48" s="7">
-        <v>41780</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
-        <v>164</v>
+        <v>92</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>167</v>
+        <v>95</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>168</v>
+        <v>96</v>
       </c>
       <c r="F49" s="7">
-        <v>42530</v>
+        <v>41780</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
-        <v>216</v>
+        <v>164</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>125</v>
+        <v>166</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="F50" s="7">
-        <v>43502</v>
+        <v>42530</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="4" t="s">
-        <v>29</v>
+        <v>216</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>32</v>
+        <v>124</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>33</v>
+        <v>217</v>
       </c>
       <c r="F51" s="7">
-        <v>40164.4375</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="4" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="F52" s="7">
-        <v>41854</v>
+        <v>40164.4375</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="7">
+        <v>41854</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E54" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="F53" s="9">
+      <c r="F54" s="9">
         <v>37415</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A54" s="10" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B55" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C55" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E55" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F55" s="7">
         <v>43997</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A55" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="F55" s="7">
-        <v>44166</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="4" t="s">
-        <v>107</v>
+        <v>256</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>108</v>
+        <v>257</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>109</v>
+        <v>258</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>111</v>
+        <v>259</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>260</v>
       </c>
       <c r="F56" s="7">
-        <v>41857</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>147</v>
+        <v>108</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>149</v>
+        <v>110</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="F57" s="7">
-        <v>42467</v>
+        <v>41857</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="4" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="F58" s="7">
-        <v>42420</v>
+        <v>42467</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="4" t="s">
-        <v>230</v>
+        <v>136</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>231</v>
+        <v>137</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>233</v>
+        <v>138</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>234</v>
+        <v>140</v>
       </c>
       <c r="F59" s="7">
-        <v>43973</v>
+        <v>42420</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="4" t="s">
-        <v>14</v>
+        <v>230</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>15</v>
+        <v>231</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>17</v>
+        <v>232</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>18</v>
+        <v>234</v>
       </c>
       <c r="F60" s="7">
-        <v>40081.550694444442</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="4" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>152</v>
+        <v>16</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>153</v>
+        <v>17</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>154</v>
+        <v>18</v>
       </c>
       <c r="F61" s="7">
-        <v>42472</v>
+        <v>40081.550694444442</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="F62" s="7">
-        <v>43054</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
-        <v>236</v>
+        <v>181</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>304</v>
+        <v>30</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>223</v>
+        <v>182</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="F63" s="7">
-        <v>43973</v>
+        <v>43054</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
-        <v>291</v>
+        <v>236</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E64" t="s">
-        <v>292</v>
+        <v>304</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="F64" s="7">
-        <v>44580</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="4" t="s">
-        <v>175</v>
+        <v>291</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>176</v>
+        <v>294</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>177</v>
+        <v>295</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>179</v>
+        <v>293</v>
+      </c>
+      <c r="E65" t="s">
+        <v>292</v>
       </c>
       <c r="F65" s="7">
-        <v>42739</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="4" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>41</v>
+        <v>177</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>42</v>
+        <v>178</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="F66" s="7">
-        <v>40522.519444444442</v>
+        <v>42739</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="4" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="F67" s="7">
-        <v>41890</v>
+        <v>40522.519444444442</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="4" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="F68" s="7">
-        <v>42852</v>
+        <v>41890</v>
       </c>
     </row>
     <row r="69" spans="1:7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A69" s="4" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>68</v>
@@ -2847,142 +2859,165 @@
     </row>
     <row r="70" spans="1:7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A70" s="4" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>207</v>
+        <v>68</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>208</v>
+        <v>69</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="F70" s="9">
-        <v>43487</v>
+        <v>70</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" s="7">
+        <v>42852</v>
       </c>
       <c r="G70" s="4"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="4" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F71" s="7">
-        <v>42505</v>
+        <v>209</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F71" s="9">
+        <v>43487</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F72" s="7">
+        <v>42505</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A73" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E73" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F73" s="7">
         <v>42439</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G72">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G73">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D45" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
-    <hyperlink ref="D50" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
-    <hyperlink ref="D41" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
-    <hyperlink ref="D36" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
-    <hyperlink ref="D29" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
-    <hyperlink ref="D59" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
-    <hyperlink ref="D28" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
-    <hyperlink ref="D63" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
-    <hyperlink ref="D7" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
-    <hyperlink ref="D2" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
-    <hyperlink ref="D16" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
-    <hyperlink ref="D55" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
-    <hyperlink ref="D34" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
-    <hyperlink ref="D24" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
-    <hyperlink ref="D54" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
-    <hyperlink ref="D70" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
-    <hyperlink ref="D53" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
-    <hyperlink ref="D19" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
-    <hyperlink ref="D26" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
-    <hyperlink ref="D62" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
-    <hyperlink ref="D69" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
-    <hyperlink ref="D65" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
-    <hyperlink ref="D11" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
-    <hyperlink ref="D10" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
-    <hyperlink ref="D49" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
-    <hyperlink ref="D71" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
-    <hyperlink ref="D37" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
-    <hyperlink ref="D22" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
-    <hyperlink ref="D60" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
-    <hyperlink ref="D38" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
-    <hyperlink ref="D14" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
-    <hyperlink ref="D51" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
-    <hyperlink ref="D30" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
-    <hyperlink ref="D66" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
-    <hyperlink ref="D44" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
-    <hyperlink ref="D4" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
-    <hyperlink ref="D25" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
-    <hyperlink ref="D40" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
-    <hyperlink ref="D42" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
-    <hyperlink ref="D68" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
-    <hyperlink ref="D8" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
-    <hyperlink ref="D32" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
-    <hyperlink ref="D35" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
-    <hyperlink ref="D9" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
-    <hyperlink ref="D48" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
-    <hyperlink ref="D39" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
-    <hyperlink ref="D52" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
-    <hyperlink ref="D56" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
-    <hyperlink ref="D67" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
-    <hyperlink ref="D43" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
-    <hyperlink ref="D17" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
-    <hyperlink ref="D3" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
-    <hyperlink ref="D21" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
-    <hyperlink ref="D58" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D72" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
-    <hyperlink ref="D57" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
-    <hyperlink ref="D61" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
-    <hyperlink ref="D5" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
-    <hyperlink ref="D15" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
-    <hyperlink ref="D31" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
-    <hyperlink ref="D46" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
-    <hyperlink ref="D47" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
-    <hyperlink ref="D64" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
-    <hyperlink ref="D18" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
-    <hyperlink ref="D20" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
-    <hyperlink ref="D33" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
-    <hyperlink ref="D23" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
+    <hyperlink ref="D46" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D51" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
+    <hyperlink ref="D42" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D37" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D30" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
+    <hyperlink ref="D60" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
+    <hyperlink ref="D29" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
+    <hyperlink ref="D64" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
+    <hyperlink ref="D8" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
+    <hyperlink ref="D3" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
+    <hyperlink ref="D17" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
+    <hyperlink ref="D56" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
+    <hyperlink ref="D35" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
+    <hyperlink ref="D25" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
+    <hyperlink ref="D55" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
+    <hyperlink ref="D71" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
+    <hyperlink ref="D54" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
+    <hyperlink ref="D27" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
+    <hyperlink ref="D63" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
+    <hyperlink ref="D70" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
+    <hyperlink ref="D66" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
+    <hyperlink ref="D12" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
+    <hyperlink ref="D11" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
+    <hyperlink ref="D50" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
+    <hyperlink ref="D72" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
+    <hyperlink ref="D38" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
+    <hyperlink ref="D23" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
+    <hyperlink ref="D61" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
+    <hyperlink ref="D39" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
+    <hyperlink ref="D15" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
+    <hyperlink ref="D52" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
+    <hyperlink ref="D31" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
+    <hyperlink ref="D67" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
+    <hyperlink ref="D45" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
+    <hyperlink ref="D5" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
+    <hyperlink ref="D26" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
+    <hyperlink ref="D41" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
+    <hyperlink ref="D43" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
+    <hyperlink ref="D69" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
+    <hyperlink ref="D9" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
+    <hyperlink ref="D33" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
+    <hyperlink ref="D36" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
+    <hyperlink ref="D10" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
+    <hyperlink ref="D49" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
+    <hyperlink ref="D40" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
+    <hyperlink ref="D53" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
+    <hyperlink ref="D57" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
+    <hyperlink ref="D68" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
+    <hyperlink ref="D44" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
+    <hyperlink ref="D18" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
+    <hyperlink ref="D4" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
+    <hyperlink ref="D22" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
+    <hyperlink ref="D59" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
+    <hyperlink ref="D73" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D58" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
+    <hyperlink ref="D62" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
+    <hyperlink ref="D6" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
+    <hyperlink ref="D16" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
+    <hyperlink ref="D32" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
+    <hyperlink ref="D47" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
+    <hyperlink ref="D48" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
+    <hyperlink ref="D65" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
+    <hyperlink ref="D19" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D21" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
+    <hyperlink ref="D34" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
+    <hyperlink ref="D24" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
+    <hyperlink ref="D14" r:id="rId69" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
+    <hyperlink ref="D28" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
+    <hyperlink ref="D2" r:id="rId71" display="mailto:frank.vyncke@yin4yang.com" xr:uid="{E29600CB-349C-4C55-AC29-3B61912C4757}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId69"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId72"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Register XMPi Issue #32
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DB7AB6-1D32-44D8-B86A-8EE905BBD953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB2927A-268F-47BF-9D5E-CD910CF7AFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="338">
   <si>
     <t>ITXT</t>
   </si>
@@ -1030,6 +1030,21 @@
   </si>
   <si>
     <t>Yin4Yang BV</t>
+  </si>
+  <si>
+    <t>XMPi</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>Koganas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nathan@xmpie.com </t>
+  </si>
+  <si>
+    <t>XMPie Ltd.</t>
   </si>
 </sst>
 </file>
@@ -1446,11 +1461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -2920,30 +2935,46 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B73" t="s">
+        <v>334</v>
+      </c>
+      <c r="C73" t="s">
+        <v>335</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="F73" s="7">
+        <v>44775</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A74" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E74" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F74" s="7">
         <v>42439</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G73">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:G1" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}"/>
   <hyperlinks>
     <hyperlink ref="D46" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
     <hyperlink ref="D51" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
@@ -3000,7 +3031,7 @@
     <hyperlink ref="D4" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
     <hyperlink ref="D22" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
     <hyperlink ref="D59" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D73" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D74" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
     <hyperlink ref="D58" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
     <hyperlink ref="D62" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
     <hyperlink ref="D6" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
@@ -3016,8 +3047,9 @@
     <hyperlink ref="D14" r:id="rId69" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
     <hyperlink ref="D28" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
     <hyperlink ref="D2" r:id="rId71" display="mailto:frank.vyncke@yin4yang.com" xr:uid="{E29600CB-349C-4C55-AC29-3B61912C4757}"/>
+    <hyperlink ref="D73" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId72"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId73"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Register DLLB for #33
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB2927A-268F-47BF-9D5E-CD910CF7AFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8D734D-F99F-48FA-9D22-368B17E37307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PDF Prefix Registry" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PDF Prefix Registry'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="343">
   <si>
     <t>ITXT</t>
   </si>
@@ -1045,6 +1045,21 @@
   </si>
   <si>
     <t>XMPie Ltd.</t>
+  </si>
+  <si>
+    <t>DLLB</t>
+  </si>
+  <si>
+    <t>Boris</t>
+  </si>
+  <si>
+    <t>Doubrov</t>
+  </si>
+  <si>
+    <t>boris.doubrov@duallab.com</t>
+  </si>
+  <si>
+    <t>Dual Lab</t>
   </si>
 </sst>
 </file>
@@ -1130,22 +1145,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1461,56 +1473,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.78515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="4"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.78515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>330</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>321</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1519,230 +1530,230 @@
       <c r="E2" t="s">
         <v>332</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <v>44775</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>267</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>44221</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>128</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>41931</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>40664.775694444441</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>155</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>124</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>158</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>42492</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>271</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>272</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>273</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <v>44280</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>242</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>243</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>244</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>246</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <v>43997</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>40997</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s">
         <v>89</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <v>41758</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
         <v>171</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>42739</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>171</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>173</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <v>42739</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.75" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <v>40060.538888888892</v>
       </c>
     </row>
@@ -1762,33 +1773,32 @@
       <c r="E14" t="s">
         <v>314</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="7">
         <v>44676</v>
       </c>
-      <c r="G14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="4" t="s">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <v>40105.464583333334</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
+      <c r="A16" t="s">
         <v>276</v>
       </c>
       <c r="B16" t="s">
@@ -1803,637 +1813,636 @@
       <c r="E16" t="s">
         <v>279</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="5">
         <v>44580</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
+      <c r="A17" t="s">
+        <v>338</v>
+      </c>
+      <c r="B17" t="s">
+        <v>339</v>
+      </c>
+      <c r="C17" t="s">
+        <v>340</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E17" t="s">
+        <v>342</v>
+      </c>
+      <c r="F17" s="5">
+        <v>44915</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>261</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" t="s">
         <v>262</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" t="s">
         <v>263</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E18" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F18" s="5">
         <v>44174</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" t="s">
         <v>124</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E19" t="s">
         <v>305</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F19" s="5">
         <v>41924</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>296</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>299</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>300</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>297</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F20" s="5">
         <v>44580</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G20" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>190</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" t="s">
         <v>191</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" t="s">
         <v>192</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E21" t="s">
         <v>194</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F21" s="5">
         <v>43231</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>306</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" t="s">
         <v>307</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>308</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E22" t="s">
         <v>310</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F22" s="5">
         <v>44581</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G22" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>131</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" t="s">
         <v>132</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" t="s">
         <v>133</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E23" t="s">
         <v>135</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F23" s="5">
         <v>41680</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E24" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F24" s="5">
         <v>40079.444444444445</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" t="s">
         <v>212</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" t="s">
         <v>213</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>326</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F25" s="5">
         <v>44774</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>247</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" t="s">
         <v>176</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" t="s">
         <v>248</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E26" t="s">
         <v>250</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F26" s="5">
         <v>44037</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E27" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F27" s="5">
         <v>40714.365972222222</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F27" s="7">
-        <v>43212</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" t="s">
+        <v>187</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28" t="s">
+        <v>189</v>
+      </c>
+      <c r="F28" s="5">
+        <v>43212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>315</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>316</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>317</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>318</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F29" s="7">
         <v>44676</v>
       </c>
-      <c r="G28"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="4" t="s">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>235</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" t="s">
         <v>303</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" t="s">
         <v>304</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E30" t="s">
         <v>224</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F30" s="5">
         <v>43973</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="4" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>225</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" t="s">
         <v>226</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" t="s">
         <v>227</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E31" t="s">
         <v>229</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F31" s="5">
         <v>43616</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A31" s="4" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E32" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F32" s="5">
         <v>40305.557638888888</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>280</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" t="s">
         <v>281</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" t="s">
         <v>282</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>284</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F33" s="5">
         <v>44580</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C34" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E34" t="s">
         <v>81</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F34" s="5">
         <v>40966</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>319</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" t="s">
         <v>320</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>321</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>323</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F35" s="5">
         <v>44700</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="4" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>251</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" t="s">
         <v>252</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C36" t="s">
         <v>253</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E36" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F36" s="5">
         <v>44151</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="4" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E37" t="s">
         <v>86</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F37" s="5">
         <v>41736</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="4" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>222</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" t="s">
         <v>303</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" t="s">
         <v>304</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E38" t="s">
         <v>224</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F38" s="5">
         <v>43614</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E39" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F39" s="5">
         <v>39932.427083333336</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E40" t="s">
         <v>23</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F40" s="5">
         <v>40094.793055555558</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="4" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" t="s">
         <v>99</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="4" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E42" t="s">
         <v>61</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F42" s="5">
         <v>40854.607638888891</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>218</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" t="s">
         <v>220</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F43" s="5">
         <v>43503</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="4" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E44" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F44" s="5">
         <v>41039</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="4" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E45" t="s">
         <v>121</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F45" s="5">
         <v>41900</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C46" t="s">
         <v>46</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E46" t="s">
         <v>48</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F46" s="5">
         <v>40560.762499999997</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="4" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>211</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" t="s">
         <v>212</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C47" t="s">
         <v>213</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E47" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F47" s="5">
         <v>43502</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="4" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>285</v>
-      </c>
-      <c r="B47" t="s">
-        <v>288</v>
-      </c>
-      <c r="C47" t="s">
-        <v>289</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E47" t="s">
-        <v>287</v>
-      </c>
-      <c r="F47" s="7">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="4" t="s">
-        <v>286</v>
       </c>
       <c r="B48" t="s">
         <v>288</v>
@@ -2447,609 +2456,632 @@
       <c r="E48" t="s">
         <v>287</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="5">
         <v>44580</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="4" t="s">
+      <c r="A49" t="s">
+        <v>286</v>
+      </c>
+      <c r="B49" t="s">
+        <v>288</v>
+      </c>
+      <c r="C49" t="s">
+        <v>289</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E49" t="s">
+        <v>287</v>
+      </c>
+      <c r="F49" s="5">
+        <v>44580</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C50" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E50" t="s">
         <v>96</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F50" s="5">
         <v>41780</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="4" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>164</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" t="s">
         <v>165</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C51" t="s">
         <v>166</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E51" t="s">
         <v>168</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F51" s="5">
         <v>42530</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="4" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>216</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" t="s">
         <v>123</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" t="s">
         <v>124</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D52" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E52" t="s">
         <v>217</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F52" s="5">
         <v>43502</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="4" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C53" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E53" t="s">
         <v>33</v>
       </c>
-      <c r="F52" s="7">
+      <c r="F53" s="5">
         <v>40164.4375</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53" s="4" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" t="s">
         <v>103</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C54" t="s">
         <v>104</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E54" t="s">
         <v>106</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F54" s="5">
         <v>41854</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A54" s="4" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>201</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" t="s">
         <v>202</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C55" t="s">
         <v>203</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E55" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="F54" s="9">
+      <c r="F55" s="7">
         <v>37415</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A55" s="10" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B56" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C56" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E56" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F56" s="5">
         <v>43997</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A56" s="4" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>256</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" t="s">
         <v>257</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C57" t="s">
         <v>258</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="E57" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="F56" s="7">
+      <c r="F57" s="5">
         <v>44166</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="4" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C58" t="s">
         <v>109</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E58" t="s">
         <v>111</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F58" s="5">
         <v>41857</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A58" s="4" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>146</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" t="s">
         <v>147</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C59" t="s">
         <v>148</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E59" t="s">
         <v>150</v>
       </c>
-      <c r="F58" s="7">
+      <c r="F59" s="5">
         <v>42467</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59" s="4" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>136</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" t="s">
         <v>137</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C60" t="s">
         <v>138</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E60" t="s">
         <v>140</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F60" s="5">
         <v>42420</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A60" s="4" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>230</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" t="s">
         <v>231</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C61" t="s">
         <v>232</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D61" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E61" t="s">
         <v>234</v>
       </c>
-      <c r="F60" s="7">
+      <c r="F61" s="5">
         <v>43973</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A61" s="4" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C62" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E62" t="s">
         <v>18</v>
       </c>
-      <c r="F61" s="7">
+      <c r="F62" s="5">
         <v>40081.550694444442</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A62" s="4" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
         <v>151</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" t="s">
         <v>73</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" t="s">
         <v>152</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E63" t="s">
         <v>154</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F63" s="5">
         <v>42472</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A63" s="4" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
         <v>181</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C64" t="s">
         <v>182</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E64" t="s">
         <v>184</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F64" s="5">
         <v>43054</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A64" s="4" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
         <v>236</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" t="s">
         <v>303</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C65" t="s">
         <v>304</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E65" t="s">
         <v>224</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F65" s="5">
         <v>43973</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A65" s="4" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
         <v>291</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" t="s">
         <v>294</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C66" t="s">
         <v>295</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" t="s">
         <v>292</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F66" s="5">
         <v>44580</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A66" s="4" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
         <v>175</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" t="s">
         <v>176</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C67" t="s">
         <v>177</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E67" t="s">
         <v>179</v>
       </c>
-      <c r="F66" s="7">
+      <c r="F67" s="5">
         <v>42739</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A67" s="4" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>39</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" t="s">
         <v>40</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C68" t="s">
         <v>41</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E68" t="s">
         <v>43</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F68" s="5">
         <v>40522.519444444442</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A68" s="4" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>112</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" t="s">
         <v>113</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C69" t="s">
         <v>114</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E69" t="s">
         <v>116</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F69" s="5">
         <v>41890</v>
       </c>
     </row>
-    <row r="69" spans="1:7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="4" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
         <v>67</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F69" s="7">
-        <v>42852</v>
-      </c>
-      <c r="G69" s="4"/>
-    </row>
-    <row r="70" spans="1:7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" t="s">
         <v>69</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" t="s">
         <v>71</v>
       </c>
-      <c r="F70" s="7">
+      <c r="F70" s="5">
         <v>42852</v>
       </c>
-      <c r="G70" s="4"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A71" s="4" t="s">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>180</v>
+      </c>
+      <c r="B71" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E71" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" s="5">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
         <v>206</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" t="s">
         <v>207</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C72" t="s">
         <v>208</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="E72" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F71" s="9">
+      <c r="F72" s="7">
         <v>43487</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A72" s="4" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
         <v>159</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" t="s">
         <v>160</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C73" t="s">
         <v>161</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E73" t="s">
         <v>163</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F73" s="5">
         <v>42505</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A73" s="4" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
         <v>333</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>334</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>335</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E74" t="s">
         <v>337</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F74" s="5">
         <v>44775</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A74" s="4" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
         <v>141</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" t="s">
         <v>142</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C75" t="s">
         <v>143</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E75" t="s">
         <v>145</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F75" s="5">
         <v>42439</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}"/>
+  <autoFilter ref="A1:G1" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G75">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D46" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
-    <hyperlink ref="D51" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
-    <hyperlink ref="D42" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
-    <hyperlink ref="D37" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
-    <hyperlink ref="D30" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
-    <hyperlink ref="D60" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
-    <hyperlink ref="D29" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
-    <hyperlink ref="D64" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
+    <hyperlink ref="D47" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D52" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
+    <hyperlink ref="D43" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D38" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D31" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
+    <hyperlink ref="D61" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
+    <hyperlink ref="D30" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
+    <hyperlink ref="D65" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
     <hyperlink ref="D8" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
     <hyperlink ref="D7" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
     <hyperlink ref="D3" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
-    <hyperlink ref="D17" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
-    <hyperlink ref="D56" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
-    <hyperlink ref="D35" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
-    <hyperlink ref="D25" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
-    <hyperlink ref="D55" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
-    <hyperlink ref="D71" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
-    <hyperlink ref="D54" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
-    <hyperlink ref="D20" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
-    <hyperlink ref="D27" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
-    <hyperlink ref="D63" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
-    <hyperlink ref="D70" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
-    <hyperlink ref="D66" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
+    <hyperlink ref="D18" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
+    <hyperlink ref="D57" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
+    <hyperlink ref="D36" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
+    <hyperlink ref="D26" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
+    <hyperlink ref="D56" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
+    <hyperlink ref="D72" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
+    <hyperlink ref="D55" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
+    <hyperlink ref="D21" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
+    <hyperlink ref="D28" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
+    <hyperlink ref="D64" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
+    <hyperlink ref="D71" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
+    <hyperlink ref="D67" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
     <hyperlink ref="D12" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
     <hyperlink ref="D11" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
-    <hyperlink ref="D50" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
-    <hyperlink ref="D72" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
-    <hyperlink ref="D38" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
-    <hyperlink ref="D23" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
-    <hyperlink ref="D61" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
-    <hyperlink ref="D39" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
+    <hyperlink ref="D51" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
+    <hyperlink ref="D73" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
+    <hyperlink ref="D39" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
+    <hyperlink ref="D24" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
+    <hyperlink ref="D62" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
+    <hyperlink ref="D40" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
     <hyperlink ref="D15" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
-    <hyperlink ref="D52" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
-    <hyperlink ref="D31" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
-    <hyperlink ref="D67" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
-    <hyperlink ref="D45" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
+    <hyperlink ref="D53" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
+    <hyperlink ref="D32" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
+    <hyperlink ref="D68" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
+    <hyperlink ref="D46" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
     <hyperlink ref="D5" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
-    <hyperlink ref="D26" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
-    <hyperlink ref="D41" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
-    <hyperlink ref="D43" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
-    <hyperlink ref="D69" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
+    <hyperlink ref="D27" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
+    <hyperlink ref="D42" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
+    <hyperlink ref="D44" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
+    <hyperlink ref="D70" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
     <hyperlink ref="D9" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
-    <hyperlink ref="D33" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
-    <hyperlink ref="D36" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
+    <hyperlink ref="D34" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
+    <hyperlink ref="D37" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
     <hyperlink ref="D10" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
-    <hyperlink ref="D49" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
-    <hyperlink ref="D40" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
-    <hyperlink ref="D53" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
-    <hyperlink ref="D57" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
-    <hyperlink ref="D68" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
-    <hyperlink ref="D44" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
-    <hyperlink ref="D18" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
+    <hyperlink ref="D50" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
+    <hyperlink ref="D41" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
+    <hyperlink ref="D54" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
+    <hyperlink ref="D58" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
+    <hyperlink ref="D69" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
+    <hyperlink ref="D45" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
+    <hyperlink ref="D19" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
     <hyperlink ref="D4" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
-    <hyperlink ref="D22" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
-    <hyperlink ref="D59" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D74" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
-    <hyperlink ref="D58" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
-    <hyperlink ref="D62" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
+    <hyperlink ref="D23" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
+    <hyperlink ref="D60" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
+    <hyperlink ref="D75" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D59" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
+    <hyperlink ref="D63" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
     <hyperlink ref="D6" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
     <hyperlink ref="D16" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
-    <hyperlink ref="D32" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
-    <hyperlink ref="D47" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
-    <hyperlink ref="D48" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
-    <hyperlink ref="D65" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
-    <hyperlink ref="D19" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
-    <hyperlink ref="D21" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
-    <hyperlink ref="D34" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
-    <hyperlink ref="D24" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
+    <hyperlink ref="D33" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
+    <hyperlink ref="D48" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
+    <hyperlink ref="D49" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
+    <hyperlink ref="D66" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
+    <hyperlink ref="D20" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D22" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
+    <hyperlink ref="D35" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
+    <hyperlink ref="D25" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
     <hyperlink ref="D14" r:id="rId69" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
-    <hyperlink ref="D28" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
+    <hyperlink ref="D29" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
     <hyperlink ref="D2" r:id="rId71" display="mailto:frank.vyncke@yin4yang.com" xr:uid="{E29600CB-349C-4C55-AC29-3B61912C4757}"/>
-    <hyperlink ref="D73" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
+    <hyperlink ref="D74" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
+    <hyperlink ref="D17" r:id="rId73" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId73"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId74"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Assign "aftx" for Issue #34
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8D734D-F99F-48FA-9D22-368B17E37307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB7E1CB-3B62-4926-AA07-2A67281AE8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="349">
   <si>
     <t>ITXT</t>
   </si>
@@ -1060,6 +1060,24 @@
   </si>
   <si>
     <t>Dual Lab</t>
+  </si>
+  <si>
+    <t>aftx</t>
+  </si>
+  <si>
+    <t>Andras</t>
+  </si>
+  <si>
+    <t>Dippold</t>
+  </si>
+  <si>
+    <t>andras.dippold@affinitext.com</t>
+  </si>
+  <si>
+    <t>Affinitext Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/adobe/pdf-names-list/issues/34 </t>
   </si>
 </sst>
 </file>
@@ -1473,11 +1491,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F76" sqref="F76"/>
+      <selection pane="bottomLeft" activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -1579,147 +1597,150 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>343</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>344</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>345</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>51</v>
+        <v>346</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>347</v>
       </c>
       <c r="F5" s="5">
-        <v>40664.775694444441</v>
+        <v>44987</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>157</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>158</v>
+        <v>52</v>
       </c>
       <c r="F6" s="5">
-        <v>42492</v>
+        <v>40664.775694444441</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>124</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>275</v>
+        <v>157</v>
+      </c>
+      <c r="E7" t="s">
+        <v>158</v>
       </c>
       <c r="F7" s="5">
-        <v>44280</v>
+        <v>42492</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>242</v>
+        <v>271</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="C8" t="s">
-        <v>244</v>
+        <v>273</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E8" t="s">
-        <v>246</v>
+        <v>274</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>275</v>
       </c>
       <c r="F8" s="5">
-        <v>43997</v>
+        <v>44280</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>242</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>244</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>75</v>
+        <v>245</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>246</v>
       </c>
       <c r="F9" s="5">
-        <v>40997</v>
+        <v>43997</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F10" s="5">
-        <v>41758</v>
+        <v>40997</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>89</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>172</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="F11" s="5">
-        <v>42739</v>
+        <v>41758</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
         <v>170</v>
@@ -1737,732 +1758,732 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="31.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" s="5">
+        <v>42739</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.75" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F14" s="5">
         <v>40060.538888888892</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>311</v>
-      </c>
-      <c r="B14" t="s">
-        <v>312</v>
-      </c>
-      <c r="C14" t="s">
-        <v>313</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E14" t="s">
-        <v>314</v>
-      </c>
-      <c r="F14" s="7">
-        <v>44676</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>311</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>312</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>313</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>327</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="5">
-        <v>40105.464583333334</v>
+        <v>314</v>
+      </c>
+      <c r="F15" s="7">
+        <v>44676</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>276</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>277</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>278</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>279</v>
+        <v>28</v>
       </c>
       <c r="F16" s="5">
-        <v>44580</v>
+        <v>40105.464583333334</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>338</v>
+        <v>276</v>
       </c>
       <c r="B17" t="s">
-        <v>339</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>340</v>
+        <v>277</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>341</v>
+        <v>278</v>
       </c>
       <c r="E17" t="s">
-        <v>342</v>
+        <v>279</v>
       </c>
       <c r="F17" s="5">
-        <v>44915</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>261</v>
+        <v>338</v>
       </c>
       <c r="B18" t="s">
-        <v>262</v>
+        <v>339</v>
       </c>
       <c r="C18" t="s">
-        <v>263</v>
+        <v>340</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>265</v>
+        <v>341</v>
+      </c>
+      <c r="E18" t="s">
+        <v>342</v>
       </c>
       <c r="F18" s="5">
-        <v>44174</v>
+        <v>44915</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>261</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>262</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>263</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" t="s">
-        <v>305</v>
+        <v>264</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>265</v>
       </c>
       <c r="F19" s="5">
-        <v>41924</v>
+        <v>44174</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>296</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>299</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
-        <v>300</v>
+        <v>124</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>298</v>
+        <v>125</v>
       </c>
       <c r="E20" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="F20" s="5">
-        <v>44580</v>
-      </c>
-      <c r="G20" t="s">
-        <v>302</v>
+        <v>41924</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>190</v>
+        <v>296</v>
       </c>
       <c r="B21" t="s">
-        <v>191</v>
+        <v>299</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>300</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>193</v>
+        <v>298</v>
       </c>
       <c r="E21" t="s">
-        <v>194</v>
+        <v>297</v>
       </c>
       <c r="F21" s="5">
-        <v>43231</v>
+        <v>44580</v>
+      </c>
+      <c r="G21" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>306</v>
+        <v>190</v>
       </c>
       <c r="B22" t="s">
-        <v>307</v>
+        <v>191</v>
       </c>
       <c r="C22" t="s">
-        <v>308</v>
+        <v>192</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>309</v>
+        <v>193</v>
       </c>
       <c r="E22" t="s">
-        <v>310</v>
+        <v>194</v>
       </c>
       <c r="F22" s="5">
-        <v>44581</v>
-      </c>
-      <c r="G22" t="s">
-        <v>302</v>
+        <v>43231</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>306</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>307</v>
       </c>
       <c r="C23" t="s">
-        <v>133</v>
+        <v>308</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>134</v>
+        <v>309</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>310</v>
       </c>
       <c r="F23" s="5">
-        <v>41680</v>
+        <v>44581</v>
+      </c>
+      <c r="G23" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="F24" s="5">
-        <v>40079.444444444445</v>
+        <v>41680</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>324</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>213</v>
+        <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>325</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>326</v>
+        <v>13</v>
       </c>
       <c r="F25" s="5">
-        <v>44774</v>
+        <v>40079.444444444445</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>247</v>
+        <v>324</v>
       </c>
       <c r="B26" t="s">
-        <v>176</v>
+        <v>212</v>
       </c>
       <c r="C26" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>249</v>
+        <v>325</v>
       </c>
       <c r="E26" t="s">
-        <v>250</v>
+        <v>326</v>
       </c>
       <c r="F26" s="5">
-        <v>44037</v>
+        <v>44774</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>247</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>248</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>55</v>
+        <v>249</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>250</v>
       </c>
       <c r="F27" s="5">
-        <v>40714.365972222222</v>
+        <v>44037</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>185</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>186</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>188</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>189</v>
+        <v>56</v>
       </c>
       <c r="F28" s="5">
-        <v>43212</v>
+        <v>40714.365972222222</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>315</v>
+        <v>185</v>
       </c>
       <c r="B29" t="s">
-        <v>316</v>
+        <v>186</v>
       </c>
       <c r="C29" t="s">
-        <v>317</v>
+        <v>187</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>329</v>
+        <v>188</v>
       </c>
       <c r="E29" t="s">
-        <v>318</v>
-      </c>
-      <c r="F29" s="7">
-        <v>44676</v>
+        <v>189</v>
+      </c>
+      <c r="F29" s="5">
+        <v>43212</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>235</v>
+        <v>315</v>
       </c>
       <c r="B30" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="C30" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>223</v>
+        <v>329</v>
       </c>
       <c r="E30" t="s">
-        <v>224</v>
-      </c>
-      <c r="F30" s="5">
-        <v>43973</v>
+        <v>318</v>
+      </c>
+      <c r="F30" s="7">
+        <v>44676</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="B31" t="s">
-        <v>226</v>
+        <v>303</v>
       </c>
       <c r="C31" t="s">
-        <v>227</v>
+        <v>304</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E31" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F31" s="5">
-        <v>43616</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>225</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>226</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>227</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>37</v>
+        <v>228</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>229</v>
       </c>
       <c r="F32" s="5">
-        <v>40305.557638888888</v>
+        <v>43616</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>280</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>281</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>283</v>
+        <v>37</v>
       </c>
       <c r="E33" t="s">
-        <v>284</v>
+        <v>38</v>
       </c>
       <c r="F33" s="5">
-        <v>44580</v>
+        <v>40305.557638888888</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>280</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>281</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>282</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>80</v>
+        <v>283</v>
       </c>
       <c r="E34" t="s">
-        <v>81</v>
+        <v>284</v>
       </c>
       <c r="F34" s="5">
-        <v>40966</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>319</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>320</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>321</v>
+        <v>79</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>322</v>
+        <v>80</v>
       </c>
       <c r="E35" t="s">
-        <v>323</v>
+        <v>81</v>
       </c>
       <c r="F35" s="5">
-        <v>44700</v>
+        <v>40966</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>251</v>
+        <v>319</v>
       </c>
       <c r="B36" t="s">
-        <v>252</v>
+        <v>320</v>
       </c>
       <c r="C36" t="s">
-        <v>253</v>
+        <v>321</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>255</v>
+        <v>322</v>
+      </c>
+      <c r="E36" t="s">
+        <v>323</v>
       </c>
       <c r="F36" s="5">
-        <v>44151</v>
+        <v>44700</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>251</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>253</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" t="s">
-        <v>86</v>
+        <v>254</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>255</v>
       </c>
       <c r="F37" s="5">
-        <v>41736</v>
+        <v>44151</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>222</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>303</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>304</v>
+        <v>84</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>223</v>
+        <v>85</v>
       </c>
       <c r="E38" t="s">
-        <v>224</v>
+        <v>86</v>
       </c>
       <c r="F38" s="5">
-        <v>43614</v>
+        <v>41736</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>222</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>303</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>304</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>3</v>
+        <v>223</v>
       </c>
       <c r="E39" t="s">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="F39" s="5">
-        <v>39932.427083333336</v>
+        <v>43614</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F40" s="5">
-        <v>40094.793055555558</v>
+        <v>39932.427083333336</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
+        <v>23</v>
+      </c>
+      <c r="F41" s="5">
+        <v>40094.793055555558</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="C42" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E42" t="s">
-        <v>61</v>
-      </c>
-      <c r="F42" s="5">
-        <v>40854.607638888891</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>218</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>78</v>
+        <v>57</v>
+      </c>
+      <c r="B43" t="s">
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>220</v>
+        <v>59</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>219</v>
+        <v>60</v>
+      </c>
+      <c r="E43" t="s">
+        <v>61</v>
       </c>
       <c r="F43" s="5">
-        <v>43503</v>
+        <v>40854.607638888891</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" t="s">
-        <v>63</v>
+        <v>218</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>220</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E44" t="s">
-        <v>66</v>
+        <v>221</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="F44" s="5">
-        <v>41039</v>
+        <v>43503</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="E45" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="F45" s="5">
-        <v>41900</v>
+        <v>41039</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="E46" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="F46" s="5">
-        <v>40560.762499999997</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>212</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>213</v>
+        <v>46</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>214</v>
+        <v>47</v>
       </c>
       <c r="E47" t="s">
-        <v>215</v>
+        <v>48</v>
       </c>
       <c r="F47" s="5">
-        <v>43502</v>
+        <v>40560.762499999997</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>285</v>
+        <v>211</v>
       </c>
       <c r="B48" t="s">
-        <v>288</v>
+        <v>212</v>
       </c>
       <c r="C48" t="s">
-        <v>289</v>
+        <v>213</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>290</v>
+        <v>214</v>
       </c>
       <c r="E48" t="s">
-        <v>287</v>
+        <v>215</v>
       </c>
       <c r="F48" s="5">
-        <v>44580</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B49" t="s">
         <v>288</v>
@@ -2482,427 +2503,427 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>286</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>288</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>289</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>95</v>
+        <v>290</v>
       </c>
       <c r="E50" t="s">
-        <v>96</v>
+        <v>287</v>
       </c>
       <c r="F50" s="5">
-        <v>41780</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>164</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>167</v>
+        <v>95</v>
       </c>
       <c r="E51" t="s">
-        <v>168</v>
+        <v>96</v>
       </c>
       <c r="F51" s="5">
-        <v>42530</v>
+        <v>41780</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>216</v>
+        <v>164</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="C52" t="s">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>125</v>
+        <v>167</v>
       </c>
       <c r="E52" t="s">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="F52" s="5">
-        <v>43502</v>
+        <v>42530</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>216</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="C53" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="E53" t="s">
-        <v>33</v>
+        <v>217</v>
       </c>
       <c r="F53" s="5">
-        <v>40164.4375</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="E54" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="F54" s="5">
-        <v>41854</v>
+        <v>40164.4375</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" t="s">
+        <v>106</v>
+      </c>
+      <c r="F55" s="5">
+        <v>41854</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>201</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>202</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>203</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F56" s="7">
         <v>37415</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A56" s="8" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B57" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C57" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E57" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F57" s="5">
         <v>43997</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>256</v>
-      </c>
-      <c r="B57" t="s">
-        <v>257</v>
-      </c>
-      <c r="C57" t="s">
-        <v>258</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="F57" s="5">
-        <v>44166</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>256</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>257</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>258</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E58" t="s">
-        <v>111</v>
+        <v>259</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="F58" s="5">
-        <v>41857</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>108</v>
       </c>
       <c r="C59" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>149</v>
+        <v>110</v>
       </c>
       <c r="E59" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="F59" s="5">
-        <v>42467</v>
+        <v>41857</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E60" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="F60" s="5">
-        <v>42420</v>
+        <v>42467</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>230</v>
+        <v>136</v>
       </c>
       <c r="B61" t="s">
-        <v>231</v>
+        <v>137</v>
       </c>
       <c r="C61" t="s">
-        <v>232</v>
+        <v>138</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>233</v>
+        <v>139</v>
       </c>
       <c r="E61" t="s">
-        <v>234</v>
+        <v>140</v>
       </c>
       <c r="F61" s="5">
-        <v>43973</v>
+        <v>42420</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>230</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>231</v>
       </c>
       <c r="C62" t="s">
-        <v>16</v>
+        <v>232</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
       <c r="E62" t="s">
-        <v>18</v>
+        <v>234</v>
       </c>
       <c r="F62" s="5">
-        <v>40081.550694444442</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="C63" t="s">
-        <v>152</v>
+        <v>16</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>153</v>
+        <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>154</v>
+        <v>18</v>
       </c>
       <c r="F63" s="5">
-        <v>42472</v>
+        <v>40081.550694444442</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="C64" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="E64" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="F64" s="5">
-        <v>43054</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>236</v>
+        <v>181</v>
       </c>
       <c r="B65" t="s">
-        <v>303</v>
+        <v>30</v>
       </c>
       <c r="C65" t="s">
-        <v>304</v>
+        <v>182</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="E65" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="F65" s="5">
-        <v>43973</v>
+        <v>43054</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>291</v>
+        <v>236</v>
       </c>
       <c r="B66" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="C66" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>293</v>
+        <v>223</v>
       </c>
       <c r="E66" t="s">
-        <v>292</v>
+        <v>224</v>
       </c>
       <c r="F66" s="5">
-        <v>44580</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>175</v>
+        <v>291</v>
       </c>
       <c r="B67" t="s">
-        <v>176</v>
+        <v>294</v>
       </c>
       <c r="C67" t="s">
-        <v>177</v>
+        <v>295</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>178</v>
+        <v>293</v>
       </c>
       <c r="E67" t="s">
-        <v>179</v>
+        <v>292</v>
       </c>
       <c r="F67" s="5">
-        <v>42739</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="C68" t="s">
-        <v>41</v>
+        <v>177</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>42</v>
+        <v>178</v>
       </c>
       <c r="E68" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="F68" s="5">
-        <v>40522.519444444442</v>
+        <v>42739</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="C69" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="E69" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="F69" s="5">
-        <v>41890</v>
+        <v>40522.519444444442</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="C70" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E70" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="F70" s="5">
-        <v>42852</v>
+        <v>41890</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
         <v>68</v>
@@ -2922,166 +2943,188 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="B72" t="s">
-        <v>207</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
-        <v>208</v>
+        <v>69</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="F72" s="7">
-        <v>43487</v>
+        <v>70</v>
+      </c>
+      <c r="E72" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" s="5">
+        <v>42852</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="B73" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="C73" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E73" t="s">
-        <v>163</v>
-      </c>
-      <c r="F73" s="5">
-        <v>42505</v>
+        <v>209</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F73" s="7">
+        <v>43487</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>333</v>
+        <v>159</v>
       </c>
       <c r="B74" t="s">
-        <v>334</v>
+        <v>160</v>
       </c>
       <c r="C74" t="s">
-        <v>335</v>
+        <v>161</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>336</v>
+        <v>162</v>
       </c>
       <c r="E74" t="s">
-        <v>337</v>
+        <v>163</v>
       </c>
       <c r="F74" s="5">
-        <v>44775</v>
+        <v>42505</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
+        <v>333</v>
+      </c>
+      <c r="B75" t="s">
+        <v>334</v>
+      </c>
+      <c r="C75" t="s">
+        <v>335</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E75" t="s">
+        <v>337</v>
+      </c>
+      <c r="F75" s="5">
+        <v>44775</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
         <v>141</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>142</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E76" t="s">
         <v>145</v>
       </c>
-      <c r="F75" s="5">
+      <c r="F76" s="5">
         <v>42439</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G75">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G76">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D47" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
-    <hyperlink ref="D52" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
-    <hyperlink ref="D43" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
-    <hyperlink ref="D38" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
-    <hyperlink ref="D31" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
-    <hyperlink ref="D61" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
-    <hyperlink ref="D30" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
-    <hyperlink ref="D65" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
-    <hyperlink ref="D8" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
-    <hyperlink ref="D7" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
+    <hyperlink ref="D48" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D53" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
+    <hyperlink ref="D44" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D39" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D32" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
+    <hyperlink ref="D62" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
+    <hyperlink ref="D31" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
+    <hyperlink ref="D66" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
+    <hyperlink ref="D8" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
     <hyperlink ref="D3" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
-    <hyperlink ref="D18" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
-    <hyperlink ref="D57" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
-    <hyperlink ref="D36" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
-    <hyperlink ref="D26" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
-    <hyperlink ref="D56" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
-    <hyperlink ref="D72" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
-    <hyperlink ref="D55" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
-    <hyperlink ref="D21" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
-    <hyperlink ref="D28" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
-    <hyperlink ref="D64" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
-    <hyperlink ref="D71" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
-    <hyperlink ref="D67" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
-    <hyperlink ref="D12" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
-    <hyperlink ref="D11" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
-    <hyperlink ref="D51" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
-    <hyperlink ref="D73" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
-    <hyperlink ref="D39" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
-    <hyperlink ref="D24" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
-    <hyperlink ref="D62" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
-    <hyperlink ref="D40" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
-    <hyperlink ref="D15" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
-    <hyperlink ref="D53" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
-    <hyperlink ref="D32" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
-    <hyperlink ref="D68" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
-    <hyperlink ref="D46" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
-    <hyperlink ref="D5" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
-    <hyperlink ref="D27" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
-    <hyperlink ref="D42" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
-    <hyperlink ref="D44" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
-    <hyperlink ref="D70" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
-    <hyperlink ref="D9" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
-    <hyperlink ref="D34" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
-    <hyperlink ref="D37" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
-    <hyperlink ref="D10" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
-    <hyperlink ref="D50" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
-    <hyperlink ref="D41" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
-    <hyperlink ref="D54" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
-    <hyperlink ref="D58" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
-    <hyperlink ref="D69" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
-    <hyperlink ref="D45" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
-    <hyperlink ref="D19" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
+    <hyperlink ref="D19" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
+    <hyperlink ref="D58" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
+    <hyperlink ref="D37" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
+    <hyperlink ref="D27" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
+    <hyperlink ref="D57" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
+    <hyperlink ref="D73" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
+    <hyperlink ref="D56" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
+    <hyperlink ref="D22" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
+    <hyperlink ref="D29" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
+    <hyperlink ref="D65" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
+    <hyperlink ref="D72" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
+    <hyperlink ref="D68" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
+    <hyperlink ref="D13" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
+    <hyperlink ref="D12" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
+    <hyperlink ref="D52" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
+    <hyperlink ref="D74" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
+    <hyperlink ref="D40" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
+    <hyperlink ref="D25" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
+    <hyperlink ref="D63" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
+    <hyperlink ref="D41" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
+    <hyperlink ref="D16" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
+    <hyperlink ref="D54" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
+    <hyperlink ref="D33" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
+    <hyperlink ref="D69" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
+    <hyperlink ref="D47" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
+    <hyperlink ref="D6" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
+    <hyperlink ref="D28" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
+    <hyperlink ref="D43" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
+    <hyperlink ref="D45" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
+    <hyperlink ref="D71" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
+    <hyperlink ref="D10" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
+    <hyperlink ref="D35" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
+    <hyperlink ref="D38" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
+    <hyperlink ref="D11" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
+    <hyperlink ref="D51" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
+    <hyperlink ref="D42" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
+    <hyperlink ref="D55" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
+    <hyperlink ref="D59" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
+    <hyperlink ref="D70" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
+    <hyperlink ref="D46" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
+    <hyperlink ref="D20" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
     <hyperlink ref="D4" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
-    <hyperlink ref="D23" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
-    <hyperlink ref="D60" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D75" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
-    <hyperlink ref="D59" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
-    <hyperlink ref="D63" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
-    <hyperlink ref="D6" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
-    <hyperlink ref="D16" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
-    <hyperlink ref="D33" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
-    <hyperlink ref="D48" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
-    <hyperlink ref="D49" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
-    <hyperlink ref="D66" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
-    <hyperlink ref="D20" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
-    <hyperlink ref="D22" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
-    <hyperlink ref="D35" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
-    <hyperlink ref="D25" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
-    <hyperlink ref="D14" r:id="rId69" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
-    <hyperlink ref="D29" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
+    <hyperlink ref="D24" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
+    <hyperlink ref="D61" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
+    <hyperlink ref="D76" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D60" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
+    <hyperlink ref="D64" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
+    <hyperlink ref="D7" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
+    <hyperlink ref="D17" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
+    <hyperlink ref="D34" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
+    <hyperlink ref="D49" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
+    <hyperlink ref="D50" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
+    <hyperlink ref="D67" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
+    <hyperlink ref="D21" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D23" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
+    <hyperlink ref="D36" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
+    <hyperlink ref="D26" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
+    <hyperlink ref="D15" r:id="rId69" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
+    <hyperlink ref="D30" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
     <hyperlink ref="D2" r:id="rId71" display="mailto:frank.vyncke@yin4yang.com" xr:uid="{E29600CB-349C-4C55-AC29-3B61912C4757}"/>
-    <hyperlink ref="D74" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
-    <hyperlink ref="D17" r:id="rId73" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
+    <hyperlink ref="D75" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
+    <hyperlink ref="D18" r:id="rId73" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
+    <hyperlink ref="D5" r:id="rId74" xr:uid="{33D12C26-CC5E-4925-86B6-4AE855A6371F}"/>
+    <hyperlink ref="G5" r:id="rId75" xr:uid="{2FA39695-7884-42EC-9380-C8EFD7B7EAD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId74"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId76"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add prefixes for #35 and #36 and Mail for EA-PDF
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/PDF_Name_Registries/pdf-names-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072577C0-F4B3-8947-A10C-ECDDD901904E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC2F440-0C0C-4A6F-8289-B77C59FB6C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="500" windowWidth="25920" windowHeight="16620" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
+    <workbookView xWindow="1509" yWindow="1509" windowWidth="19285" windowHeight="12025" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
     <sheet name="PDF Prefix Registry" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="369">
   <si>
     <t>ITXT</t>
   </si>
@@ -1093,6 +1093,51 @@
   </si>
   <si>
     <t>Coalithon for Content Provenance and Authenticity (C2PA)</t>
+  </si>
+  <si>
+    <t>See also AgSi</t>
+  </si>
+  <si>
+    <t>AgSi</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Fröhlich</t>
+  </si>
+  <si>
+    <t>sebastian.froehlich@bearingpoint.com</t>
+  </si>
+  <si>
+    <t>Agree&amp;Sign GmbH (a BearingPoint Company)</t>
+  </si>
+  <si>
+    <t>https://github.com/adobe/pdf-names-list/issues/35</t>
+  </si>
+  <si>
+    <t>BePo</t>
+  </si>
+  <si>
+    <t>BearingPoint GmbH</t>
+  </si>
+  <si>
+    <t>https://github.com/adobe/pdf-names-list/issues/36</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Wyatt</t>
+  </si>
+  <si>
+    <t>peter.wyatt@pdfa.org</t>
+  </si>
+  <si>
+    <t>To support EA-PDF</t>
   </si>
 </sst>
 </file>
@@ -1506,25 +1551,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.35546875" customWidth="1"/>
+    <col min="2" max="2" width="16.640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="83.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>195</v>
       </c>
@@ -1547,7 +1592,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>330</v>
       </c>
@@ -1570,7 +1615,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -1590,7 +1635,7 @@
         <v>44221</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -1610,7 +1655,7 @@
         <v>41931</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>343</v>
       </c>
@@ -1633,1446 +1678,1518 @@
         <v>348</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C6" t="s">
+        <v>357</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E6" t="s">
+        <v>359</v>
+      </c>
+      <c r="F6" s="5">
+        <v>45147</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F7" s="5">
         <v>40664.775694444441</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>155</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>156</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>158</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F8" s="5">
         <v>42492</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>271</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>272</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>273</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F9" s="5">
         <v>44280</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>361</v>
+      </c>
+      <c r="B10" t="s">
+        <v>356</v>
+      </c>
+      <c r="C10" t="s">
+        <v>357</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="F10" s="5">
+        <v>45147</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>242</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>243</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>244</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E11" t="s">
         <v>246</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F11" s="5">
         <v>43997</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>73</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E12" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F12" s="5">
         <v>40997</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>349</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>350</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>351</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E13" t="s">
         <v>353</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F13" s="5">
         <v>45142</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>87</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>88</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F14" s="5">
         <v>41758</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>169</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>170</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>171</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" t="s">
         <v>173</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F15" s="5">
         <v>42739</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>174</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>170</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>171</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E16" t="s">
         <v>173</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F16" s="5">
         <v>42739</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="17" spans="1:7" ht="31.75" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F17" s="5">
         <v>40060.538888888892</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>311</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>312</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>313</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
         <v>314</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F18" s="7">
         <v>44676</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E19" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F19" s="5">
         <v>40105.464583333334</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>276</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>78</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>277</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>279</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F20" s="5">
         <v>44580</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="G20" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>338</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>339</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>340</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" t="s">
         <v>342</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F21" s="5">
         <v>44915</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>261</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>262</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>263</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F22" s="5">
         <v>44174</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>122</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>123</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>124</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>305</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F23" s="5">
         <v>41924</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>296</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>299</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>300</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>297</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F24" s="5">
         <v>44580</v>
-      </c>
-      <c r="G22" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B23" t="s">
-        <v>191</v>
-      </c>
-      <c r="C23" t="s">
-        <v>192</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E23" t="s">
-        <v>194</v>
-      </c>
-      <c r="F23" s="5">
-        <v>43231</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>306</v>
-      </c>
-      <c r="B24" t="s">
-        <v>307</v>
-      </c>
-      <c r="C24" t="s">
-        <v>308</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E24" t="s">
-        <v>310</v>
-      </c>
-      <c r="F24" s="5">
-        <v>44581</v>
       </c>
       <c r="G24" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25" t="s">
+        <v>191</v>
+      </c>
+      <c r="C25" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" t="s">
+        <v>194</v>
+      </c>
+      <c r="F25" s="5">
+        <v>43231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>306</v>
+      </c>
+      <c r="B26" t="s">
+        <v>307</v>
+      </c>
+      <c r="C26" t="s">
+        <v>308</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E26" t="s">
+        <v>310</v>
+      </c>
+      <c r="F26" s="5">
+        <v>44581</v>
+      </c>
+      <c r="G26" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>131</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>132</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>133</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>135</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F27" s="5">
         <v>41680</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>10</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E28" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F28" s="5">
         <v>40079.444444444445</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>324</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>212</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>213</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>326</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F29" s="5">
         <v>44774</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>247</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>176</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>248</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E30" t="s">
         <v>250</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F30" s="5">
         <v>44037</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>53</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>54</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C31" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E31" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F31" s="5">
         <v>40714.365972222222</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>185</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>186</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C32" t="s">
         <v>187</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E32" t="s">
         <v>189</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F32" s="5">
         <v>43212</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>315</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>316</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>317</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E33" t="s">
         <v>318</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F33" s="7">
         <v>44676</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>235</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>303</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>304</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E34" t="s">
         <v>224</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F34" s="5">
         <v>43973</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>225</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>226</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>227</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E35" t="s">
         <v>229</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F35" s="5">
         <v>43616</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>35</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E36" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F36" s="5">
         <v>40305.557638888888</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>280</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>281</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>282</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E37" t="s">
         <v>284</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F37" s="5">
         <v>44580</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>77</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>78</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E38" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F38" s="5">
         <v>40966</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>319</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>320</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>321</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E39" t="s">
         <v>323</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F39" s="5">
         <v>44700</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>251</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>252</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>253</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E40" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F40" s="5">
         <v>44151</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>82</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>83</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E41" t="s">
         <v>86</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F41" s="5">
         <v>41736</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>222</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>303</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>304</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E42" t="s">
         <v>224</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F42" s="5">
         <v>43614</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>0</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>1</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E43" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F43" s="5">
         <v>39932.427083333336</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>19</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>20</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E44" t="s">
         <v>23</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F44" s="5">
         <v>40094.793055555558</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>97</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B45" t="s">
         <v>98</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
         <v>99</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E45" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>57</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>58</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E46" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F46" s="5">
         <v>40854.607638888891</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>364</v>
+      </c>
+      <c r="B47" t="s">
+        <v>365</v>
+      </c>
+      <c r="C47" t="s">
+        <v>366</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E47" t="s">
+        <v>217</v>
+      </c>
+      <c r="F47" s="5">
+        <v>45147</v>
+      </c>
+      <c r="G47" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>218</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C48" t="s">
         <v>220</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F48" s="5">
         <v>43503</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>62</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B49" t="s">
         <v>63</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C49" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E49" t="s">
         <v>66</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F49" s="5">
         <v>41039</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>117</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B50" t="s">
         <v>118</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C50" t="s">
         <v>119</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E50" t="s">
         <v>121</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F50" s="5">
         <v>41900</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>44</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>45</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C51" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E51" t="s">
         <v>48</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F51" s="5">
         <v>40560.762499999997</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>211</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B52" t="s">
         <v>212</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C52" t="s">
         <v>213</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E52" t="s">
         <v>215</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F52" s="5">
         <v>43502</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>285</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B53" t="s">
         <v>288</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C53" t="s">
         <v>289</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E53" t="s">
         <v>287</v>
       </c>
-      <c r="F50" s="5">
+      <c r="F53" s="5">
         <v>44580</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>286</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B54" t="s">
         <v>288</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C54" t="s">
         <v>289</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E54" t="s">
         <v>287</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F54" s="5">
         <v>44580</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>92</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B55" t="s">
         <v>93</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C55" t="s">
         <v>94</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E55" t="s">
         <v>96</v>
       </c>
-      <c r="F52" s="5">
+      <c r="F55" s="5">
         <v>41780</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>164</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B56" t="s">
         <v>165</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C56" t="s">
         <v>166</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E56" t="s">
         <v>168</v>
       </c>
-      <c r="F53" s="5">
+      <c r="F56" s="5">
         <v>42530</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>216</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B57" t="s">
         <v>123</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C57" t="s">
         <v>124</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E57" t="s">
         <v>217</v>
       </c>
-      <c r="F54" s="5">
+      <c r="F57" s="5">
         <v>43502</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>29</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" t="s">
         <v>30</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C58" t="s">
         <v>31</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E58" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="5">
+      <c r="F58" s="5">
         <v>40164.4375</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>102</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" t="s">
         <v>103</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C59" t="s">
         <v>104</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E59" t="s">
         <v>106</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F59" s="5">
         <v>41854</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>201</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B60" t="s">
         <v>202</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C60" t="s">
         <v>203</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E60" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F60" s="7">
         <v>37415</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B61" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C61" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E61" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F58" s="5">
+      <c r="F61" s="5">
         <v>43997</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
         <v>256</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B62" t="s">
         <v>257</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C62" t="s">
         <v>258</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E62" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="F59" s="5">
+      <c r="F62" s="5">
         <v>44166</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
         <v>107</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B63" t="s">
         <v>108</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C63" t="s">
         <v>109</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E63" t="s">
         <v>111</v>
       </c>
-      <c r="F60" s="5">
+      <c r="F63" s="5">
         <v>41857</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
         <v>146</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B64" t="s">
         <v>147</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C64" t="s">
         <v>148</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E64" t="s">
         <v>150</v>
       </c>
-      <c r="F61" s="5">
+      <c r="F64" s="5">
         <v>42467</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
         <v>136</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B65" t="s">
         <v>137</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C65" t="s">
         <v>138</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E65" t="s">
         <v>140</v>
       </c>
-      <c r="F62" s="5">
+      <c r="F65" s="5">
         <v>42420</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
         <v>230</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B66" t="s">
         <v>231</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C66" t="s">
         <v>232</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E66" t="s">
         <v>234</v>
       </c>
-      <c r="F63" s="5">
+      <c r="F66" s="5">
         <v>43973</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
         <v>14</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B67" t="s">
         <v>15</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C67" t="s">
         <v>16</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E67" t="s">
         <v>18</v>
       </c>
-      <c r="F64" s="5">
+      <c r="F67" s="5">
         <v>40081.550694444442</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>151</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B68" t="s">
         <v>73</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C68" t="s">
         <v>152</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E68" t="s">
         <v>154</v>
       </c>
-      <c r="F65" s="5">
+      <c r="F68" s="5">
         <v>42472</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>181</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B69" t="s">
         <v>30</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C69" t="s">
         <v>182</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E69" t="s">
         <v>184</v>
       </c>
-      <c r="F66" s="5">
+      <c r="F69" s="5">
         <v>43054</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
         <v>236</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B70" t="s">
         <v>303</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C70" t="s">
         <v>304</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E70" t="s">
         <v>224</v>
       </c>
-      <c r="F67" s="5">
+      <c r="F70" s="5">
         <v>43973</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
         <v>291</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B71" t="s">
         <v>294</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C71" t="s">
         <v>295</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E71" t="s">
         <v>292</v>
       </c>
-      <c r="F68" s="5">
+      <c r="F71" s="5">
         <v>44580</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
         <v>175</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B72" t="s">
         <v>176</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C72" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E72" t="s">
         <v>179</v>
       </c>
-      <c r="F69" s="5">
+      <c r="F72" s="5">
         <v>42739</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
         <v>39</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B73" t="s">
         <v>40</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C73" t="s">
         <v>41</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E73" t="s">
         <v>43</v>
       </c>
-      <c r="F70" s="5">
+      <c r="F73" s="5">
         <v>40522.519444444442</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
         <v>112</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B74" t="s">
         <v>113</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C74" t="s">
         <v>114</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E74" t="s">
         <v>116</v>
       </c>
-      <c r="F71" s="5">
+      <c r="F74" s="5">
         <v>41890</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
         <v>67</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B75" t="s">
         <v>68</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C75" t="s">
         <v>69</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E75" t="s">
         <v>71</v>
       </c>
-      <c r="F72" s="5">
+      <c r="F75" s="5">
         <v>42852</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
         <v>180</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" t="s">
         <v>68</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C76" t="s">
         <v>69</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E76" t="s">
         <v>71</v>
       </c>
-      <c r="F73" s="5">
+      <c r="F76" s="5">
         <v>42852</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
         <v>206</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B77" t="s">
         <v>207</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C77" t="s">
         <v>208</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E77" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F77" s="7">
         <v>43487</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
         <v>159</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B78" t="s">
         <v>160</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C78" t="s">
         <v>161</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E78" t="s">
         <v>163</v>
       </c>
-      <c r="F75" s="5">
+      <c r="F78" s="5">
         <v>42505</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
         <v>333</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B79" t="s">
         <v>334</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C79" t="s">
         <v>335</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E79" t="s">
         <v>337</v>
       </c>
-      <c r="F76" s="5">
+      <c r="F79" s="5">
         <v>44775</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
         <v>141</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B80" t="s">
         <v>142</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C80" t="s">
         <v>143</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E80" t="s">
         <v>145</v>
       </c>
-      <c r="F77" s="5">
+      <c r="F80" s="5">
         <v>42439</v>
       </c>
     </row>
@@ -3083,84 +3200,89 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D49" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
-    <hyperlink ref="D54" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
-    <hyperlink ref="D45" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
-    <hyperlink ref="D40" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
-    <hyperlink ref="D33" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
-    <hyperlink ref="D63" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
-    <hyperlink ref="D32" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
-    <hyperlink ref="D67" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
-    <hyperlink ref="D9" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
-    <hyperlink ref="D8" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
+    <hyperlink ref="D52" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D57" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
+    <hyperlink ref="D48" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D42" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D35" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
+    <hyperlink ref="D66" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
+    <hyperlink ref="D34" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
+    <hyperlink ref="D70" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
+    <hyperlink ref="D9" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
     <hyperlink ref="D3" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
-    <hyperlink ref="D20" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
-    <hyperlink ref="D59" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
-    <hyperlink ref="D38" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
-    <hyperlink ref="D28" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
-    <hyperlink ref="D58" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
-    <hyperlink ref="D74" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
-    <hyperlink ref="D57" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
-    <hyperlink ref="D23" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
-    <hyperlink ref="D30" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
-    <hyperlink ref="D66" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
-    <hyperlink ref="D73" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
-    <hyperlink ref="D69" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
-    <hyperlink ref="D14" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
-    <hyperlink ref="D13" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
-    <hyperlink ref="D53" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
-    <hyperlink ref="D75" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
-    <hyperlink ref="D41" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
-    <hyperlink ref="D26" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
-    <hyperlink ref="D64" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
-    <hyperlink ref="D42" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
-    <hyperlink ref="D17" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
-    <hyperlink ref="D55" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
-    <hyperlink ref="D34" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
-    <hyperlink ref="D70" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
-    <hyperlink ref="D48" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
-    <hyperlink ref="D6" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
-    <hyperlink ref="D29" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
-    <hyperlink ref="D44" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
-    <hyperlink ref="D46" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
-    <hyperlink ref="D72" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
-    <hyperlink ref="D10" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
-    <hyperlink ref="D36" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
-    <hyperlink ref="D39" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
-    <hyperlink ref="D12" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
-    <hyperlink ref="D52" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
-    <hyperlink ref="D43" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
-    <hyperlink ref="D56" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
-    <hyperlink ref="D60" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
-    <hyperlink ref="D71" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
-    <hyperlink ref="D47" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
-    <hyperlink ref="D21" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
+    <hyperlink ref="D22" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
+    <hyperlink ref="D62" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
+    <hyperlink ref="D40" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
+    <hyperlink ref="D30" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
+    <hyperlink ref="D61" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
+    <hyperlink ref="D77" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
+    <hyperlink ref="D60" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
+    <hyperlink ref="D25" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
+    <hyperlink ref="D32" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
+    <hyperlink ref="D69" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
+    <hyperlink ref="D76" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
+    <hyperlink ref="D72" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
+    <hyperlink ref="D16" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
+    <hyperlink ref="D15" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
+    <hyperlink ref="D56" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
+    <hyperlink ref="D78" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
+    <hyperlink ref="D43" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
+    <hyperlink ref="D28" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
+    <hyperlink ref="D67" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
+    <hyperlink ref="D44" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
+    <hyperlink ref="D19" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
+    <hyperlink ref="D58" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
+    <hyperlink ref="D36" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
+    <hyperlink ref="D73" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
+    <hyperlink ref="D51" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
+    <hyperlink ref="D7" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
+    <hyperlink ref="D31" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
+    <hyperlink ref="D46" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
+    <hyperlink ref="D49" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
+    <hyperlink ref="D75" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
+    <hyperlink ref="D12" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
+    <hyperlink ref="D38" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
+    <hyperlink ref="D41" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
+    <hyperlink ref="D14" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
+    <hyperlink ref="D55" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
+    <hyperlink ref="D45" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
+    <hyperlink ref="D59" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
+    <hyperlink ref="D63" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
+    <hyperlink ref="D74" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
+    <hyperlink ref="D50" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
+    <hyperlink ref="D23" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
     <hyperlink ref="D4" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
-    <hyperlink ref="D25" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
-    <hyperlink ref="D62" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D77" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
-    <hyperlink ref="D61" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
-    <hyperlink ref="D65" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
-    <hyperlink ref="D7" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
-    <hyperlink ref="D18" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
-    <hyperlink ref="D35" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
-    <hyperlink ref="D50" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
-    <hyperlink ref="D51" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
-    <hyperlink ref="D68" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
-    <hyperlink ref="D22" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
-    <hyperlink ref="D24" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
-    <hyperlink ref="D37" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
-    <hyperlink ref="D27" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
-    <hyperlink ref="D16" r:id="rId69" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
-    <hyperlink ref="D31" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
+    <hyperlink ref="D27" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
+    <hyperlink ref="D65" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
+    <hyperlink ref="D80" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D64" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
+    <hyperlink ref="D68" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
+    <hyperlink ref="D8" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
+    <hyperlink ref="D20" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
+    <hyperlink ref="D37" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
+    <hyperlink ref="D53" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
+    <hyperlink ref="D54" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
+    <hyperlink ref="D71" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
+    <hyperlink ref="D24" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D26" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
+    <hyperlink ref="D39" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
+    <hyperlink ref="D29" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
+    <hyperlink ref="D18" r:id="rId69" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
+    <hyperlink ref="D33" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
     <hyperlink ref="D2" r:id="rId71" display="mailto:frank.vyncke@yin4yang.com" xr:uid="{E29600CB-349C-4C55-AC29-3B61912C4757}"/>
-    <hyperlink ref="D76" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
-    <hyperlink ref="D19" r:id="rId73" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
+    <hyperlink ref="D79" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
+    <hyperlink ref="D21" r:id="rId73" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
     <hyperlink ref="D5" r:id="rId74" xr:uid="{33D12C26-CC5E-4925-86B6-4AE855A6371F}"/>
     <hyperlink ref="G5" r:id="rId75" xr:uid="{2FA39695-7884-42EC-9380-C8EFD7B7EAD9}"/>
-    <hyperlink ref="D11" r:id="rId76" xr:uid="{B237CB2B-4475-8C4E-A2C5-5839FB07318E}"/>
+    <hyperlink ref="D13" r:id="rId76" xr:uid="{B237CB2B-4475-8C4E-A2C5-5839FB07318E}"/>
+    <hyperlink ref="D6" r:id="rId77" xr:uid="{3C6DADFB-91D3-4B16-BA60-22286260FB72}"/>
+    <hyperlink ref="G6" r:id="rId78" xr:uid="{EF6627CA-3B1A-440B-85D4-A1B7067549BD}"/>
+    <hyperlink ref="D10" r:id="rId79" xr:uid="{058D1BE7-4CFF-4740-BC92-2074C717A677}"/>
+    <hyperlink ref="G10" r:id="rId80" xr:uid="{B9062A46-48F6-45FB-8197-4FD986CC482D}"/>
+    <hyperlink ref="D47" r:id="rId81" xr:uid="{0CFEC845-7F90-4802-9D24-4AC8905CD11B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId77"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId82"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolve request #41 for CPAP
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBD7328-684F-42B8-9045-A6833C6033F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364A4C5D-92DB-41CF-A4C4-A193A295D698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12771" yWindow="0" windowWidth="13029" windowHeight="16509" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
+    <workbookView xWindow="-32650" yWindow="1360" windowWidth="25700" windowHeight="16050" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
     <sheet name="PDF Prefix Registry" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="395">
   <si>
     <t>ITXT</t>
   </si>
@@ -1198,6 +1198,24 @@
   </si>
   <si>
     <t>j.hagen@xs4all.nl</t>
+  </si>
+  <si>
+    <t>CPAP</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Van Vuren</t>
+  </si>
+  <si>
+    <t>james.vanvuren@safesend.com</t>
+  </si>
+  <si>
+    <t>cPaperless, LLC</t>
+  </si>
+  <si>
+    <t>https://github.com/adobe/pdf-names-list/issues/41</t>
   </si>
 </sst>
 </file>
@@ -1611,11 +1629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -2006,782 +2024,785 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>389</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>390</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>391</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>392</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="5">
-        <v>40105.464583333334</v>
+        <v>393</v>
+      </c>
+      <c r="F19" s="7">
+        <v>45484</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>276</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>277</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>278</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>279</v>
+        <v>28</v>
       </c>
       <c r="F20" s="5">
-        <v>44580</v>
-      </c>
-      <c r="G20" t="s">
-        <v>354</v>
+        <v>40105.464583333334</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>338</v>
+        <v>276</v>
       </c>
       <c r="B21" t="s">
-        <v>339</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>340</v>
+        <v>277</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>341</v>
+        <v>278</v>
       </c>
       <c r="E21" t="s">
-        <v>342</v>
+        <v>279</v>
       </c>
       <c r="F21" s="5">
-        <v>44915</v>
+        <v>44580</v>
+      </c>
+      <c r="G21" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>261</v>
+        <v>338</v>
       </c>
       <c r="B22" t="s">
-        <v>262</v>
+        <v>339</v>
       </c>
       <c r="C22" t="s">
-        <v>263</v>
+        <v>340</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>265</v>
+        <v>341</v>
+      </c>
+      <c r="E22" t="s">
+        <v>342</v>
       </c>
       <c r="F22" s="5">
-        <v>44174</v>
+        <v>44915</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>261</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>262</v>
       </c>
       <c r="C23" t="s">
-        <v>124</v>
+        <v>263</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E23" t="s">
-        <v>305</v>
+        <v>264</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>265</v>
       </c>
       <c r="F23" s="5">
-        <v>41924</v>
+        <v>44174</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>296</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>299</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>300</v>
+        <v>124</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>298</v>
+        <v>125</v>
       </c>
       <c r="E24" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="F24" s="5">
-        <v>44580</v>
-      </c>
-      <c r="G24" t="s">
-        <v>302</v>
+        <v>41924</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>190</v>
+        <v>296</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>299</v>
       </c>
       <c r="C25" t="s">
-        <v>192</v>
+        <v>300</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>193</v>
+        <v>298</v>
       </c>
       <c r="E25" t="s">
-        <v>194</v>
+        <v>297</v>
       </c>
       <c r="F25" s="5">
-        <v>43231</v>
+        <v>44580</v>
+      </c>
+      <c r="G25" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>306</v>
+        <v>190</v>
       </c>
       <c r="B26" t="s">
-        <v>307</v>
+        <v>191</v>
       </c>
       <c r="C26" t="s">
-        <v>308</v>
+        <v>192</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>309</v>
+        <v>193</v>
       </c>
       <c r="E26" t="s">
-        <v>310</v>
+        <v>194</v>
       </c>
       <c r="F26" s="5">
-        <v>44581</v>
-      </c>
-      <c r="G26" t="s">
-        <v>302</v>
+        <v>43231</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>306</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>307</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>308</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>134</v>
+        <v>309</v>
       </c>
       <c r="E27" t="s">
-        <v>135</v>
+        <v>310</v>
       </c>
       <c r="F27" s="5">
-        <v>41680</v>
+        <v>44581</v>
+      </c>
+      <c r="G27" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="F28" s="5">
-        <v>40079.444444444445</v>
+        <v>41680</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>324</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>213</v>
+        <v>11</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>325</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>326</v>
+        <v>13</v>
       </c>
       <c r="F29" s="5">
-        <v>44774</v>
+        <v>40079.444444444445</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>247</v>
+        <v>324</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
+        <v>212</v>
       </c>
       <c r="C30" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>249</v>
+        <v>325</v>
       </c>
       <c r="E30" t="s">
-        <v>250</v>
+        <v>326</v>
       </c>
       <c r="F30" s="5">
-        <v>44037</v>
+        <v>44774</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>247</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>248</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>55</v>
+        <v>249</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>250</v>
       </c>
       <c r="F31" s="5">
-        <v>40714.365972222222</v>
+        <v>44037</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>185</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>188</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s">
-        <v>189</v>
+        <v>56</v>
       </c>
       <c r="F32" s="5">
-        <v>43212</v>
+        <v>40714.365972222222</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>315</v>
+        <v>185</v>
       </c>
       <c r="B33" t="s">
-        <v>316</v>
+        <v>186</v>
       </c>
       <c r="C33" t="s">
-        <v>317</v>
+        <v>187</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>329</v>
+        <v>188</v>
       </c>
       <c r="E33" t="s">
-        <v>318</v>
-      </c>
-      <c r="F33" s="7">
-        <v>44676</v>
+        <v>189</v>
+      </c>
+      <c r="F33" s="5">
+        <v>43212</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>235</v>
+        <v>315</v>
       </c>
       <c r="B34" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="C34" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>223</v>
+        <v>329</v>
       </c>
       <c r="E34" t="s">
-        <v>224</v>
-      </c>
-      <c r="F34" s="5">
-        <v>43973</v>
+        <v>318</v>
+      </c>
+      <c r="F34" s="7">
+        <v>44676</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="B35" t="s">
-        <v>226</v>
+        <v>303</v>
       </c>
       <c r="C35" t="s">
-        <v>227</v>
+        <v>304</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E35" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F35" s="5">
-        <v>43616</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>225</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>227</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>37</v>
+        <v>228</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>229</v>
       </c>
       <c r="F36" s="5">
-        <v>40305.557638888888</v>
+        <v>43616</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>280</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>281</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>283</v>
+        <v>37</v>
       </c>
       <c r="E37" t="s">
-        <v>284</v>
+        <v>38</v>
       </c>
       <c r="F37" s="5">
-        <v>44580</v>
+        <v>40305.557638888888</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>280</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>281</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>282</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>80</v>
+        <v>283</v>
       </c>
       <c r="E38" t="s">
-        <v>81</v>
+        <v>284</v>
       </c>
       <c r="F38" s="5">
-        <v>40966</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>374</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>202</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>375</v>
+        <v>79</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>376</v>
+        <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>377</v>
+        <v>81</v>
       </c>
       <c r="F39" s="5">
-        <v>45355</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>378</v>
+        <v>40966</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>319</v>
+        <v>374</v>
       </c>
       <c r="B40" t="s">
-        <v>320</v>
+        <v>202</v>
       </c>
       <c r="C40" t="s">
-        <v>321</v>
+        <v>375</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>322</v>
+        <v>376</v>
       </c>
       <c r="E40" t="s">
-        <v>323</v>
+        <v>377</v>
       </c>
       <c r="F40" s="5">
-        <v>44700</v>
+        <v>45355</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>251</v>
+        <v>319</v>
       </c>
       <c r="B41" t="s">
-        <v>252</v>
+        <v>320</v>
       </c>
       <c r="C41" t="s">
-        <v>253</v>
+        <v>321</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>255</v>
+        <v>322</v>
+      </c>
+      <c r="E41" t="s">
+        <v>323</v>
       </c>
       <c r="F41" s="5">
-        <v>44151</v>
+        <v>44700</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>251</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>253</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" t="s">
-        <v>86</v>
+        <v>254</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>255</v>
       </c>
       <c r="F42" s="5">
-        <v>41736</v>
+        <v>44151</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>222</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>303</v>
+        <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>304</v>
+        <v>84</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>223</v>
+        <v>85</v>
       </c>
       <c r="E43" t="s">
-        <v>224</v>
+        <v>86</v>
       </c>
       <c r="F43" s="5">
-        <v>43614</v>
+        <v>41736</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>222</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>303</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>304</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>3</v>
+        <v>223</v>
       </c>
       <c r="E44" t="s">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="F44" s="5">
-        <v>39932.427083333336</v>
+        <v>43614</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F45" s="5">
-        <v>40094.793055555558</v>
+        <v>39932.427083333336</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>101</v>
+        <v>23</v>
+      </c>
+      <c r="F46" s="5">
+        <v>40094.793055555558</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>385</v>
+        <v>97</v>
       </c>
       <c r="B47" t="s">
-        <v>237</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>238</v>
+        <v>99</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>388</v>
+        <v>100</v>
       </c>
       <c r="E47" t="s">
-        <v>386</v>
-      </c>
-      <c r="F47" s="5">
-        <v>45419</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>387</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>385</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>237</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>238</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>60</v>
+        <v>388</v>
       </c>
       <c r="E48" t="s">
-        <v>61</v>
+        <v>386</v>
       </c>
       <c r="F48" s="5">
-        <v>40854.607638888891</v>
+        <v>45419</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>364</v>
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>365</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>366</v>
+        <v>59</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>367</v>
+        <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>217</v>
+        <v>61</v>
       </c>
       <c r="F49" s="5">
-        <v>45147</v>
-      </c>
-      <c r="G49" t="s">
-        <v>368</v>
+        <v>40854.607638888891</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>218</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>78</v>
+        <v>364</v>
+      </c>
+      <c r="B50" t="s">
+        <v>365</v>
       </c>
       <c r="C50" t="s">
-        <v>220</v>
+        <v>366</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>219</v>
+        <v>367</v>
+      </c>
+      <c r="E50" t="s">
+        <v>217</v>
       </c>
       <c r="F50" s="5">
-        <v>43503</v>
+        <v>45147</v>
+      </c>
+      <c r="G50" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B51" t="s">
-        <v>63</v>
+        <v>218</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>220</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E51" t="s">
-        <v>66</v>
+        <v>221</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="F51" s="5">
-        <v>41039</v>
+        <v>43503</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="E52" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="F52" s="5">
-        <v>41900</v>
+        <v>41039</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="E53" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="F53" s="5">
-        <v>40560.762499999997</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>369</v>
+        <v>44</v>
       </c>
       <c r="B54" t="s">
-        <v>370</v>
+        <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>371</v>
+        <v>46</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>372</v>
+        <v>47</v>
       </c>
       <c r="E54" t="s">
-        <v>373</v>
+        <v>48</v>
       </c>
       <c r="F54" s="5">
-        <v>45275</v>
+        <v>40560.762499999997</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>211</v>
+        <v>369</v>
       </c>
       <c r="B55" t="s">
-        <v>212</v>
+        <v>370</v>
       </c>
       <c r="C55" t="s">
-        <v>213</v>
+        <v>371</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>214</v>
+        <v>372</v>
       </c>
       <c r="E55" t="s">
-        <v>215</v>
+        <v>373</v>
       </c>
       <c r="F55" s="5">
-        <v>43502</v>
+        <v>45275</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>285</v>
+        <v>211</v>
       </c>
       <c r="B56" t="s">
-        <v>288</v>
+        <v>212</v>
       </c>
       <c r="C56" t="s">
-        <v>289</v>
+        <v>213</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>290</v>
+        <v>214</v>
       </c>
       <c r="E56" t="s">
-        <v>287</v>
+        <v>215</v>
       </c>
       <c r="F56" s="5">
-        <v>44580</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B57" t="s">
         <v>288</v>
@@ -2801,450 +2822,450 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>286</v>
       </c>
       <c r="B58" t="s">
-        <v>93</v>
+        <v>288</v>
       </c>
       <c r="C58" t="s">
-        <v>94</v>
+        <v>289</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>95</v>
+        <v>290</v>
       </c>
       <c r="E58" t="s">
-        <v>96</v>
+        <v>287</v>
       </c>
       <c r="F58" s="5">
-        <v>41780</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>164</v>
+        <v>92</v>
       </c>
       <c r="B59" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="C59" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>167</v>
+        <v>95</v>
       </c>
       <c r="E59" t="s">
-        <v>168</v>
+        <v>96</v>
       </c>
       <c r="F59" s="5">
-        <v>42530</v>
+        <v>41780</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>216</v>
+        <v>164</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="C60" t="s">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>125</v>
+        <v>167</v>
       </c>
       <c r="E60" t="s">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="F60" s="5">
-        <v>43502</v>
+        <v>42530</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>216</v>
       </c>
       <c r="B61" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="E61" t="s">
-        <v>33</v>
+        <v>217</v>
       </c>
       <c r="F61" s="5">
-        <v>40164.4375</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="E62" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="F62" s="5">
-        <v>41854</v>
+        <v>40164.4375</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E63" t="s">
+        <v>106</v>
+      </c>
+      <c r="F63" s="5">
+        <v>41854</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
         <v>201</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>202</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>203</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E64" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F64" s="7">
         <v>37415</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A64" s="8" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A65" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B65" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C65" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E65" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F64" s="5">
+      <c r="F65" s="5">
         <v>43997</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>256</v>
-      </c>
-      <c r="B65" t="s">
-        <v>257</v>
-      </c>
-      <c r="C65" t="s">
-        <v>258</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="F65" s="5">
-        <v>44166</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>256</v>
       </c>
       <c r="B66" t="s">
-        <v>108</v>
+        <v>257</v>
       </c>
       <c r="C66" t="s">
-        <v>109</v>
+        <v>258</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E66" t="s">
-        <v>111</v>
+        <v>259</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="F66" s="5">
-        <v>41857</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
-        <v>147</v>
+        <v>108</v>
       </c>
       <c r="C67" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>149</v>
+        <v>110</v>
       </c>
       <c r="E67" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="F67" s="5">
-        <v>42467</v>
+        <v>41857</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E68" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="F68" s="5">
-        <v>42420</v>
+        <v>42467</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>230</v>
+        <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>231</v>
+        <v>137</v>
       </c>
       <c r="C69" t="s">
-        <v>232</v>
+        <v>138</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>233</v>
+        <v>139</v>
       </c>
       <c r="E69" t="s">
-        <v>234</v>
+        <v>140</v>
       </c>
       <c r="F69" s="5">
-        <v>43973</v>
+        <v>42420</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>230</v>
       </c>
       <c r="B70" t="s">
-        <v>15</v>
+        <v>231</v>
       </c>
       <c r="C70" t="s">
-        <v>16</v>
+        <v>232</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
       <c r="E70" t="s">
-        <v>18</v>
+        <v>234</v>
       </c>
       <c r="F70" s="5">
-        <v>40081.550694444442</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>152</v>
+        <v>16</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>153</v>
+        <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>154</v>
+        <v>18</v>
       </c>
       <c r="F71" s="5">
-        <v>42472</v>
+        <v>40081.550694444442</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="B72" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="C72" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="E72" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="F72" s="5">
-        <v>43054</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>236</v>
+        <v>181</v>
       </c>
       <c r="B73" t="s">
-        <v>303</v>
+        <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>304</v>
+        <v>182</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="E73" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="F73" s="5">
-        <v>43973</v>
+        <v>43054</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>291</v>
+        <v>236</v>
       </c>
       <c r="B74" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="C74" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>293</v>
+        <v>223</v>
       </c>
       <c r="E74" t="s">
-        <v>292</v>
+        <v>224</v>
       </c>
       <c r="F74" s="5">
-        <v>44580</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>175</v>
+        <v>291</v>
       </c>
       <c r="B75" t="s">
-        <v>176</v>
+        <v>294</v>
       </c>
       <c r="C75" t="s">
-        <v>177</v>
+        <v>295</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>178</v>
+        <v>293</v>
       </c>
       <c r="E75" t="s">
-        <v>179</v>
+        <v>292</v>
       </c>
       <c r="F75" s="5">
-        <v>42739</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>379</v>
+        <v>175</v>
       </c>
       <c r="B76" t="s">
-        <v>380</v>
+        <v>176</v>
       </c>
       <c r="C76" t="s">
-        <v>381</v>
+        <v>177</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>382</v>
+        <v>178</v>
       </c>
       <c r="E76" t="s">
-        <v>383</v>
+        <v>179</v>
       </c>
       <c r="F76" s="5">
-        <v>45358</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>384</v>
+        <v>42739</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>379</v>
       </c>
       <c r="B77" t="s">
-        <v>40</v>
+        <v>380</v>
       </c>
       <c r="C77" t="s">
-        <v>41</v>
+        <v>381</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>42</v>
+        <v>382</v>
       </c>
       <c r="E77" t="s">
-        <v>43</v>
+        <v>383</v>
       </c>
       <c r="F77" s="5">
-        <v>40522.519444444442</v>
+        <v>45358</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="B78" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="E78" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="F78" s="5">
-        <v>41890</v>
+        <v>40522.519444444442</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="C79" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E79" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="F79" s="5">
-        <v>42852</v>
+        <v>41890</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="B80" t="s">
         <v>68</v>
@@ -3264,81 +3285,101 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="B81" t="s">
-        <v>207</v>
+        <v>68</v>
       </c>
       <c r="C81" t="s">
-        <v>208</v>
+        <v>69</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="F81" s="7">
-        <v>43487</v>
+        <v>70</v>
+      </c>
+      <c r="E81" t="s">
+        <v>71</v>
+      </c>
+      <c r="F81" s="5">
+        <v>42852</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="B82" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="C82" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E82" t="s">
-        <v>163</v>
-      </c>
-      <c r="F82" s="5">
-        <v>42505</v>
+        <v>209</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F82" s="7">
+        <v>43487</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>333</v>
+        <v>159</v>
       </c>
       <c r="B83" t="s">
-        <v>334</v>
+        <v>160</v>
       </c>
       <c r="C83" t="s">
-        <v>335</v>
+        <v>161</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>336</v>
+        <v>162</v>
       </c>
       <c r="E83" t="s">
-        <v>337</v>
+        <v>163</v>
       </c>
       <c r="F83" s="5">
-        <v>44775</v>
+        <v>42505</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
+        <v>333</v>
+      </c>
+      <c r="B84" t="s">
+        <v>334</v>
+      </c>
+      <c r="C84" t="s">
+        <v>335</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E84" t="s">
+        <v>337</v>
+      </c>
+      <c r="F84" s="5">
+        <v>44775</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
         <v>141</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>142</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>143</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E85" t="s">
         <v>145</v>
       </c>
-      <c r="F84" s="5">
+      <c r="F85" s="5">
         <v>42439</v>
       </c>
     </row>
@@ -3349,79 +3390,79 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D55" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
-    <hyperlink ref="D60" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
-    <hyperlink ref="D50" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
-    <hyperlink ref="D43" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
-    <hyperlink ref="D35" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
-    <hyperlink ref="D69" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
-    <hyperlink ref="D34" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
-    <hyperlink ref="D73" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
+    <hyperlink ref="D56" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D61" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
+    <hyperlink ref="D51" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D44" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D36" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
+    <hyperlink ref="D70" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
+    <hyperlink ref="D35" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
+    <hyperlink ref="D74" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
     <hyperlink ref="D11" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
     <hyperlink ref="D9" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
     <hyperlink ref="D3" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
-    <hyperlink ref="D22" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
-    <hyperlink ref="D65" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
-    <hyperlink ref="D41" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
-    <hyperlink ref="D30" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
-    <hyperlink ref="D64" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
-    <hyperlink ref="D81" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
-    <hyperlink ref="D63" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
-    <hyperlink ref="D25" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
-    <hyperlink ref="D32" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
-    <hyperlink ref="D72" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
-    <hyperlink ref="D80" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
-    <hyperlink ref="D75" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
+    <hyperlink ref="D23" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
+    <hyperlink ref="D66" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
+    <hyperlink ref="D42" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
+    <hyperlink ref="D31" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
+    <hyperlink ref="D65" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
+    <hyperlink ref="D82" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
+    <hyperlink ref="D64" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
+    <hyperlink ref="D26" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
+    <hyperlink ref="D33" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
+    <hyperlink ref="D73" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
+    <hyperlink ref="D81" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
+    <hyperlink ref="D76" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
     <hyperlink ref="D16" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
     <hyperlink ref="D15" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
-    <hyperlink ref="D59" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
-    <hyperlink ref="D82" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
-    <hyperlink ref="D44" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
-    <hyperlink ref="D28" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
-    <hyperlink ref="D70" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
-    <hyperlink ref="D45" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
-    <hyperlink ref="D19" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
-    <hyperlink ref="D61" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
-    <hyperlink ref="D36" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
-    <hyperlink ref="D77" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
-    <hyperlink ref="D53" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
+    <hyperlink ref="D60" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
+    <hyperlink ref="D83" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
+    <hyperlink ref="D45" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
+    <hyperlink ref="D29" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
+    <hyperlink ref="D71" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
+    <hyperlink ref="D46" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
+    <hyperlink ref="D20" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
+    <hyperlink ref="D62" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
+    <hyperlink ref="D37" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
+    <hyperlink ref="D78" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
+    <hyperlink ref="D54" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
     <hyperlink ref="D7" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
-    <hyperlink ref="D31" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
-    <hyperlink ref="D48" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
-    <hyperlink ref="D51" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
-    <hyperlink ref="D79" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
+    <hyperlink ref="D32" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
+    <hyperlink ref="D49" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
+    <hyperlink ref="D52" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
+    <hyperlink ref="D80" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
     <hyperlink ref="D12" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
-    <hyperlink ref="D38" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
-    <hyperlink ref="D42" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
+    <hyperlink ref="D39" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
+    <hyperlink ref="D43" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
     <hyperlink ref="D14" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
-    <hyperlink ref="D58" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
-    <hyperlink ref="D46" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
-    <hyperlink ref="D62" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
-    <hyperlink ref="D66" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
-    <hyperlink ref="D78" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
-    <hyperlink ref="D52" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
-    <hyperlink ref="D23" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
+    <hyperlink ref="D59" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
+    <hyperlink ref="D47" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
+    <hyperlink ref="D63" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
+    <hyperlink ref="D67" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
+    <hyperlink ref="D79" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
+    <hyperlink ref="D53" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
+    <hyperlink ref="D24" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
     <hyperlink ref="D4" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
-    <hyperlink ref="D27" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
-    <hyperlink ref="D68" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D84" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
-    <hyperlink ref="D67" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
-    <hyperlink ref="D71" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
+    <hyperlink ref="D28" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
+    <hyperlink ref="D69" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
+    <hyperlink ref="D85" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D68" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
+    <hyperlink ref="D72" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
     <hyperlink ref="D8" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
-    <hyperlink ref="D20" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
-    <hyperlink ref="D37" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
-    <hyperlink ref="D56" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
-    <hyperlink ref="D57" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
-    <hyperlink ref="D74" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
-    <hyperlink ref="D24" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
-    <hyperlink ref="D26" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
-    <hyperlink ref="D40" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
-    <hyperlink ref="D29" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
+    <hyperlink ref="D21" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
+    <hyperlink ref="D38" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
+    <hyperlink ref="D57" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
+    <hyperlink ref="D58" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
+    <hyperlink ref="D75" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
+    <hyperlink ref="D25" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D27" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
+    <hyperlink ref="D41" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
+    <hyperlink ref="D30" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
     <hyperlink ref="D18" r:id="rId69" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
-    <hyperlink ref="D33" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
+    <hyperlink ref="D34" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
     <hyperlink ref="D2" r:id="rId71" display="mailto:frank.vyncke@yin4yang.com" xr:uid="{E29600CB-349C-4C55-AC29-3B61912C4757}"/>
-    <hyperlink ref="D83" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
-    <hyperlink ref="D21" r:id="rId73" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
+    <hyperlink ref="D84" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
+    <hyperlink ref="D22" r:id="rId73" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
     <hyperlink ref="D5" r:id="rId74" xr:uid="{33D12C26-CC5E-4925-86B6-4AE855A6371F}"/>
     <hyperlink ref="G5" r:id="rId75" xr:uid="{2FA39695-7884-42EC-9380-C8EFD7B7EAD9}"/>
     <hyperlink ref="D13" r:id="rId76" xr:uid="{B237CB2B-4475-8C4E-A2C5-5839FB07318E}"/>
@@ -3429,16 +3470,17 @@
     <hyperlink ref="G6" r:id="rId78" xr:uid="{EF6627CA-3B1A-440B-85D4-A1B7067549BD}"/>
     <hyperlink ref="D10" r:id="rId79" xr:uid="{058D1BE7-4CFF-4740-BC92-2074C717A677}"/>
     <hyperlink ref="G10" r:id="rId80" xr:uid="{B9062A46-48F6-45FB-8197-4FD986CC482D}"/>
-    <hyperlink ref="D49" r:id="rId81" xr:uid="{0CFEC845-7F90-4802-9D24-4AC8905CD11B}"/>
-    <hyperlink ref="D54" r:id="rId82" xr:uid="{81B44739-2F1A-4DDB-90E8-2523712052F0}"/>
-    <hyperlink ref="D39" r:id="rId83" xr:uid="{72B2BA10-0B55-4ACF-9CC1-DA30FB4C2741}"/>
-    <hyperlink ref="G39" r:id="rId84" xr:uid="{1106BFBB-F6F3-4E8A-8B65-06381130271C}"/>
-    <hyperlink ref="D76" r:id="rId85" xr:uid="{249742DB-9523-4D5C-B3FC-194F7D7BB889}"/>
-    <hyperlink ref="G76" r:id="rId86" xr:uid="{BD0ABADB-115E-43D9-8791-2BFF7CAEC355}"/>
-    <hyperlink ref="G47" r:id="rId87" xr:uid="{44657DD4-3FFA-4E6F-8898-631518A1BFDC}"/>
-    <hyperlink ref="D47" r:id="rId88" xr:uid="{D5A339A1-161D-40E3-9F69-B4599246184B}"/>
+    <hyperlink ref="D50" r:id="rId81" xr:uid="{0CFEC845-7F90-4802-9D24-4AC8905CD11B}"/>
+    <hyperlink ref="D55" r:id="rId82" xr:uid="{81B44739-2F1A-4DDB-90E8-2523712052F0}"/>
+    <hyperlink ref="D40" r:id="rId83" xr:uid="{72B2BA10-0B55-4ACF-9CC1-DA30FB4C2741}"/>
+    <hyperlink ref="G40" r:id="rId84" xr:uid="{1106BFBB-F6F3-4E8A-8B65-06381130271C}"/>
+    <hyperlink ref="D77" r:id="rId85" xr:uid="{249742DB-9523-4D5C-B3FC-194F7D7BB889}"/>
+    <hyperlink ref="G77" r:id="rId86" xr:uid="{BD0ABADB-115E-43D9-8791-2BFF7CAEC355}"/>
+    <hyperlink ref="G48" r:id="rId87" xr:uid="{44657DD4-3FFA-4E6F-8898-631518A1BFDC}"/>
+    <hyperlink ref="D48" r:id="rId88" xr:uid="{D5A339A1-161D-40E3-9F69-B4599246184B}"/>
+    <hyperlink ref="G19" r:id="rId89" xr:uid="{C64F139E-8286-4E7A-8B5E-9D69FC9A0C25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId89"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId90"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolve #43 and #44
MSFT and ESIC updates
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364A4C5D-92DB-41CF-A4C4-A193A295D698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FF7809-DAE0-45D1-9D17-F8F451FCBF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32650" yWindow="1360" windowWidth="25700" windowHeight="16050" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
     <sheet name="PDF Prefix Registry" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="402">
   <si>
     <t>ITXT</t>
   </si>
@@ -221,15 +221,6 @@
     <t>MSFT</t>
   </si>
   <si>
-    <t>Barack</t>
-  </si>
-  <si>
-    <t>Cohen</t>
-  </si>
-  <si>
-    <t>barakc@microsoft.com</t>
-  </si>
-  <si>
     <t>Microsoft Corporation</t>
   </si>
   <si>
@@ -1016,10 +1007,6 @@
     <t xml:space="preserve">info@stefanochizzolini.it </t>
   </si>
   <si>
-    <t xml:space="preserve">Secretariat@cip4.org 
-Tim.Donahue@Kodak.com  </t>
-  </si>
-  <si>
     <t xml:space="preserve">q@as207960.net </t>
   </si>
   <si>
@@ -1216,6 +1203,39 @@
   </si>
   <si>
     <t>https://github.com/adobe/pdf-names-list/issues/41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/adobe/pdf-names-list/issues/44 </t>
+  </si>
+  <si>
+    <t>pdf_names_registry@microsoft.com</t>
+  </si>
+  <si>
+    <t>S.</t>
+  </si>
+  <si>
+    <t>G.</t>
+  </si>
+  <si>
+    <t>Secretariat@cip4.org, Tim.Donahue@Kodak.com</t>
+  </si>
+  <si>
+    <t>ESIC</t>
+  </si>
+  <si>
+    <t>ETSI Electronic Signatures and Infrastructures Committee (for PAdES)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/adobe/pdf-names-list/issues/43 </t>
+  </si>
+  <si>
+    <t>Antoine</t>
+  </si>
+  <si>
+    <t>Burckard</t>
+  </si>
+  <si>
+    <t>Antoine.Burckard@etsi.org</t>
   </si>
 </sst>
 </file>
@@ -1308,12 +1328,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1629,11 +1649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -1649,65 +1669,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F2" s="5">
         <v>44775</v>
       </c>
       <c r="G2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="C3" t="s">
-        <v>268</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="F3" s="5">
         <v>44221</v>
@@ -1715,19 +1735,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>127</v>
-      </c>
-      <c r="C4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" t="s">
-        <v>130</v>
       </c>
       <c r="F4" s="5">
         <v>41931</v>
@@ -1735,48 +1755,48 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E5" t="s">
         <v>343</v>
-      </c>
-      <c r="B5" t="s">
-        <v>344</v>
-      </c>
-      <c r="C5" t="s">
-        <v>345</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="E5" t="s">
-        <v>347</v>
       </c>
       <c r="F5" s="5">
         <v>44987</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B6" t="s">
+        <v>352</v>
+      </c>
+      <c r="C6" t="s">
+        <v>353</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E6" t="s">
         <v>355</v>
-      </c>
-      <c r="B6" t="s">
-        <v>356</v>
-      </c>
-      <c r="C6" t="s">
-        <v>357</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="E6" t="s">
-        <v>359</v>
       </c>
       <c r="F6" s="5">
         <v>45147</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -1801,19 +1821,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" t="s">
         <v>155</v>
-      </c>
-      <c r="B8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E8" t="s">
-        <v>158</v>
       </c>
       <c r="F8" s="5">
         <v>42492</v>
@@ -1821,19 +1841,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" s="8" t="s">
         <v>272</v>
-      </c>
-      <c r="C9" t="s">
-        <v>273</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>275</v>
       </c>
       <c r="F9" s="5">
         <v>44280</v>
@@ -1841,42 +1861,42 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B10" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C10" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>358</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>362</v>
       </c>
       <c r="F10" s="5">
         <v>45147</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>243</v>
-      </c>
-      <c r="C11" t="s">
-        <v>244</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E11" t="s">
-        <v>246</v>
       </c>
       <c r="F11" s="5">
         <v>43997</v>
@@ -1884,19 +1904,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" t="s">
-        <v>76</v>
       </c>
       <c r="F12" s="5">
         <v>40997</v>
@@ -1904,19 +1924,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B13" t="s">
+        <v>346</v>
+      </c>
+      <c r="C13" t="s">
+        <v>347</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E13" t="s">
         <v>349</v>
-      </c>
-      <c r="B13" t="s">
-        <v>350</v>
-      </c>
-      <c r="C13" t="s">
-        <v>351</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="E13" t="s">
-        <v>353</v>
       </c>
       <c r="F13" s="5">
         <v>45142</v>
@@ -1924,19 +1944,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B14" t="s">
+      <c r="E14" t="s">
         <v>88</v>
-      </c>
-      <c r="C14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" t="s">
-        <v>91</v>
       </c>
       <c r="F14" s="5">
         <v>41758</v>
@@ -1944,19 +1964,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B15" t="s">
+      <c r="E15" t="s">
         <v>170</v>
-      </c>
-      <c r="C15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E15" t="s">
-        <v>173</v>
       </c>
       <c r="F15" s="5">
         <v>42739</v>
@@ -1964,19 +1984,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E16" t="s">
         <v>170</v>
-      </c>
-      <c r="C16" t="s">
-        <v>171</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E16" t="s">
-        <v>173</v>
       </c>
       <c r="F16" s="5">
         <v>42739</v>
@@ -1992,8 +2012,8 @@
       <c r="C17" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>328</v>
+      <c r="D17" s="9" t="s">
+        <v>395</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -2004,45 +2024,45 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>308</v>
+      </c>
+      <c r="B18" t="s">
+        <v>309</v>
+      </c>
+      <c r="C18" t="s">
+        <v>310</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E18" t="s">
         <v>311</v>
       </c>
-      <c r="B18" t="s">
-        <v>312</v>
-      </c>
-      <c r="C18" t="s">
-        <v>313</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E18" t="s">
-        <v>314</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>44676</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>385</v>
+      </c>
+      <c r="B19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C19" t="s">
+        <v>387</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E19" t="s">
         <v>389</v>
       </c>
-      <c r="B19" t="s">
+      <c r="F19" s="6">
+        <v>45484</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="C19" t="s">
-        <v>391</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="E19" t="s">
-        <v>393</v>
-      </c>
-      <c r="F19" s="7">
-        <v>45484</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -2067,42 +2087,42 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>273</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E21" t="s">
         <v>276</v>
-      </c>
-      <c r="B21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" t="s">
-        <v>277</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E21" t="s">
-        <v>279</v>
       </c>
       <c r="F21" s="5">
         <v>44580</v>
       </c>
       <c r="G21" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>334</v>
+      </c>
+      <c r="B22" t="s">
+        <v>335</v>
+      </c>
+      <c r="C22" t="s">
+        <v>336</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E22" t="s">
         <v>338</v>
-      </c>
-      <c r="B22" t="s">
-        <v>339</v>
-      </c>
-      <c r="C22" t="s">
-        <v>340</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="E22" t="s">
-        <v>342</v>
       </c>
       <c r="F22" s="5">
         <v>44915</v>
@@ -2110,19 +2130,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
+        <v>258</v>
+      </c>
+      <c r="B23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C23" t="s">
+        <v>260</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B23" t="s">
+      <c r="E23" s="8" t="s">
         <v>262</v>
-      </c>
-      <c r="C23" t="s">
-        <v>263</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>265</v>
       </c>
       <c r="F23" s="5">
         <v>44174</v>
@@ -2130,19 +2150,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B24" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="E24" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F24" s="5">
         <v>41924</v>
@@ -2150,691 +2170,697 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>293</v>
+      </c>
+      <c r="B25" t="s">
         <v>296</v>
       </c>
-      <c r="B25" t="s">
-        <v>299</v>
-      </c>
       <c r="C25" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E25" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F25" s="5">
         <v>44580</v>
       </c>
       <c r="G25" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>190</v>
+        <v>396</v>
       </c>
       <c r="B26" t="s">
-        <v>191</v>
+        <v>399</v>
       </c>
       <c r="C26" t="s">
-        <v>192</v>
+        <v>400</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>193</v>
+        <v>401</v>
       </c>
       <c r="E26" t="s">
-        <v>194</v>
+        <v>397</v>
       </c>
       <c r="F26" s="5">
-        <v>43231</v>
+        <v>45502</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>306</v>
+        <v>187</v>
       </c>
       <c r="B27" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="C27" t="s">
-        <v>308</v>
+        <v>189</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>309</v>
+        <v>190</v>
       </c>
       <c r="E27" t="s">
-        <v>310</v>
+        <v>191</v>
       </c>
       <c r="F27" s="5">
-        <v>44581</v>
-      </c>
-      <c r="G27" t="s">
-        <v>302</v>
+        <v>43231</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>303</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>304</v>
       </c>
       <c r="C28" t="s">
-        <v>133</v>
+        <v>305</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>134</v>
+        <v>306</v>
       </c>
       <c r="E28" t="s">
-        <v>135</v>
+        <v>307</v>
       </c>
       <c r="F28" s="5">
-        <v>41680</v>
+        <v>44581</v>
+      </c>
+      <c r="G28" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="F29" s="5">
-        <v>40079.444444444445</v>
+        <v>41680</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>324</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>212</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>213</v>
+        <v>11</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>325</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>326</v>
+        <v>13</v>
       </c>
       <c r="F30" s="5">
-        <v>44774</v>
+        <v>40079.444444444445</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>247</v>
+        <v>321</v>
       </c>
       <c r="B31" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="C31" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>249</v>
+        <v>322</v>
       </c>
       <c r="E31" t="s">
-        <v>250</v>
+        <v>323</v>
       </c>
       <c r="F31" s="5">
-        <v>44037</v>
+        <v>44774</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>244</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>245</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>55</v>
+        <v>246</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>247</v>
       </c>
       <c r="F32" s="5">
-        <v>40714.365972222222</v>
+        <v>44037</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>185</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>186</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>188</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>189</v>
+        <v>56</v>
       </c>
       <c r="F33" s="5">
-        <v>43212</v>
+        <v>40714.365972222222</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>315</v>
+        <v>182</v>
       </c>
       <c r="B34" t="s">
-        <v>316</v>
+        <v>183</v>
       </c>
       <c r="C34" t="s">
-        <v>317</v>
+        <v>184</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>329</v>
+        <v>185</v>
       </c>
       <c r="E34" t="s">
-        <v>318</v>
-      </c>
-      <c r="F34" s="7">
-        <v>44676</v>
+        <v>186</v>
+      </c>
+      <c r="F34" s="5">
+        <v>43212</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>235</v>
+        <v>312</v>
       </c>
       <c r="B35" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="C35" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>223</v>
+        <v>325</v>
       </c>
       <c r="E35" t="s">
-        <v>224</v>
-      </c>
-      <c r="F35" s="5">
-        <v>43973</v>
+        <v>315</v>
+      </c>
+      <c r="F35" s="6">
+        <v>44676</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B36" t="s">
-        <v>226</v>
+        <v>300</v>
       </c>
       <c r="C36" t="s">
-        <v>227</v>
+        <v>301</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E36" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="F36" s="5">
-        <v>43616</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>222</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>223</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>224</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>37</v>
+        <v>225</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>226</v>
       </c>
       <c r="F37" s="5">
-        <v>40305.557638888888</v>
+        <v>43616</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>280</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>281</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>283</v>
+        <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>284</v>
+        <v>38</v>
       </c>
       <c r="F38" s="5">
-        <v>44580</v>
+        <v>40305.557638888888</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>277</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>278</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>279</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="E39" t="s">
-        <v>81</v>
+        <v>281</v>
       </c>
       <c r="F39" s="5">
-        <v>40966</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>374</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>202</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>375</v>
+        <v>76</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>376</v>
+        <v>77</v>
       </c>
       <c r="E40" t="s">
-        <v>377</v>
+        <v>78</v>
       </c>
       <c r="F40" s="5">
-        <v>45355</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>378</v>
+        <v>40966</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>319</v>
+        <v>370</v>
       </c>
       <c r="B41" t="s">
-        <v>320</v>
+        <v>199</v>
       </c>
       <c r="C41" t="s">
-        <v>321</v>
+        <v>371</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>322</v>
+        <v>372</v>
       </c>
       <c r="E41" t="s">
-        <v>323</v>
+        <v>373</v>
       </c>
       <c r="F41" s="5">
-        <v>44700</v>
+        <v>45355</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>251</v>
+        <v>316</v>
       </c>
       <c r="B42" t="s">
-        <v>252</v>
+        <v>317</v>
       </c>
       <c r="C42" t="s">
-        <v>253</v>
+        <v>318</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>255</v>
+        <v>319</v>
+      </c>
+      <c r="E42" t="s">
+        <v>320</v>
       </c>
       <c r="F42" s="5">
-        <v>44151</v>
+        <v>44700</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>248</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>249</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>250</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" t="s">
-        <v>86</v>
+        <v>251</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>252</v>
       </c>
       <c r="F43" s="5">
-        <v>41736</v>
+        <v>44151</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>222</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>303</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>304</v>
+        <v>81</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>223</v>
+        <v>82</v>
       </c>
       <c r="E44" t="s">
-        <v>224</v>
+        <v>83</v>
       </c>
       <c r="F44" s="5">
-        <v>43614</v>
+        <v>41736</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>301</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="E45" t="s">
-        <v>4</v>
+        <v>221</v>
       </c>
       <c r="F45" s="5">
-        <v>39932.427083333336</v>
+        <v>43614</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F46" s="5">
-        <v>40094.793055555558</v>
+        <v>39932.427083333336</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="E47" t="s">
-        <v>101</v>
+        <v>23</v>
+      </c>
+      <c r="F47" s="5">
+        <v>40094.793055555558</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>385</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
-        <v>237</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>238</v>
+        <v>96</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>388</v>
+        <v>97</v>
       </c>
       <c r="E48" t="s">
-        <v>386</v>
-      </c>
-      <c r="F48" s="5">
-        <v>45419</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>387</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>381</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="C49" t="s">
-        <v>59</v>
+        <v>235</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>60</v>
+        <v>384</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>382</v>
       </c>
       <c r="F49" s="5">
-        <v>40854.607638888891</v>
+        <v>45419</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>364</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>365</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>366</v>
+        <v>59</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>367</v>
+        <v>60</v>
       </c>
       <c r="E50" t="s">
-        <v>217</v>
+        <v>61</v>
       </c>
       <c r="F50" s="5">
-        <v>45147</v>
-      </c>
-      <c r="G50" t="s">
-        <v>368</v>
+        <v>40854.607638888891</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>218</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>78</v>
+        <v>360</v>
+      </c>
+      <c r="B51" t="s">
+        <v>361</v>
       </c>
       <c r="C51" t="s">
-        <v>220</v>
+        <v>362</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>219</v>
+        <v>363</v>
+      </c>
+      <c r="E51" t="s">
+        <v>214</v>
       </c>
       <c r="F51" s="5">
-        <v>43503</v>
+        <v>45147</v>
+      </c>
+      <c r="G51" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" t="s">
-        <v>63</v>
+        <v>215</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>217</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E52" t="s">
-        <v>66</v>
+        <v>218</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="F52" s="5">
-        <v>41039</v>
+        <v>43503</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>393</v>
       </c>
       <c r="C53" t="s">
-        <v>119</v>
+        <v>394</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>120</v>
+        <v>392</v>
       </c>
       <c r="E53" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="F53" s="5">
-        <v>41900</v>
+        <v>45502</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="E54" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="F54" s="5">
-        <v>40560.762499999997</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>369</v>
+        <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>370</v>
+        <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>371</v>
+        <v>46</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>372</v>
+        <v>47</v>
       </c>
       <c r="E55" t="s">
-        <v>373</v>
+        <v>48</v>
       </c>
       <c r="F55" s="5">
-        <v>45275</v>
+        <v>40560.762499999997</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>211</v>
+        <v>365</v>
       </c>
       <c r="B56" t="s">
-        <v>212</v>
+        <v>366</v>
       </c>
       <c r="C56" t="s">
-        <v>213</v>
+        <v>367</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>214</v>
+        <v>368</v>
       </c>
       <c r="E56" t="s">
-        <v>215</v>
+        <v>369</v>
       </c>
       <c r="F56" s="5">
-        <v>43502</v>
+        <v>45275</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>285</v>
+        <v>208</v>
       </c>
       <c r="B57" t="s">
-        <v>288</v>
+        <v>209</v>
       </c>
       <c r="C57" t="s">
-        <v>289</v>
+        <v>210</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>290</v>
+        <v>211</v>
       </c>
       <c r="E57" t="s">
-        <v>287</v>
+        <v>212</v>
       </c>
       <c r="F57" s="5">
-        <v>44580</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
+        <v>282</v>
+      </c>
+      <c r="B58" t="s">
+        <v>285</v>
+      </c>
+      <c r="C58" t="s">
         <v>286</v>
       </c>
-      <c r="B58" t="s">
-        <v>288</v>
-      </c>
-      <c r="C58" t="s">
-        <v>289</v>
-      </c>
       <c r="D58" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E58" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F58" s="5">
         <v>44580</v>
@@ -2842,462 +2868,462 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>283</v>
       </c>
       <c r="B59" t="s">
-        <v>93</v>
+        <v>285</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
+        <v>286</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>95</v>
+        <v>287</v>
       </c>
       <c r="E59" t="s">
-        <v>96</v>
+        <v>284</v>
       </c>
       <c r="F59" s="5">
-        <v>41780</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>165</v>
+        <v>90</v>
       </c>
       <c r="C60" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>167</v>
+        <v>92</v>
       </c>
       <c r="E60" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="F60" s="5">
-        <v>42530</v>
+        <v>41780</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>216</v>
+        <v>161</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="C61" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="E61" t="s">
-        <v>217</v>
+        <v>165</v>
       </c>
       <c r="F61" s="5">
-        <v>43502</v>
+        <v>42530</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>29</v>
+        <v>213</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="C62" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="E62" t="s">
-        <v>33</v>
+        <v>214</v>
       </c>
       <c r="F62" s="5">
-        <v>40164.4375</v>
+        <v>43502</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C63" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="E63" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="F63" s="5">
-        <v>41854</v>
+        <v>40164.4375</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
+        <v>99</v>
+      </c>
+      <c r="B64" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E64" t="s">
+        <v>103</v>
+      </c>
+      <c r="F64" s="5">
+        <v>41854</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>198</v>
+      </c>
+      <c r="B65" t="s">
+        <v>199</v>
+      </c>
+      <c r="C65" t="s">
+        <v>200</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B64" t="s">
+      <c r="E65" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C64" t="s">
-        <v>203</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="F64" s="7">
+      <c r="F65" s="6">
         <v>37415</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A65" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="B65" s="8" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A66" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E66" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="F65" s="5">
+      <c r="F66" s="5">
         <v>43997</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>256</v>
-      </c>
-      <c r="B66" t="s">
-        <v>257</v>
-      </c>
-      <c r="C66" t="s">
-        <v>258</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="F66" s="5">
-        <v>44166</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>107</v>
+        <v>253</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>254</v>
       </c>
       <c r="C67" t="s">
-        <v>109</v>
+        <v>255</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E67" t="s">
-        <v>111</v>
+        <v>256</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="F67" s="5">
-        <v>41857</v>
+        <v>44166</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="B68" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="C68" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="E68" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="F68" s="5">
-        <v>42467</v>
+        <v>41857</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C69" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="E69" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="F69" s="5">
-        <v>42420</v>
+        <v>42467</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="B70" t="s">
-        <v>231</v>
+        <v>134</v>
       </c>
       <c r="C70" t="s">
-        <v>232</v>
+        <v>135</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>233</v>
+        <v>136</v>
       </c>
       <c r="E70" t="s">
-        <v>234</v>
+        <v>137</v>
       </c>
       <c r="F70" s="5">
-        <v>43973</v>
+        <v>42420</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>227</v>
       </c>
       <c r="B71" t="s">
-        <v>15</v>
+        <v>228</v>
       </c>
       <c r="C71" t="s">
-        <v>16</v>
+        <v>229</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>17</v>
+        <v>230</v>
       </c>
       <c r="E71" t="s">
-        <v>18</v>
+        <v>231</v>
       </c>
       <c r="F71" s="5">
-        <v>40081.550694444442</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="C72" t="s">
-        <v>152</v>
+        <v>16</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>153</v>
+        <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>154</v>
+        <v>18</v>
       </c>
       <c r="F72" s="5">
-        <v>42472</v>
+        <v>40081.550694444442</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
       <c r="E73" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="F73" s="5">
-        <v>43054</v>
+        <v>42472</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>178</v>
       </c>
       <c r="B74" t="s">
-        <v>303</v>
+        <v>30</v>
       </c>
       <c r="C74" t="s">
-        <v>304</v>
+        <v>179</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="E74" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="F74" s="5">
-        <v>43973</v>
+        <v>43054</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="B75" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C75" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>293</v>
+        <v>220</v>
       </c>
       <c r="E75" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="F75" s="5">
-        <v>44580</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>175</v>
+        <v>288</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>291</v>
       </c>
       <c r="C76" t="s">
-        <v>177</v>
+        <v>292</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>178</v>
+        <v>290</v>
       </c>
       <c r="E76" t="s">
-        <v>179</v>
+        <v>289</v>
       </c>
       <c r="F76" s="5">
-        <v>42739</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>379</v>
+        <v>172</v>
       </c>
       <c r="B77" t="s">
-        <v>380</v>
+        <v>173</v>
       </c>
       <c r="C77" t="s">
-        <v>381</v>
+        <v>174</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="E77" t="s">
-        <v>383</v>
+        <v>176</v>
       </c>
       <c r="F77" s="5">
-        <v>45358</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>384</v>
+        <v>42739</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>39</v>
+        <v>375</v>
       </c>
       <c r="B78" t="s">
-        <v>40</v>
+        <v>376</v>
       </c>
       <c r="C78" t="s">
-        <v>41</v>
+        <v>377</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>42</v>
+        <v>378</v>
       </c>
       <c r="E78" t="s">
-        <v>43</v>
+        <v>379</v>
       </c>
       <c r="F78" s="5">
-        <v>40522.519444444442</v>
+        <v>45358</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="C79" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="E79" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="F79" s="5">
-        <v>41890</v>
+        <v>40522.519444444442</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="C80" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="E80" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="F80" s="5">
-        <v>42852</v>
+        <v>41890</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>180</v>
+        <v>64</v>
       </c>
       <c r="B81" t="s">
+        <v>65</v>
+      </c>
+      <c r="C81" t="s">
+        <v>66</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E81" t="s">
         <v>68</v>
-      </c>
-      <c r="C81" t="s">
-        <v>69</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E81" t="s">
-        <v>71</v>
       </c>
       <c r="F81" s="5">
         <v>42852</v>
@@ -3305,81 +3331,101 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="B82" t="s">
-        <v>207</v>
+        <v>65</v>
       </c>
       <c r="C82" t="s">
-        <v>208</v>
+        <v>66</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="F82" s="7">
-        <v>43487</v>
+        <v>67</v>
+      </c>
+      <c r="E82" t="s">
+        <v>68</v>
+      </c>
+      <c r="F82" s="5">
+        <v>42852</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
       <c r="B83" t="s">
-        <v>160</v>
+        <v>204</v>
       </c>
       <c r="C83" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E83" t="s">
-        <v>163</v>
-      </c>
-      <c r="F83" s="5">
-        <v>42505</v>
+        <v>206</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F83" s="6">
+        <v>43487</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>333</v>
+        <v>156</v>
       </c>
       <c r="B84" t="s">
-        <v>334</v>
+        <v>157</v>
       </c>
       <c r="C84" t="s">
-        <v>335</v>
+        <v>158</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>336</v>
+        <v>159</v>
       </c>
       <c r="E84" t="s">
-        <v>337</v>
+        <v>160</v>
       </c>
       <c r="F84" s="5">
-        <v>44775</v>
+        <v>42505</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
+        <v>329</v>
+      </c>
+      <c r="B85" t="s">
+        <v>330</v>
+      </c>
+      <c r="C85" t="s">
+        <v>331</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E85" t="s">
+        <v>333</v>
+      </c>
+      <c r="F85" s="5">
+        <v>44775</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>138</v>
+      </c>
+      <c r="B86" t="s">
+        <v>139</v>
+      </c>
+      <c r="C86" t="s">
+        <v>140</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B85" t="s">
+      <c r="E86" t="s">
         <v>142</v>
       </c>
-      <c r="C85" t="s">
-        <v>143</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E85" t="s">
-        <v>145</v>
-      </c>
-      <c r="F85" s="5">
+      <c r="F86" s="5">
         <v>42439</v>
       </c>
     </row>
@@ -3390,97 +3436,101 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D56" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
-    <hyperlink ref="D61" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
-    <hyperlink ref="D51" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
-    <hyperlink ref="D44" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
-    <hyperlink ref="D36" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
-    <hyperlink ref="D70" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
-    <hyperlink ref="D35" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
-    <hyperlink ref="D74" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
+    <hyperlink ref="D57" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D62" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
+    <hyperlink ref="D52" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D45" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D37" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
+    <hyperlink ref="D71" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
+    <hyperlink ref="D36" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
+    <hyperlink ref="D75" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
     <hyperlink ref="D11" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
     <hyperlink ref="D9" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
     <hyperlink ref="D3" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
     <hyperlink ref="D23" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
-    <hyperlink ref="D66" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
-    <hyperlink ref="D42" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
-    <hyperlink ref="D31" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
-    <hyperlink ref="D65" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
-    <hyperlink ref="D82" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
-    <hyperlink ref="D64" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
-    <hyperlink ref="D26" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
-    <hyperlink ref="D33" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
-    <hyperlink ref="D73" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
-    <hyperlink ref="D81" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
-    <hyperlink ref="D76" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
+    <hyperlink ref="D67" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
+    <hyperlink ref="D43" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
+    <hyperlink ref="D32" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
+    <hyperlink ref="D66" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
+    <hyperlink ref="D83" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
+    <hyperlink ref="D65" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
+    <hyperlink ref="D27" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
+    <hyperlink ref="D34" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
+    <hyperlink ref="D74" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
+    <hyperlink ref="D82" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
+    <hyperlink ref="D77" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
     <hyperlink ref="D16" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
     <hyperlink ref="D15" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
-    <hyperlink ref="D60" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
-    <hyperlink ref="D83" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
-    <hyperlink ref="D45" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
-    <hyperlink ref="D29" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
-    <hyperlink ref="D71" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
-    <hyperlink ref="D46" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
+    <hyperlink ref="D61" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
+    <hyperlink ref="D84" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
+    <hyperlink ref="D46" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
+    <hyperlink ref="D30" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
+    <hyperlink ref="D72" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
+    <hyperlink ref="D47" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
     <hyperlink ref="D20" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
-    <hyperlink ref="D62" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
-    <hyperlink ref="D37" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
-    <hyperlink ref="D78" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
-    <hyperlink ref="D54" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
+    <hyperlink ref="D63" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
+    <hyperlink ref="D38" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
+    <hyperlink ref="D79" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
+    <hyperlink ref="D55" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
     <hyperlink ref="D7" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
-    <hyperlink ref="D32" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
-    <hyperlink ref="D49" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
-    <hyperlink ref="D52" r:id="rId40" xr:uid="{3543B8E5-2462-4903-BF7C-D94033E8C10C}"/>
-    <hyperlink ref="D80" r:id="rId41" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
-    <hyperlink ref="D12" r:id="rId42" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
-    <hyperlink ref="D39" r:id="rId43" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
-    <hyperlink ref="D43" r:id="rId44" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
-    <hyperlink ref="D14" r:id="rId45" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
-    <hyperlink ref="D59" r:id="rId46" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
-    <hyperlink ref="D47" r:id="rId47" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
-    <hyperlink ref="D63" r:id="rId48" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
-    <hyperlink ref="D67" r:id="rId49" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
-    <hyperlink ref="D79" r:id="rId50" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
-    <hyperlink ref="D53" r:id="rId51" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
-    <hyperlink ref="D24" r:id="rId52" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
-    <hyperlink ref="D4" r:id="rId53" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
-    <hyperlink ref="D28" r:id="rId54" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
-    <hyperlink ref="D69" r:id="rId55" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D85" r:id="rId56" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
-    <hyperlink ref="D68" r:id="rId57" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
-    <hyperlink ref="D72" r:id="rId58" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
-    <hyperlink ref="D8" r:id="rId59" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
-    <hyperlink ref="D21" r:id="rId60" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
-    <hyperlink ref="D38" r:id="rId61" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
-    <hyperlink ref="D57" r:id="rId62" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
-    <hyperlink ref="D58" r:id="rId63" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
-    <hyperlink ref="D75" r:id="rId64" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
-    <hyperlink ref="D25" r:id="rId65" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
-    <hyperlink ref="D27" r:id="rId66" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
-    <hyperlink ref="D41" r:id="rId67" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
-    <hyperlink ref="D30" r:id="rId68" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
-    <hyperlink ref="D18" r:id="rId69" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
-    <hyperlink ref="D34" r:id="rId70" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
-    <hyperlink ref="D2" r:id="rId71" display="mailto:frank.vyncke@yin4yang.com" xr:uid="{E29600CB-349C-4C55-AC29-3B61912C4757}"/>
-    <hyperlink ref="D84" r:id="rId72" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
-    <hyperlink ref="D22" r:id="rId73" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
-    <hyperlink ref="D5" r:id="rId74" xr:uid="{33D12C26-CC5E-4925-86B6-4AE855A6371F}"/>
-    <hyperlink ref="G5" r:id="rId75" xr:uid="{2FA39695-7884-42EC-9380-C8EFD7B7EAD9}"/>
-    <hyperlink ref="D13" r:id="rId76" xr:uid="{B237CB2B-4475-8C4E-A2C5-5839FB07318E}"/>
-    <hyperlink ref="D6" r:id="rId77" xr:uid="{3C6DADFB-91D3-4B16-BA60-22286260FB72}"/>
-    <hyperlink ref="G6" r:id="rId78" xr:uid="{EF6627CA-3B1A-440B-85D4-A1B7067549BD}"/>
-    <hyperlink ref="D10" r:id="rId79" xr:uid="{058D1BE7-4CFF-4740-BC92-2074C717A677}"/>
-    <hyperlink ref="G10" r:id="rId80" xr:uid="{B9062A46-48F6-45FB-8197-4FD986CC482D}"/>
-    <hyperlink ref="D50" r:id="rId81" xr:uid="{0CFEC845-7F90-4802-9D24-4AC8905CD11B}"/>
-    <hyperlink ref="D55" r:id="rId82" xr:uid="{81B44739-2F1A-4DDB-90E8-2523712052F0}"/>
-    <hyperlink ref="D40" r:id="rId83" xr:uid="{72B2BA10-0B55-4ACF-9CC1-DA30FB4C2741}"/>
-    <hyperlink ref="G40" r:id="rId84" xr:uid="{1106BFBB-F6F3-4E8A-8B65-06381130271C}"/>
-    <hyperlink ref="D77" r:id="rId85" xr:uid="{249742DB-9523-4D5C-B3FC-194F7D7BB889}"/>
-    <hyperlink ref="G77" r:id="rId86" xr:uid="{BD0ABADB-115E-43D9-8791-2BFF7CAEC355}"/>
-    <hyperlink ref="G48" r:id="rId87" xr:uid="{44657DD4-3FFA-4E6F-8898-631518A1BFDC}"/>
-    <hyperlink ref="D48" r:id="rId88" xr:uid="{D5A339A1-161D-40E3-9F69-B4599246184B}"/>
-    <hyperlink ref="G19" r:id="rId89" xr:uid="{C64F139E-8286-4E7A-8B5E-9D69FC9A0C25}"/>
+    <hyperlink ref="D33" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
+    <hyperlink ref="D50" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
+    <hyperlink ref="D81" r:id="rId40" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
+    <hyperlink ref="D12" r:id="rId41" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
+    <hyperlink ref="D40" r:id="rId42" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
+    <hyperlink ref="D44" r:id="rId43" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
+    <hyperlink ref="D14" r:id="rId44" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
+    <hyperlink ref="D60" r:id="rId45" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
+    <hyperlink ref="D48" r:id="rId46" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
+    <hyperlink ref="D64" r:id="rId47" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
+    <hyperlink ref="D68" r:id="rId48" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
+    <hyperlink ref="D80" r:id="rId49" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
+    <hyperlink ref="D54" r:id="rId50" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
+    <hyperlink ref="D24" r:id="rId51" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
+    <hyperlink ref="D4" r:id="rId52" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
+    <hyperlink ref="D29" r:id="rId53" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
+    <hyperlink ref="D70" r:id="rId54" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
+    <hyperlink ref="D86" r:id="rId55" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D69" r:id="rId56" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
+    <hyperlink ref="D73" r:id="rId57" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
+    <hyperlink ref="D8" r:id="rId58" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
+    <hyperlink ref="D21" r:id="rId59" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
+    <hyperlink ref="D39" r:id="rId60" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
+    <hyperlink ref="D58" r:id="rId61" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
+    <hyperlink ref="D59" r:id="rId62" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
+    <hyperlink ref="D76" r:id="rId63" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
+    <hyperlink ref="D25" r:id="rId64" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D28" r:id="rId65" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
+    <hyperlink ref="D42" r:id="rId66" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
+    <hyperlink ref="D31" r:id="rId67" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
+    <hyperlink ref="D18" r:id="rId68" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
+    <hyperlink ref="D35" r:id="rId69" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
+    <hyperlink ref="D2" r:id="rId70" display="mailto:frank.vyncke@yin4yang.com" xr:uid="{E29600CB-349C-4C55-AC29-3B61912C4757}"/>
+    <hyperlink ref="D85" r:id="rId71" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
+    <hyperlink ref="D22" r:id="rId72" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
+    <hyperlink ref="D5" r:id="rId73" xr:uid="{33D12C26-CC5E-4925-86B6-4AE855A6371F}"/>
+    <hyperlink ref="G5" r:id="rId74" xr:uid="{2FA39695-7884-42EC-9380-C8EFD7B7EAD9}"/>
+    <hyperlink ref="D13" r:id="rId75" xr:uid="{B237CB2B-4475-8C4E-A2C5-5839FB07318E}"/>
+    <hyperlink ref="D6" r:id="rId76" xr:uid="{3C6DADFB-91D3-4B16-BA60-22286260FB72}"/>
+    <hyperlink ref="G6" r:id="rId77" xr:uid="{EF6627CA-3B1A-440B-85D4-A1B7067549BD}"/>
+    <hyperlink ref="D10" r:id="rId78" xr:uid="{058D1BE7-4CFF-4740-BC92-2074C717A677}"/>
+    <hyperlink ref="G10" r:id="rId79" xr:uid="{B9062A46-48F6-45FB-8197-4FD986CC482D}"/>
+    <hyperlink ref="D51" r:id="rId80" xr:uid="{0CFEC845-7F90-4802-9D24-4AC8905CD11B}"/>
+    <hyperlink ref="D56" r:id="rId81" xr:uid="{81B44739-2F1A-4DDB-90E8-2523712052F0}"/>
+    <hyperlink ref="D41" r:id="rId82" xr:uid="{72B2BA10-0B55-4ACF-9CC1-DA30FB4C2741}"/>
+    <hyperlink ref="G41" r:id="rId83" xr:uid="{1106BFBB-F6F3-4E8A-8B65-06381130271C}"/>
+    <hyperlink ref="D78" r:id="rId84" xr:uid="{249742DB-9523-4D5C-B3FC-194F7D7BB889}"/>
+    <hyperlink ref="G78" r:id="rId85" xr:uid="{BD0ABADB-115E-43D9-8791-2BFF7CAEC355}"/>
+    <hyperlink ref="G49" r:id="rId86" xr:uid="{44657DD4-3FFA-4E6F-8898-631518A1BFDC}"/>
+    <hyperlink ref="D49" r:id="rId87" xr:uid="{D5A339A1-161D-40E3-9F69-B4599246184B}"/>
+    <hyperlink ref="G19" r:id="rId88" xr:uid="{C64F139E-8286-4E7A-8B5E-9D69FC9A0C25}"/>
+    <hyperlink ref="G53" r:id="rId89" xr:uid="{5D505EE9-2263-469C-9455-D353F4C9921E}"/>
+    <hyperlink ref="D53" r:id="rId90" xr:uid="{5715AC7F-4208-4141-884D-FD2EB9CB5E95}"/>
+    <hyperlink ref="D17" r:id="rId91" xr:uid="{50E71DF8-A245-41B4-83A8-E6488454D9A4}"/>
+    <hyperlink ref="G26" r:id="rId92" xr:uid="{15520162-C027-42E1-8EC1-CA7EA9FD18BC}"/>
+    <hyperlink ref="D26" r:id="rId93" xr:uid="{E9A12839-D069-4292-A5EA-36394565B8A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId90"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId94"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolve #47 and #48
</commit_message>
<xml_diff>
--- a/ISO PDF Registry.xlsx
+++ b/ISO PDF Registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\share\pdf-names-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D0858B-6342-4FA2-B685-980DE60164DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7023F607-D2F6-4F0C-8A2D-7E3C8EA1F5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26510" yWindow="1780" windowWidth="23910" windowHeight="17960" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="29016" windowHeight="18696" xr2:uid="{9E3ABFD2-C7ED-CB44-90E8-944996B24765}"/>
   </bookViews>
   <sheets>
     <sheet name="PDF Prefix Registry" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="428">
   <si>
     <t>ITXT</t>
   </si>
@@ -1281,6 +1281,39 @@
   </si>
   <si>
     <t>https://github.com/adobe/pdf-names-list/issues/46</t>
+  </si>
+  <si>
+    <t>AOCR</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Falk</t>
+  </si>
+  <si>
+    <t>al@us.altova.com</t>
+  </si>
+  <si>
+    <t>Altova GmbH</t>
+  </si>
+  <si>
+    <t>https://github.com/adobe/pdf-names-list/issues/47</t>
+  </si>
+  <si>
+    <t>PHNK</t>
+  </si>
+  <si>
+    <t>Matthias</t>
+  </si>
+  <si>
+    <t>Valvekens</t>
+  </si>
+  <si>
+    <t>dev@mvalvekens.be</t>
+  </si>
+  <si>
+    <t>https://github.com/adobe/pdf-names-list/issues/48</t>
   </si>
 </sst>
 </file>
@@ -1694,25 +1727,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E74889-C943-2949-BDAA-069F646F779D}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.35546875" customWidth="1"/>
-    <col min="2" max="2" width="16.640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.3984375" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="83.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>192</v>
       </c>
@@ -1735,7 +1768,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>326</v>
       </c>
@@ -1758,7 +1791,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>263</v>
       </c>
@@ -1778,7 +1811,7 @@
         <v>44221</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -1798,7 +1831,7 @@
         <v>41931</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>339</v>
       </c>
@@ -1821,7 +1854,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>351</v>
       </c>
@@ -1844,7 +1877,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1864,172 +1897,175 @@
         <v>40664.775694444441</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>417</v>
+      </c>
+      <c r="B8" t="s">
+        <v>418</v>
+      </c>
+      <c r="C8" t="s">
+        <v>419</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E8" t="s">
+        <v>421</v>
+      </c>
+      <c r="F8" s="5">
+        <v>45803</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>152</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>153</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>155</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F9" s="5">
         <v>42492</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>268</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>269</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>270</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F10" s="5">
         <v>44280</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>357</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>352</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>353</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F11" s="5">
         <v>45147</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>239</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>240</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>241</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>243</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F12" s="5">
         <v>43997</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>69</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>70</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F13" s="5">
         <v>40997</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>345</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>346</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>347</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>349</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F14" s="5">
         <v>45142</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>84</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>85</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F15" s="5">
         <v>41758</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>166</v>
-      </c>
-      <c r="B15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E15" t="s">
-        <v>170</v>
-      </c>
-      <c r="F15" s="5">
-        <v>42739</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>171</v>
       </c>
       <c r="B16" t="s">
         <v>167</v>
@@ -2047,919 +2083,919 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="31.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17" s="5">
+        <v>42739</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F18" s="5">
         <v>40060.538888888892</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>308</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>309</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>310</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>311</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F19" s="6">
         <v>44676</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>385</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>386</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>387</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>389</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F20" s="6">
         <v>45484</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F21" s="5">
         <v>40105.464583333334</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>411</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>412</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>413</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>415</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F22" s="5">
         <v>45749</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>273</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>75</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>274</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>276</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F23" s="5">
         <v>44580</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>334</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>335</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>336</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>338</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F24" s="5">
         <v>44915</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>258</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>259</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>260</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F25" s="5">
         <v>44174</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>119</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>120</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>121</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>302</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F26" s="5">
         <v>41924</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>293</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>296</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>297</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>294</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F27" s="5">
         <v>44580</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>396</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>399</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>400</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>397</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F28" s="5">
         <v>45502</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>187</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>188</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>189</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>191</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F29" s="5">
         <v>43231</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>303</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>304</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>305</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>307</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F30" s="5">
         <v>44581</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>128</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>129</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>132</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F31" s="5">
         <v>41680</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>9</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>10</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F32" s="5">
         <v>40079.444444444445</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>321</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>209</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>210</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>323</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F33" s="5">
         <v>44774</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>244</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>173</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>245</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>247</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F34" s="5">
         <v>44037</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>53</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>54</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F35" s="5">
         <v>40714.365972222222</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>182</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>183</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>184</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>186</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F36" s="5">
         <v>43212</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>312</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>313</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>314</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>315</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F37" s="6">
         <v>44676</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>232</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>300</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>301</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>221</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F38" s="5">
         <v>43973</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>222</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>223</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>224</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F39" s="5">
         <v>43616</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>34</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>35</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F40" s="5">
         <v>40305.557638888888</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>277</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>278</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>279</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>281</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F41" s="5">
         <v>44580</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>402</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>403</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>404</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>406</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F42" s="5">
         <v>45673</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>74</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>75</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
         <v>78</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F43" s="5">
         <v>40966</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>370</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>199</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>371</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>373</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F44" s="5">
         <v>45355</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>316</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>317</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>318</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>320</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F45" s="5">
         <v>44700</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>248</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>249</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>250</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F46" s="5">
         <v>44151</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>79</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>80</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>83</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F47" s="5">
         <v>41736</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>219</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>300</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>301</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>221</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F48" s="5">
         <v>43614</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>0</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>1</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>2</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F49" s="5">
         <v>39932.427083333336</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>19</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>20</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>23</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F50" s="5">
         <v>40094.793055555558</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>94</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>95</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>381</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>234</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>235</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>382</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F52" s="5">
         <v>45419</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>57</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>58</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>59</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>61</v>
       </c>
-      <c r="F52" s="5">
+      <c r="F53" s="5">
         <v>40854.607638888891</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>360</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>361</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>362</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>214</v>
       </c>
-      <c r="F53" s="5">
+      <c r="F54" s="5">
         <v>45147</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>215</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>217</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F54" s="5">
+      <c r="F55" s="5">
         <v>43503</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>62</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>393</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>394</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>63</v>
       </c>
-      <c r="F55" s="5">
+      <c r="F56" s="5">
         <v>45502</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>114</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>115</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>116</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>118</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F57" s="5">
         <v>41900</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>44</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>45</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>46</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E58" t="s">
         <v>48</v>
       </c>
-      <c r="F57" s="5">
+      <c r="F58" s="5">
         <v>40560.762499999997</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>365</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>366</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>367</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
         <v>369</v>
       </c>
-      <c r="F58" s="5">
+      <c r="F59" s="5">
         <v>45275</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>208</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>209</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>210</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
         <v>212</v>
       </c>
-      <c r="F59" s="5">
+      <c r="F60" s="5">
         <v>43502</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>282</v>
-      </c>
-      <c r="B60" t="s">
-        <v>285</v>
-      </c>
-      <c r="C60" t="s">
-        <v>286</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E60" t="s">
-        <v>284</v>
-      </c>
-      <c r="F60" s="5">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>283</v>
       </c>
       <c r="B61" t="s">
         <v>285</v>
@@ -2977,589 +3013,629 @@
         <v>44580</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>283</v>
+      </c>
+      <c r="B62" t="s">
+        <v>285</v>
+      </c>
+      <c r="C62" t="s">
+        <v>286</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E62" t="s">
+        <v>284</v>
+      </c>
+      <c r="F62" s="5">
+        <v>44580</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>408</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>361</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>362</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" t="s">
         <v>214</v>
       </c>
-      <c r="F62" s="5">
+      <c r="F63" s="5">
         <v>45695</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>89</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>90</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>91</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" t="s">
         <v>93</v>
       </c>
-      <c r="F63" s="5">
+      <c r="F64" s="5">
         <v>41780</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>161</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>162</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>163</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" t="s">
         <v>165</v>
       </c>
-      <c r="F64" s="5">
+      <c r="F65" s="5">
         <v>42530</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>213</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>120</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>121</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" t="s">
         <v>214</v>
       </c>
-      <c r="F65" s="5">
+      <c r="F66" s="5">
         <v>43502</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>29</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>30</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>31</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E67" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="5">
+      <c r="F67" s="5">
         <v>40164.4375</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>423</v>
+      </c>
+      <c r="B68" t="s">
+        <v>424</v>
+      </c>
+      <c r="C68" t="s">
+        <v>425</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="F68" s="5">
+        <v>45803</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>99</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B69" t="s">
         <v>100</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C69" t="s">
         <v>101</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E69" t="s">
         <v>103</v>
       </c>
-      <c r="F67" s="5">
+      <c r="F69" s="5">
         <v>41854</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>198</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" t="s">
         <v>199</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C70" t="s">
         <v>200</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E70" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="F68" s="6">
+      <c r="F70" s="6">
         <v>37415</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A69" s="7" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C71" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E71" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="F69" s="5">
+      <c r="F71" s="5">
         <v>43997</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>253</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B72" t="s">
         <v>254</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C72" t="s">
         <v>255</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="F70" s="5">
+      <c r="F72" s="5">
         <v>44166</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>104</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B73" t="s">
         <v>105</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>106</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E73" t="s">
         <v>108</v>
       </c>
-      <c r="F71" s="5">
+      <c r="F73" s="5">
         <v>41857</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>143</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B74" t="s">
         <v>144</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C74" t="s">
         <v>145</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E74" t="s">
         <v>147</v>
       </c>
-      <c r="F72" s="5">
+      <c r="F74" s="5">
         <v>42467</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>133</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B75" t="s">
         <v>134</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C75" t="s">
         <v>135</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E75" t="s">
         <v>137</v>
       </c>
-      <c r="F73" s="5">
+      <c r="F75" s="5">
         <v>42420</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>227</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B76" t="s">
         <v>228</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C76" t="s">
         <v>229</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E76" t="s">
         <v>231</v>
       </c>
-      <c r="F74" s="5">
+      <c r="F76" s="5">
         <v>43973</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>14</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B77" t="s">
         <v>15</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>16</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E77" t="s">
         <v>18</v>
       </c>
-      <c r="F75" s="5">
+      <c r="F77" s="5">
         <v>40081.550694444442</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>148</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B78" t="s">
         <v>70</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C78" t="s">
         <v>149</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E78" t="s">
         <v>151</v>
       </c>
-      <c r="F76" s="5">
+      <c r="F78" s="5">
         <v>42472</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>178</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B79" t="s">
         <v>30</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C79" t="s">
         <v>179</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E79" t="s">
         <v>181</v>
       </c>
-      <c r="F77" s="5">
+      <c r="F79" s="5">
         <v>43054</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>233</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B80" t="s">
         <v>300</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C80" t="s">
         <v>301</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E80" t="s">
         <v>221</v>
       </c>
-      <c r="F78" s="5">
+      <c r="F80" s="5">
         <v>43973</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>288</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B81" t="s">
         <v>291</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C81" t="s">
         <v>292</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E81" t="s">
         <v>289</v>
       </c>
-      <c r="F79" s="5">
+      <c r="F81" s="5">
         <v>44580</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>172</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
         <v>173</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C82" t="s">
         <v>174</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E82" t="s">
         <v>176</v>
       </c>
-      <c r="F80" s="5">
+      <c r="F82" s="5">
         <v>42739</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>375</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B83" t="s">
         <v>376</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>377</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E83" t="s">
         <v>379</v>
       </c>
-      <c r="F81" s="5">
+      <c r="F83" s="5">
         <v>45358</v>
       </c>
-      <c r="G81" s="1" t="s">
+      <c r="G83" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>39</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B84" t="s">
         <v>40</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C84" t="s">
         <v>41</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E84" t="s">
         <v>43</v>
       </c>
-      <c r="F82" s="5">
+      <c r="F84" s="5">
         <v>40522.519444444442</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>109</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B85" t="s">
         <v>110</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C85" t="s">
         <v>111</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E85" t="s">
         <v>113</v>
       </c>
-      <c r="F83" s="5">
+      <c r="F85" s="5">
         <v>41890</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>64</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B86" t="s">
         <v>65</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C86" t="s">
         <v>66</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E86" t="s">
         <v>68</v>
       </c>
-      <c r="F84" s="5">
+      <c r="F86" s="5">
         <v>42852</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>177</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>65</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C87" t="s">
         <v>66</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E87" t="s">
         <v>68</v>
       </c>
-      <c r="F85" s="5">
+      <c r="F87" s="5">
         <v>42852</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>203</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B88" t="s">
         <v>204</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C88" t="s">
         <v>205</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E86" s="5" t="s">
+      <c r="E88" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="F86" s="6">
+      <c r="F88" s="6">
         <v>43487</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>156</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>157</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C89" t="s">
         <v>158</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E89" t="s">
         <v>160</v>
       </c>
-      <c r="F87" s="5">
+      <c r="F89" s="5">
         <v>42505</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>409</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B90" t="s">
         <v>361</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
         <v>362</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E90" t="s">
         <v>214</v>
       </c>
-      <c r="F88" s="5">
+      <c r="F90" s="5">
         <v>45695</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G90" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>329</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B91" t="s">
         <v>330</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C91" t="s">
         <v>331</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E91" t="s">
         <v>333</v>
       </c>
-      <c r="F89" s="5">
+      <c r="F91" s="5">
         <v>44775</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A90" t="s">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>138</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B92" t="s">
         <v>139</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C92" t="s">
         <v>140</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E92" t="s">
         <v>142</v>
       </c>
-      <c r="F90" s="5">
+      <c r="F92" s="5">
         <v>42439</v>
       </c>
     </row>
@@ -3570,107 +3646,111 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D59" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
-    <hyperlink ref="D65" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
-    <hyperlink ref="D54" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
-    <hyperlink ref="D47" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
-    <hyperlink ref="D38" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
-    <hyperlink ref="D74" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
-    <hyperlink ref="D37" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
-    <hyperlink ref="D78" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
-    <hyperlink ref="D9" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
+    <hyperlink ref="D60" r:id="rId1" xr:uid="{407FC650-7151-6940-B8FA-60477C7D30B1}"/>
+    <hyperlink ref="D66" r:id="rId2" xr:uid="{68E4476D-88C7-5D40-9274-7B03AB299562}"/>
+    <hyperlink ref="D55" r:id="rId3" display="mailto:klink@csi.com" xr:uid="{85C07C9E-BB28-4C49-84D2-B3052E15F688}"/>
+    <hyperlink ref="D48" r:id="rId4" xr:uid="{234AD513-3ABE-F545-A037-27824EABDF68}"/>
+    <hyperlink ref="D39" r:id="rId5" xr:uid="{7924D455-5B5F-E641-AB7C-FB4BD03EF051}"/>
+    <hyperlink ref="D76" r:id="rId6" display="mailto:normand.williams@onespan.com" xr:uid="{C8F08AEB-A945-364E-84E9-3EFCB37949EA}"/>
+    <hyperlink ref="D38" r:id="rId7" xr:uid="{7AEF03BC-D893-FF42-BB52-AB9C9480EA0D}"/>
+    <hyperlink ref="D80" r:id="rId8" xr:uid="{1E7EE29B-6F34-AF43-9A6A-A4BA495EE964}"/>
+    <hyperlink ref="D12" r:id="rId9" xr:uid="{D57F2423-845A-9E44-A60D-DEEB1150BE7A}"/>
+    <hyperlink ref="D10" r:id="rId10" xr:uid="{0133BED0-2D2B-4A0F-AB7C-D58D8B5F381B}"/>
     <hyperlink ref="D3" r:id="rId11" xr:uid="{5F0875F3-1434-4B08-A87A-2BDF5EEDDAC9}"/>
-    <hyperlink ref="D24" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
-    <hyperlink ref="D70" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
-    <hyperlink ref="D45" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
-    <hyperlink ref="D33" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
-    <hyperlink ref="D69" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
-    <hyperlink ref="D86" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
-    <hyperlink ref="D68" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
-    <hyperlink ref="D28" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
-    <hyperlink ref="D35" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
-    <hyperlink ref="D77" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
-    <hyperlink ref="D85" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
-    <hyperlink ref="D80" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
-    <hyperlink ref="D16" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
-    <hyperlink ref="D15" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
-    <hyperlink ref="D64" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
-    <hyperlink ref="D87" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
-    <hyperlink ref="D48" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
-    <hyperlink ref="D31" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
-    <hyperlink ref="D75" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
-    <hyperlink ref="D49" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
-    <hyperlink ref="D20" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
-    <hyperlink ref="D66" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
-    <hyperlink ref="D39" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
-    <hyperlink ref="D82" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
-    <hyperlink ref="D57" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
+    <hyperlink ref="D25" r:id="rId12" xr:uid="{61482C13-D6B2-4AFF-AD10-908ABE8BA3F2}"/>
+    <hyperlink ref="D72" r:id="rId13" xr:uid="{8AA40E15-5F88-4955-98D8-3EDB9CE3C08B}"/>
+    <hyperlink ref="D46" r:id="rId14" xr:uid="{FEB07F00-70C8-4D84-B7DF-B36DF7C6138C}"/>
+    <hyperlink ref="D34" r:id="rId15" xr:uid="{9236AFAC-B489-4804-B65A-1988399CC4C2}"/>
+    <hyperlink ref="D71" r:id="rId16" xr:uid="{50BFEC84-47AF-4D28-B04F-52D949215BCB}"/>
+    <hyperlink ref="D88" r:id="rId17" xr:uid="{29C24CB5-B24B-4772-A291-FC2CDC7AB656}"/>
+    <hyperlink ref="D70" r:id="rId18" xr:uid="{6A8074F9-38E6-46D2-BC30-EDB597684655}"/>
+    <hyperlink ref="D29" r:id="rId19" xr:uid="{178F076F-6CAC-44EB-AA97-31037608AA41}"/>
+    <hyperlink ref="D36" r:id="rId20" xr:uid="{E467E97B-65A6-40E0-A2BA-7875E3A5C2C1}"/>
+    <hyperlink ref="D79" r:id="rId21" xr:uid="{6177B640-2E3A-4478-8CB7-5ED41AA4BC0A}"/>
+    <hyperlink ref="D87" r:id="rId22" xr:uid="{51676D7C-EE2B-463D-8301-98CF22D9B71E}"/>
+    <hyperlink ref="D82" r:id="rId23" xr:uid="{DB05FA17-E2C3-49C9-8F48-C3395EC9FB65}"/>
+    <hyperlink ref="D17" r:id="rId24" xr:uid="{8C069B77-F7A2-4DC6-9D5A-D5138E5E1158}"/>
+    <hyperlink ref="D16" r:id="rId25" xr:uid="{C770D7DE-6980-45A2-A8B6-8E4C376C05E3}"/>
+    <hyperlink ref="D65" r:id="rId26" xr:uid="{17A234E9-7249-4FCC-8BD4-B42E6DD51533}"/>
+    <hyperlink ref="D89" r:id="rId27" xr:uid="{B26FB768-9814-44C0-BE49-D50110CF8838}"/>
+    <hyperlink ref="D49" r:id="rId28" xr:uid="{2B927B9E-56D2-4AC7-A24B-BA7FAF44F900}"/>
+    <hyperlink ref="D32" r:id="rId29" xr:uid="{5F9DAD98-7221-4BEC-B311-BF6B1BD6F52E}"/>
+    <hyperlink ref="D77" r:id="rId30" xr:uid="{9388EE39-1B30-49DB-89AC-BEC39E8ACFBE}"/>
+    <hyperlink ref="D50" r:id="rId31" xr:uid="{7BC6DF64-9FBB-461B-BEE3-D705D5A5711D}"/>
+    <hyperlink ref="D21" r:id="rId32" xr:uid="{EE5546A8-9D18-43D6-949A-451AA8A97E76}"/>
+    <hyperlink ref="D67" r:id="rId33" xr:uid="{02A107CB-A6C9-40AA-AF84-5B08D008A43D}"/>
+    <hyperlink ref="D40" r:id="rId34" xr:uid="{03938AC4-898D-4B60-9A83-CF770912371F}"/>
+    <hyperlink ref="D84" r:id="rId35" xr:uid="{3EECDB74-289B-411A-BCC5-A028AA2ED5D5}"/>
+    <hyperlink ref="D58" r:id="rId36" xr:uid="{DEE2DB12-0D3D-4E58-8948-C29EDF524684}"/>
     <hyperlink ref="D7" r:id="rId37" xr:uid="{C501338A-FD0F-4F45-B8B1-BD737635609F}"/>
-    <hyperlink ref="D34" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
-    <hyperlink ref="D52" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
-    <hyperlink ref="D84" r:id="rId40" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
-    <hyperlink ref="D12" r:id="rId41" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
-    <hyperlink ref="D42" r:id="rId42" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
-    <hyperlink ref="D46" r:id="rId43" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
-    <hyperlink ref="D14" r:id="rId44" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
-    <hyperlink ref="D63" r:id="rId45" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
-    <hyperlink ref="D50" r:id="rId46" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
-    <hyperlink ref="D67" r:id="rId47" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
-    <hyperlink ref="D71" r:id="rId48" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
-    <hyperlink ref="D83" r:id="rId49" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
-    <hyperlink ref="D56" r:id="rId50" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
-    <hyperlink ref="D25" r:id="rId51" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
+    <hyperlink ref="D35" r:id="rId38" xr:uid="{973F790E-4686-49DC-8382-D85663F42FE4}"/>
+    <hyperlink ref="D53" r:id="rId39" xr:uid="{EB649DE9-649F-4972-9591-B77A8EC85DED}"/>
+    <hyperlink ref="D86" r:id="rId40" xr:uid="{381C8997-BEB8-4BF6-B715-C9CE36B18767}"/>
+    <hyperlink ref="D13" r:id="rId41" xr:uid="{E0321D7C-4A33-425C-AC81-F2844EF49280}"/>
+    <hyperlink ref="D43" r:id="rId42" xr:uid="{9362C2F6-92F8-4578-90F4-F93A12DB0620}"/>
+    <hyperlink ref="D47" r:id="rId43" xr:uid="{3D2507DB-58F1-46EB-972C-7262C11F3BC0}"/>
+    <hyperlink ref="D15" r:id="rId44" xr:uid="{FD7129AB-69C9-448B-90D0-0EB16503D948}"/>
+    <hyperlink ref="D64" r:id="rId45" xr:uid="{4F9A8AB7-9ABA-4133-A103-EC20BB3D5255}"/>
+    <hyperlink ref="D51" r:id="rId46" xr:uid="{FA35DE19-FE12-4948-8782-601512787A1F}"/>
+    <hyperlink ref="D69" r:id="rId47" xr:uid="{150BA8A8-C8E4-466E-B635-B3C8D844E311}"/>
+    <hyperlink ref="D73" r:id="rId48" xr:uid="{9D9D1EDB-1408-4DC1-94C7-2F6827AB67F5}"/>
+    <hyperlink ref="D85" r:id="rId49" xr:uid="{EB91F0BD-5E69-461C-9E7C-D329942BCBBE}"/>
+    <hyperlink ref="D57" r:id="rId50" xr:uid="{1D2CC020-5555-4E5F-87C1-5B10ECF5CEE5}"/>
+    <hyperlink ref="D26" r:id="rId51" xr:uid="{20CCBF4F-DA07-40B1-84D7-9C64B10A18DD}"/>
     <hyperlink ref="D4" r:id="rId52" xr:uid="{04F40983-3CCF-4A98-9D71-83239E621071}"/>
-    <hyperlink ref="D30" r:id="rId53" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
-    <hyperlink ref="D73" r:id="rId54" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
-    <hyperlink ref="D90" r:id="rId55" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
-    <hyperlink ref="D72" r:id="rId56" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
-    <hyperlink ref="D76" r:id="rId57" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
-    <hyperlink ref="D8" r:id="rId58" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
-    <hyperlink ref="D22" r:id="rId59" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
-    <hyperlink ref="D40" r:id="rId60" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
-    <hyperlink ref="D60" r:id="rId61" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
-    <hyperlink ref="D61" r:id="rId62" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
-    <hyperlink ref="D79" r:id="rId63" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
-    <hyperlink ref="D26" r:id="rId64" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
-    <hyperlink ref="D29" r:id="rId65" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
-    <hyperlink ref="D44" r:id="rId66" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
-    <hyperlink ref="D32" r:id="rId67" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
-    <hyperlink ref="D18" r:id="rId68" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
-    <hyperlink ref="D36" r:id="rId69" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
+    <hyperlink ref="D31" r:id="rId53" xr:uid="{B6182D1F-82B7-4DC3-BB62-5D4CE3E6347D}"/>
+    <hyperlink ref="D75" r:id="rId54" xr:uid="{7F7DBD18-50DD-4284-8836-015BE6E2AF57}"/>
+    <hyperlink ref="D92" r:id="rId55" xr:uid="{2160B5D2-BA90-4A96-B73C-39ADAF82E7EC}"/>
+    <hyperlink ref="D74" r:id="rId56" xr:uid="{35C5AF31-961F-47D5-AF98-5D77E6CC3905}"/>
+    <hyperlink ref="D78" r:id="rId57" xr:uid="{3776AFCD-5853-4CE7-A817-305F74165C06}"/>
+    <hyperlink ref="D9" r:id="rId58" xr:uid="{F7E14BE7-9BEF-429A-BC06-CA914EDCD03E}"/>
+    <hyperlink ref="D23" r:id="rId59" xr:uid="{13F0A7EA-4265-4C1A-936D-0F1F22648B66}"/>
+    <hyperlink ref="D41" r:id="rId60" display="mailto:david@zwang.com" xr:uid="{2E031ABA-CF1B-48A8-96E6-B6DCE94345AE}"/>
+    <hyperlink ref="D61" r:id="rId61" xr:uid="{1245116C-C3B7-4F34-8A1E-A3AF6A558128}"/>
+    <hyperlink ref="D62" r:id="rId62" xr:uid="{DF5F6B9A-45BB-416F-8E3D-91269D73D457}"/>
+    <hyperlink ref="D81" r:id="rId63" xr:uid="{E4C2E6D9-1E4B-4B0D-8600-86E3ECB7D1D8}"/>
+    <hyperlink ref="D27" r:id="rId64" xr:uid="{3AD048BB-9D70-41FA-8645-47CF1BE084C9}"/>
+    <hyperlink ref="D30" r:id="rId65" display="mailto:bertvk@enfocus.com" xr:uid="{6F56AFA2-CA54-4A51-B51B-36740F243F7A}"/>
+    <hyperlink ref="D45" r:id="rId66" xr:uid="{DEECD580-BF33-4FBB-A267-48E6674FF044}"/>
+    <hyperlink ref="D33" r:id="rId67" xr:uid="{3A6EE0DA-E93B-4D24-AD52-FF9D72BBC152}"/>
+    <hyperlink ref="D19" r:id="rId68" xr:uid="{897A4DB8-756C-42E5-AF7B-011BBBE00628}"/>
+    <hyperlink ref="D37" r:id="rId69" xr:uid="{47A4E692-159B-4E48-A1D4-411E278B3A43}"/>
     <hyperlink ref="D2" r:id="rId70" display="mailto:frank.vyncke@yin4yang.com" xr:uid="{E29600CB-349C-4C55-AC29-3B61912C4757}"/>
-    <hyperlink ref="D89" r:id="rId71" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
-    <hyperlink ref="D23" r:id="rId72" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
+    <hyperlink ref="D91" r:id="rId71" xr:uid="{C4C4EA22-387A-4AD7-A4B4-D79D02B39793}"/>
+    <hyperlink ref="D24" r:id="rId72" xr:uid="{BF5FD244-0DE0-493E-A7E1-0CEDCE9B77AA}"/>
     <hyperlink ref="D5" r:id="rId73" xr:uid="{33D12C26-CC5E-4925-86B6-4AE855A6371F}"/>
     <hyperlink ref="G5" r:id="rId74" xr:uid="{2FA39695-7884-42EC-9380-C8EFD7B7EAD9}"/>
-    <hyperlink ref="D13" r:id="rId75" xr:uid="{B237CB2B-4475-8C4E-A2C5-5839FB07318E}"/>
+    <hyperlink ref="D14" r:id="rId75" xr:uid="{B237CB2B-4475-8C4E-A2C5-5839FB07318E}"/>
     <hyperlink ref="D6" r:id="rId76" xr:uid="{3C6DADFB-91D3-4B16-BA60-22286260FB72}"/>
     <hyperlink ref="G6" r:id="rId77" xr:uid="{EF6627CA-3B1A-440B-85D4-A1B7067549BD}"/>
-    <hyperlink ref="D10" r:id="rId78" xr:uid="{058D1BE7-4CFF-4740-BC92-2074C717A677}"/>
-    <hyperlink ref="G10" r:id="rId79" xr:uid="{B9062A46-48F6-45FB-8197-4FD986CC482D}"/>
-    <hyperlink ref="D53" r:id="rId80" xr:uid="{0CFEC845-7F90-4802-9D24-4AC8905CD11B}"/>
-    <hyperlink ref="D58" r:id="rId81" xr:uid="{81B44739-2F1A-4DDB-90E8-2523712052F0}"/>
-    <hyperlink ref="D43" r:id="rId82" xr:uid="{72B2BA10-0B55-4ACF-9CC1-DA30FB4C2741}"/>
-    <hyperlink ref="G43" r:id="rId83" xr:uid="{1106BFBB-F6F3-4E8A-8B65-06381130271C}"/>
-    <hyperlink ref="D81" r:id="rId84" xr:uid="{249742DB-9523-4D5C-B3FC-194F7D7BB889}"/>
-    <hyperlink ref="G81" r:id="rId85" xr:uid="{BD0ABADB-115E-43D9-8791-2BFF7CAEC355}"/>
-    <hyperlink ref="G51" r:id="rId86" xr:uid="{44657DD4-3FFA-4E6F-8898-631518A1BFDC}"/>
-    <hyperlink ref="D51" r:id="rId87" xr:uid="{D5A339A1-161D-40E3-9F69-B4599246184B}"/>
-    <hyperlink ref="G19" r:id="rId88" xr:uid="{C64F139E-8286-4E7A-8B5E-9D69FC9A0C25}"/>
-    <hyperlink ref="G55" r:id="rId89" xr:uid="{5D505EE9-2263-469C-9455-D353F4C9921E}"/>
-    <hyperlink ref="D55" r:id="rId90" xr:uid="{5715AC7F-4208-4141-884D-FD2EB9CB5E95}"/>
-    <hyperlink ref="D17" r:id="rId91" xr:uid="{50E71DF8-A245-41B4-83A8-E6488454D9A4}"/>
-    <hyperlink ref="G27" r:id="rId92" xr:uid="{15520162-C027-42E1-8EC1-CA7EA9FD18BC}"/>
-    <hyperlink ref="D27" r:id="rId93" xr:uid="{E9A12839-D069-4292-A5EA-36394565B8A0}"/>
-    <hyperlink ref="D41" r:id="rId94" xr:uid="{F07464A9-7B4E-4E5B-9EEE-3F687E9DC9AC}"/>
-    <hyperlink ref="G41" r:id="rId95" xr:uid="{73C68A69-730D-4676-B564-01BC2FDA7E73}"/>
-    <hyperlink ref="D62" r:id="rId96" xr:uid="{DC40AB03-35C7-4C6E-B261-5A4793D79E6C}"/>
-    <hyperlink ref="D88" r:id="rId97" xr:uid="{474ED1A8-8C48-45EA-B1FF-F6F7564A2191}"/>
-    <hyperlink ref="D21" r:id="rId98" xr:uid="{3C768ED5-B6E7-416A-B3CF-31E9B14F1258}"/>
-    <hyperlink ref="G21" r:id="rId99" xr:uid="{5C4AC9BE-92AA-40F8-AA34-D54E19486DEE}"/>
+    <hyperlink ref="D11" r:id="rId78" xr:uid="{058D1BE7-4CFF-4740-BC92-2074C717A677}"/>
+    <hyperlink ref="G11" r:id="rId79" xr:uid="{B9062A46-48F6-45FB-8197-4FD986CC482D}"/>
+    <hyperlink ref="D54" r:id="rId80" xr:uid="{0CFEC845-7F90-4802-9D24-4AC8905CD11B}"/>
+    <hyperlink ref="D59" r:id="rId81" xr:uid="{81B44739-2F1A-4DDB-90E8-2523712052F0}"/>
+    <hyperlink ref="D44" r:id="rId82" xr:uid="{72B2BA10-0B55-4ACF-9CC1-DA30FB4C2741}"/>
+    <hyperlink ref="G44" r:id="rId83" xr:uid="{1106BFBB-F6F3-4E8A-8B65-06381130271C}"/>
+    <hyperlink ref="D83" r:id="rId84" xr:uid="{249742DB-9523-4D5C-B3FC-194F7D7BB889}"/>
+    <hyperlink ref="G83" r:id="rId85" xr:uid="{BD0ABADB-115E-43D9-8791-2BFF7CAEC355}"/>
+    <hyperlink ref="G52" r:id="rId86" xr:uid="{44657DD4-3FFA-4E6F-8898-631518A1BFDC}"/>
+    <hyperlink ref="D52" r:id="rId87" xr:uid="{D5A339A1-161D-40E3-9F69-B4599246184B}"/>
+    <hyperlink ref="G20" r:id="rId88" xr:uid="{C64F139E-8286-4E7A-8B5E-9D69FC9A0C25}"/>
+    <hyperlink ref="G56" r:id="rId89" xr:uid="{5D505EE9-2263-469C-9455-D353F4C9921E}"/>
+    <hyperlink ref="D56" r:id="rId90" xr:uid="{5715AC7F-4208-4141-884D-FD2EB9CB5E95}"/>
+    <hyperlink ref="D18" r:id="rId91" xr:uid="{50E71DF8-A245-41B4-83A8-E6488454D9A4}"/>
+    <hyperlink ref="G28" r:id="rId92" xr:uid="{15520162-C027-42E1-8EC1-CA7EA9FD18BC}"/>
+    <hyperlink ref="D28" r:id="rId93" xr:uid="{E9A12839-D069-4292-A5EA-36394565B8A0}"/>
+    <hyperlink ref="D42" r:id="rId94" xr:uid="{F07464A9-7B4E-4E5B-9EEE-3F687E9DC9AC}"/>
+    <hyperlink ref="G42" r:id="rId95" xr:uid="{73C68A69-730D-4676-B564-01BC2FDA7E73}"/>
+    <hyperlink ref="D63" r:id="rId96" xr:uid="{DC40AB03-35C7-4C6E-B261-5A4793D79E6C}"/>
+    <hyperlink ref="D90" r:id="rId97" xr:uid="{474ED1A8-8C48-45EA-B1FF-F6F7564A2191}"/>
+    <hyperlink ref="D22" r:id="rId98" xr:uid="{3C768ED5-B6E7-416A-B3CF-31E9B14F1258}"/>
+    <hyperlink ref="G22" r:id="rId99" xr:uid="{5C4AC9BE-92AA-40F8-AA34-D54E19486DEE}"/>
+    <hyperlink ref="D8" r:id="rId100" xr:uid="{0DDFD3D5-41E0-4A59-8992-A1EE6FD3C05D}"/>
+    <hyperlink ref="G8" r:id="rId101" xr:uid="{82F38FA1-9E55-4CDE-87F7-9C87D20D9E51}"/>
+    <hyperlink ref="D68" r:id="rId102" xr:uid="{F47445AD-9EE1-46DB-B7BA-B288E5B3A5E1}"/>
+    <hyperlink ref="G68" r:id="rId103" xr:uid="{E84E1C75-8DAE-4F16-81A7-9CFD148DB33C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId100"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId104"/>
 </worksheet>
 </file>
</xml_diff>